<commit_message>
feature: update supplier profile
</commit_message>
<xml_diff>
--- a/public/6. COA.xlsx
+++ b/public/6. COA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patience.uwase\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patience.uwase\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FCB1C3A-7494-496B-B0F4-E881DF1B3D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E1781F2-D358-4C20-A65D-F1F4AB24A345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4479" uniqueCount="4442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4487" uniqueCount="4450">
   <si>
     <t>ACCESS BANK -USD</t>
   </si>
@@ -13371,6 +13371,30 @@
   </si>
   <si>
     <t>AKWA PALACE LIMITED COMPANY</t>
+  </si>
+  <si>
+    <t>N0132</t>
+  </si>
+  <si>
+    <t>NEWREST ZAMBIA</t>
+  </si>
+  <si>
+    <t>P0061</t>
+  </si>
+  <si>
+    <t>PUMA ENERGY GHANA LTD</t>
+  </si>
+  <si>
+    <t>T0106</t>
+  </si>
+  <si>
+    <t>TRANSAFRICA COMMUNICATIONS</t>
+  </si>
+  <si>
+    <t>P0096</t>
+  </si>
+  <si>
+    <t>PUMA SOUTH AFRICA</t>
   </si>
 </sst>
 </file>
@@ -14064,10 +14088,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B1560"/>
+  <dimension ref="A1:B1564"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="B202" sqref="B202"/>
+    <sheetView tabSelected="1" topLeftCell="A1254" workbookViewId="0">
+      <selection activeCell="B1271" sqref="B1271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -23734,2825 +23758,2857 @@
     </row>
     <row r="1208" spans="1:2">
       <c r="A1208" s="1" t="s">
-        <v>3723</v>
+        <v>4442</v>
       </c>
       <c r="B1208" t="s">
-        <v>3724</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="1209" spans="1:2">
       <c r="A1209" s="1" t="s">
-        <v>3725</v>
+        <v>3723</v>
       </c>
       <c r="B1209" t="s">
-        <v>3725</v>
+        <v>3724</v>
       </c>
     </row>
     <row r="1210" spans="1:2">
       <c r="A1210" s="1" t="s">
-        <v>3726</v>
+        <v>3725</v>
       </c>
       <c r="B1210" t="s">
-        <v>3727</v>
+        <v>3725</v>
       </c>
     </row>
     <row r="1211" spans="1:2">
       <c r="A1211" s="1" t="s">
-        <v>3728</v>
+        <v>3726</v>
       </c>
       <c r="B1211" t="s">
-        <v>3729</v>
+        <v>3727</v>
       </c>
     </row>
     <row r="1212" spans="1:2">
       <c r="A1212" s="1" t="s">
-        <v>3730</v>
+        <v>3728</v>
       </c>
       <c r="B1212" t="s">
-        <v>3731</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="1213" spans="1:2">
       <c r="A1213" s="1" t="s">
-        <v>3732</v>
+        <v>3730</v>
       </c>
       <c r="B1213" t="s">
-        <v>3733</v>
+        <v>3731</v>
       </c>
     </row>
     <row r="1214" spans="1:2">
       <c r="A1214" s="1" t="s">
-        <v>3734</v>
+        <v>3732</v>
       </c>
       <c r="B1214" t="s">
-        <v>3735</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="1215" spans="1:2">
       <c r="A1215" s="1" t="s">
-        <v>3736</v>
+        <v>3734</v>
       </c>
       <c r="B1215" t="s">
-        <v>3737</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="1216" spans="1:2">
       <c r="A1216" s="1" t="s">
-        <v>3738</v>
+        <v>3736</v>
       </c>
       <c r="B1216" t="s">
-        <v>3739</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="1217" spans="1:2">
       <c r="A1217" s="1" t="s">
-        <v>3740</v>
+        <v>3738</v>
       </c>
       <c r="B1217" t="s">
-        <v>3741</v>
+        <v>3739</v>
       </c>
     </row>
     <row r="1218" spans="1:2">
       <c r="A1218" s="1" t="s">
-        <v>3742</v>
+        <v>3740</v>
       </c>
       <c r="B1218" t="s">
-        <v>3743</v>
+        <v>3741</v>
       </c>
     </row>
     <row r="1219" spans="1:2">
       <c r="A1219" s="1" t="s">
-        <v>3744</v>
+        <v>3742</v>
       </c>
       <c r="B1219" t="s">
-        <v>3745</v>
+        <v>3743</v>
       </c>
     </row>
     <row r="1220" spans="1:2">
       <c r="A1220" s="1" t="s">
-        <v>3746</v>
+        <v>3744</v>
       </c>
       <c r="B1220" t="s">
-        <v>3747</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="1221" spans="1:2">
       <c r="A1221" s="1" t="s">
-        <v>3748</v>
+        <v>3746</v>
       </c>
       <c r="B1221" t="s">
-        <v>3749</v>
+        <v>3747</v>
       </c>
     </row>
     <row r="1222" spans="1:2">
       <c r="A1222" s="1" t="s">
-        <v>3750</v>
+        <v>3748</v>
       </c>
       <c r="B1222" t="s">
-        <v>3751</v>
+        <v>3749</v>
       </c>
     </row>
     <row r="1223" spans="1:2">
       <c r="A1223" s="1" t="s">
-        <v>4425</v>
+        <v>3750</v>
       </c>
       <c r="B1223" t="s">
-        <v>4426</v>
+        <v>3751</v>
       </c>
     </row>
     <row r="1224" spans="1:2">
       <c r="A1224" s="1" t="s">
-        <v>3752</v>
+        <v>4425</v>
       </c>
       <c r="B1224" t="s">
-        <v>3753</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="1225" spans="1:2">
       <c r="A1225" s="1" t="s">
-        <v>3754</v>
+        <v>3752</v>
       </c>
       <c r="B1225" t="s">
-        <v>3749</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="1226" spans="1:2">
       <c r="A1226" s="1" t="s">
-        <v>3755</v>
+        <v>3754</v>
       </c>
       <c r="B1226" t="s">
-        <v>3756</v>
+        <v>3749</v>
       </c>
     </row>
     <row r="1227" spans="1:2">
       <c r="A1227" s="1" t="s">
-        <v>3757</v>
+        <v>3755</v>
       </c>
       <c r="B1227" t="s">
-        <v>3758</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="1228" spans="1:2">
       <c r="A1228" s="1" t="s">
-        <v>3759</v>
+        <v>3757</v>
       </c>
       <c r="B1228" t="s">
-        <v>3760</v>
+        <v>3758</v>
       </c>
     </row>
     <row r="1229" spans="1:2">
       <c r="A1229" s="1" t="s">
-        <v>3761</v>
+        <v>3759</v>
       </c>
       <c r="B1229" t="s">
-        <v>3762</v>
+        <v>3760</v>
       </c>
     </row>
     <row r="1230" spans="1:2">
       <c r="A1230" s="1" t="s">
-        <v>3763</v>
+        <v>3761</v>
       </c>
       <c r="B1230" t="s">
-        <v>3764</v>
+        <v>3762</v>
       </c>
     </row>
     <row r="1231" spans="1:2">
       <c r="A1231" s="1" t="s">
-        <v>3765</v>
+        <v>3763</v>
       </c>
       <c r="B1231" t="s">
-        <v>3766</v>
+        <v>3764</v>
       </c>
     </row>
     <row r="1232" spans="1:2">
       <c r="A1232" s="1" t="s">
-        <v>3767</v>
+        <v>3765</v>
       </c>
       <c r="B1232" t="s">
-        <v>3768</v>
+        <v>3766</v>
       </c>
     </row>
     <row r="1233" spans="1:2">
       <c r="A1233" s="1" t="s">
-        <v>3769</v>
+        <v>3767</v>
       </c>
       <c r="B1233" t="s">
-        <v>3770</v>
+        <v>3768</v>
       </c>
     </row>
     <row r="1234" spans="1:2">
       <c r="A1234" s="1" t="s">
-        <v>3771</v>
+        <v>3769</v>
       </c>
       <c r="B1234" t="s">
-        <v>3772</v>
+        <v>3770</v>
       </c>
     </row>
     <row r="1235" spans="1:2">
       <c r="A1235" s="1" t="s">
-        <v>3773</v>
+        <v>3771</v>
       </c>
       <c r="B1235" t="s">
-        <v>3774</v>
+        <v>3772</v>
       </c>
     </row>
     <row r="1236" spans="1:2">
       <c r="A1236" s="1" t="s">
-        <v>3775</v>
+        <v>3773</v>
       </c>
       <c r="B1236" t="s">
-        <v>3762</v>
+        <v>3774</v>
       </c>
     </row>
     <row r="1237" spans="1:2">
       <c r="A1237" s="1" t="s">
-        <v>3776</v>
+        <v>3775</v>
       </c>
       <c r="B1237" t="s">
-        <v>3777</v>
+        <v>3762</v>
       </c>
     </row>
     <row r="1238" spans="1:2">
       <c r="A1238" s="1" t="s">
-        <v>3778</v>
+        <v>3776</v>
       </c>
       <c r="B1238" t="s">
-        <v>3779</v>
+        <v>3777</v>
       </c>
     </row>
     <row r="1239" spans="1:2">
       <c r="A1239" s="1" t="s">
-        <v>3780</v>
+        <v>3778</v>
       </c>
       <c r="B1239" t="s">
-        <v>3781</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="1240" spans="1:2">
       <c r="A1240" s="1" t="s">
-        <v>3782</v>
+        <v>3780</v>
       </c>
       <c r="B1240" t="s">
-        <v>3783</v>
+        <v>3781</v>
       </c>
     </row>
     <row r="1241" spans="1:2">
       <c r="A1241" s="1" t="s">
-        <v>3784</v>
+        <v>3782</v>
       </c>
       <c r="B1241" t="s">
-        <v>3785</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="1242" spans="1:2">
       <c r="A1242" s="1" t="s">
-        <v>3786</v>
+        <v>4444</v>
       </c>
       <c r="B1242" t="s">
-        <v>3787</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="1243" spans="1:2">
       <c r="A1243" s="1" t="s">
-        <v>3788</v>
+        <v>3784</v>
       </c>
       <c r="B1243" t="s">
-        <v>3789</v>
+        <v>3785</v>
       </c>
     </row>
     <row r="1244" spans="1:2">
       <c r="A1244" s="1" t="s">
-        <v>3790</v>
+        <v>3786</v>
       </c>
       <c r="B1244" t="s">
-        <v>3791</v>
+        <v>3787</v>
       </c>
     </row>
     <row r="1245" spans="1:2">
       <c r="A1245" s="1" t="s">
-        <v>3792</v>
+        <v>3788</v>
       </c>
       <c r="B1245" t="s">
-        <v>3793</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="1246" spans="1:2">
       <c r="A1246" s="1" t="s">
-        <v>3794</v>
+        <v>3790</v>
       </c>
       <c r="B1246" t="s">
-        <v>3795</v>
+        <v>3791</v>
       </c>
     </row>
     <row r="1247" spans="1:2">
       <c r="A1247" s="1" t="s">
-        <v>3796</v>
+        <v>3792</v>
       </c>
       <c r="B1247" t="s">
-        <v>3797</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="1248" spans="1:2">
       <c r="A1248" s="1" t="s">
-        <v>3798</v>
+        <v>3794</v>
       </c>
       <c r="B1248" t="s">
-        <v>3799</v>
+        <v>3795</v>
       </c>
     </row>
     <row r="1249" spans="1:2">
       <c r="A1249" s="1" t="s">
-        <v>3800</v>
+        <v>3796</v>
       </c>
       <c r="B1249" t="s">
-        <v>3801</v>
+        <v>3797</v>
       </c>
     </row>
     <row r="1250" spans="1:2">
       <c r="A1250" s="1" t="s">
-        <v>3802</v>
+        <v>3798</v>
       </c>
       <c r="B1250" t="s">
-        <v>3803</v>
+        <v>3799</v>
       </c>
     </row>
     <row r="1251" spans="1:2">
       <c r="A1251" s="1" t="s">
-        <v>3804</v>
+        <v>3800</v>
       </c>
       <c r="B1251" t="s">
-        <v>3805</v>
+        <v>3801</v>
       </c>
     </row>
     <row r="1252" spans="1:2">
       <c r="A1252" s="1" t="s">
-        <v>3806</v>
+        <v>3802</v>
       </c>
       <c r="B1252" t="s">
-        <v>3807</v>
+        <v>3803</v>
       </c>
     </row>
     <row r="1253" spans="1:2">
       <c r="A1253" s="1" t="s">
-        <v>3808</v>
+        <v>3804</v>
       </c>
       <c r="B1253" t="s">
-        <v>3809</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="1254" spans="1:2">
       <c r="A1254" s="1" t="s">
-        <v>3810</v>
+        <v>3806</v>
       </c>
       <c r="B1254" t="s">
-        <v>3811</v>
+        <v>3807</v>
       </c>
     </row>
     <row r="1255" spans="1:2">
       <c r="A1255" s="1" t="s">
-        <v>3812</v>
+        <v>3808</v>
       </c>
       <c r="B1255" t="s">
-        <v>3813</v>
+        <v>3809</v>
       </c>
     </row>
     <row r="1256" spans="1:2">
       <c r="A1256" s="1" t="s">
-        <v>3814</v>
+        <v>3810</v>
       </c>
       <c r="B1256" t="s">
-        <v>3815</v>
+        <v>3811</v>
       </c>
     </row>
     <row r="1257" spans="1:2">
       <c r="A1257" s="1" t="s">
-        <v>3816</v>
+        <v>3812</v>
       </c>
       <c r="B1257" t="s">
-        <v>3817</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="1258" spans="1:2">
       <c r="A1258" s="1" t="s">
-        <v>3818</v>
+        <v>3814</v>
       </c>
       <c r="B1258" t="s">
-        <v>3819</v>
+        <v>3815</v>
       </c>
     </row>
     <row r="1259" spans="1:2">
       <c r="A1259" s="1" t="s">
-        <v>3820</v>
+        <v>3816</v>
       </c>
       <c r="B1259" t="s">
-        <v>3821</v>
+        <v>3817</v>
       </c>
     </row>
     <row r="1260" spans="1:2">
       <c r="A1260" s="1" t="s">
-        <v>3822</v>
+        <v>3818</v>
       </c>
       <c r="B1260" t="s">
-        <v>3823</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="1261" spans="1:2">
       <c r="A1261" s="1" t="s">
-        <v>3824</v>
+        <v>3820</v>
       </c>
       <c r="B1261" t="s">
-        <v>3825</v>
+        <v>3821</v>
       </c>
     </row>
     <row r="1262" spans="1:2">
       <c r="A1262" s="1" t="s">
-        <v>3826</v>
+        <v>3822</v>
       </c>
       <c r="B1262" t="s">
-        <v>3827</v>
+        <v>3823</v>
       </c>
     </row>
     <row r="1263" spans="1:2">
       <c r="A1263" s="1" t="s">
-        <v>3828</v>
+        <v>3824</v>
       </c>
       <c r="B1263" t="s">
-        <v>3829</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="1264" spans="1:2">
       <c r="A1264" s="1" t="s">
-        <v>3830</v>
+        <v>3826</v>
       </c>
       <c r="B1264" t="s">
-        <v>3831</v>
+        <v>3827</v>
       </c>
     </row>
     <row r="1265" spans="1:2">
       <c r="A1265" s="1" t="s">
-        <v>3832</v>
+        <v>3828</v>
       </c>
       <c r="B1265" t="s">
-        <v>3833</v>
+        <v>3829</v>
       </c>
     </row>
     <row r="1266" spans="1:2">
       <c r="A1266" s="1" t="s">
-        <v>3834</v>
+        <v>3830</v>
       </c>
       <c r="B1266" t="s">
-        <v>3835</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="1267" spans="1:2">
       <c r="A1267" s="1" t="s">
-        <v>3836</v>
+        <v>3832</v>
       </c>
       <c r="B1267" t="s">
-        <v>3837</v>
+        <v>3833</v>
       </c>
     </row>
     <row r="1268" spans="1:2">
       <c r="A1268" s="1" t="s">
-        <v>3838</v>
+        <v>4448</v>
       </c>
       <c r="B1268" t="s">
-        <v>3839</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="1269" spans="1:2">
       <c r="A1269" s="1" t="s">
-        <v>3840</v>
+        <v>3834</v>
       </c>
       <c r="B1269" t="s">
-        <v>3841</v>
+        <v>3835</v>
       </c>
     </row>
     <row r="1270" spans="1:2">
       <c r="A1270" s="1" t="s">
-        <v>3842</v>
+        <v>3836</v>
       </c>
       <c r="B1270" t="s">
-        <v>3843</v>
+        <v>3837</v>
       </c>
     </row>
     <row r="1271" spans="1:2">
       <c r="A1271" s="1" t="s">
-        <v>3844</v>
+        <v>3838</v>
       </c>
       <c r="B1271" t="s">
-        <v>3845</v>
+        <v>3839</v>
       </c>
     </row>
     <row r="1272" spans="1:2">
       <c r="A1272" s="1" t="s">
-        <v>3846</v>
+        <v>3840</v>
       </c>
       <c r="B1272" t="s">
-        <v>3559</v>
+        <v>3841</v>
       </c>
     </row>
     <row r="1273" spans="1:2">
       <c r="A1273" s="1" t="s">
-        <v>3847</v>
+        <v>3842</v>
       </c>
       <c r="B1273" t="s">
-        <v>3848</v>
+        <v>3843</v>
       </c>
     </row>
     <row r="1274" spans="1:2">
       <c r="A1274" s="1" t="s">
-        <v>3849</v>
+        <v>3844</v>
       </c>
       <c r="B1274" t="s">
-        <v>3850</v>
+        <v>3845</v>
       </c>
     </row>
     <row r="1275" spans="1:2">
       <c r="A1275" s="1" t="s">
-        <v>3851</v>
+        <v>3846</v>
       </c>
       <c r="B1275" t="s">
-        <v>2996</v>
+        <v>3559</v>
       </c>
     </row>
     <row r="1276" spans="1:2">
       <c r="A1276" s="1" t="s">
-        <v>3852</v>
+        <v>3847</v>
       </c>
       <c r="B1276" t="s">
-        <v>3853</v>
+        <v>3848</v>
       </c>
     </row>
     <row r="1277" spans="1:2">
       <c r="A1277" s="1" t="s">
-        <v>3854</v>
+        <v>3849</v>
       </c>
       <c r="B1277" t="s">
-        <v>3855</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1278" spans="1:2">
       <c r="A1278" s="1" t="s">
-        <v>3856</v>
+        <v>3851</v>
       </c>
       <c r="B1278" t="s">
-        <v>3857</v>
+        <v>2996</v>
       </c>
     </row>
     <row r="1279" spans="1:2">
       <c r="A1279" s="1" t="s">
-        <v>3858</v>
+        <v>3852</v>
       </c>
       <c r="B1279" t="s">
-        <v>3859</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1280" spans="1:2">
       <c r="A1280" s="1" t="s">
-        <v>3860</v>
+        <v>3854</v>
       </c>
       <c r="B1280" t="s">
-        <v>3861</v>
+        <v>3855</v>
       </c>
     </row>
     <row r="1281" spans="1:2">
       <c r="A1281" s="1" t="s">
-        <v>4437</v>
+        <v>3856</v>
       </c>
       <c r="B1281" t="s">
-        <v>4436</v>
+        <v>3857</v>
       </c>
     </row>
     <row r="1282" spans="1:2">
       <c r="A1282" s="1" t="s">
-        <v>3862</v>
+        <v>3858</v>
       </c>
       <c r="B1282" t="s">
-        <v>3863</v>
+        <v>3859</v>
       </c>
     </row>
     <row r="1283" spans="1:2">
       <c r="A1283" s="1" t="s">
-        <v>3864</v>
+        <v>3860</v>
       </c>
       <c r="B1283" t="s">
-        <v>3865</v>
+        <v>3861</v>
       </c>
     </row>
     <row r="1284" spans="1:2">
       <c r="A1284" s="1" t="s">
-        <v>3866</v>
+        <v>4437</v>
       </c>
       <c r="B1284" t="s">
-        <v>3867</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="1285" spans="1:2">
       <c r="A1285" s="1" t="s">
-        <v>3868</v>
+        <v>3862</v>
       </c>
       <c r="B1285" t="s">
-        <v>3869</v>
+        <v>3863</v>
       </c>
     </row>
     <row r="1286" spans="1:2">
       <c r="A1286" s="1" t="s">
-        <v>3870</v>
+        <v>3864</v>
       </c>
       <c r="B1286" t="s">
-        <v>3871</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1287" spans="1:2">
       <c r="A1287" s="1" t="s">
-        <v>3872</v>
+        <v>3866</v>
       </c>
       <c r="B1287" t="s">
-        <v>3873</v>
+        <v>3867</v>
       </c>
     </row>
     <row r="1288" spans="1:2">
       <c r="A1288" s="1" t="s">
-        <v>3874</v>
+        <v>3868</v>
       </c>
       <c r="B1288" t="s">
-        <v>3875</v>
+        <v>3869</v>
       </c>
     </row>
     <row r="1289" spans="1:2">
       <c r="A1289" s="1" t="s">
-        <v>3876</v>
+        <v>3870</v>
       </c>
       <c r="B1289" t="s">
-        <v>3877</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1290" spans="1:2">
       <c r="A1290" s="1" t="s">
-        <v>3878</v>
+        <v>3872</v>
       </c>
       <c r="B1290" t="s">
-        <v>3879</v>
+        <v>3873</v>
       </c>
     </row>
     <row r="1291" spans="1:2">
       <c r="A1291" s="1" t="s">
-        <v>3880</v>
+        <v>3874</v>
       </c>
       <c r="B1291" t="s">
-        <v>3881</v>
+        <v>3875</v>
       </c>
     </row>
     <row r="1292" spans="1:2">
       <c r="A1292" s="1" t="s">
-        <v>3882</v>
+        <v>3876</v>
       </c>
       <c r="B1292" t="s">
-        <v>3883</v>
+        <v>3877</v>
       </c>
     </row>
     <row r="1293" spans="1:2">
       <c r="A1293" s="1" t="s">
-        <v>3884</v>
+        <v>3878</v>
       </c>
       <c r="B1293" t="s">
-        <v>3885</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1294" spans="1:2">
       <c r="A1294" s="1" t="s">
-        <v>3886</v>
+        <v>3880</v>
       </c>
       <c r="B1294" t="s">
-        <v>3887</v>
+        <v>3881</v>
       </c>
     </row>
     <row r="1295" spans="1:2">
       <c r="A1295" s="1" t="s">
-        <v>3888</v>
+        <v>3882</v>
       </c>
       <c r="B1295" t="s">
-        <v>3889</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="1296" spans="1:2">
       <c r="A1296" s="1" t="s">
-        <v>3890</v>
+        <v>3884</v>
       </c>
       <c r="B1296" t="s">
-        <v>3891</v>
+        <v>3885</v>
       </c>
     </row>
     <row r="1297" spans="1:2">
       <c r="A1297" s="1" t="s">
-        <v>3892</v>
+        <v>3886</v>
       </c>
       <c r="B1297" t="s">
-        <v>3893</v>
+        <v>3887</v>
       </c>
     </row>
     <row r="1298" spans="1:2">
       <c r="A1298" s="1" t="s">
-        <v>3894</v>
+        <v>3888</v>
       </c>
       <c r="B1298" t="s">
-        <v>3895</v>
+        <v>3889</v>
       </c>
     </row>
     <row r="1299" spans="1:2">
       <c r="A1299" s="1" t="s">
-        <v>3896</v>
+        <v>3890</v>
       </c>
       <c r="B1299" t="s">
-        <v>3897</v>
+        <v>3891</v>
       </c>
     </row>
     <row r="1300" spans="1:2">
       <c r="A1300" s="1" t="s">
-        <v>3898</v>
+        <v>3892</v>
       </c>
       <c r="B1300" t="s">
-        <v>3899</v>
+        <v>3893</v>
       </c>
     </row>
     <row r="1301" spans="1:2">
       <c r="A1301" s="1" t="s">
-        <v>3900</v>
+        <v>3894</v>
       </c>
       <c r="B1301" t="s">
-        <v>3901</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="1302" spans="1:2">
       <c r="A1302" s="1" t="s">
-        <v>3902</v>
+        <v>3896</v>
       </c>
       <c r="B1302" t="s">
-        <v>3903</v>
+        <v>3897</v>
       </c>
     </row>
     <row r="1303" spans="1:2">
       <c r="A1303" s="1" t="s">
-        <v>3904</v>
+        <v>3898</v>
       </c>
       <c r="B1303" t="s">
-        <v>3905</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="1304" spans="1:2">
       <c r="A1304" s="1" t="s">
-        <v>3906</v>
+        <v>3900</v>
       </c>
       <c r="B1304" t="s">
-        <v>3907</v>
+        <v>3901</v>
       </c>
     </row>
     <row r="1305" spans="1:2">
       <c r="A1305" s="1" t="s">
-        <v>3908</v>
+        <v>3902</v>
       </c>
       <c r="B1305" t="s">
-        <v>3909</v>
+        <v>3903</v>
       </c>
     </row>
     <row r="1306" spans="1:2">
       <c r="A1306" s="1" t="s">
-        <v>3910</v>
+        <v>3904</v>
       </c>
       <c r="B1306" t="s">
-        <v>3911</v>
+        <v>3905</v>
       </c>
     </row>
     <row r="1307" spans="1:2">
       <c r="A1307" s="1" t="s">
-        <v>3912</v>
+        <v>3906</v>
       </c>
       <c r="B1307" t="s">
-        <v>3909</v>
+        <v>3907</v>
       </c>
     </row>
     <row r="1308" spans="1:2">
       <c r="A1308" s="1" t="s">
-        <v>3913</v>
+        <v>3908</v>
       </c>
       <c r="B1308" t="s">
-        <v>3914</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="1309" spans="1:2">
       <c r="A1309" s="1" t="s">
-        <v>3915</v>
+        <v>3910</v>
       </c>
       <c r="B1309" t="s">
-        <v>3916</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="1310" spans="1:2">
       <c r="A1310" s="1" t="s">
-        <v>3917</v>
+        <v>3912</v>
       </c>
       <c r="B1310" t="s">
-        <v>3918</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="1311" spans="1:2">
       <c r="A1311" s="1" t="s">
-        <v>3919</v>
+        <v>3913</v>
       </c>
       <c r="B1311" t="s">
-        <v>3920</v>
+        <v>3914</v>
       </c>
     </row>
     <row r="1312" spans="1:2">
       <c r="A1312" s="1" t="s">
-        <v>3921</v>
+        <v>3915</v>
       </c>
       <c r="B1312" t="s">
-        <v>3922</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="1313" spans="1:2">
       <c r="A1313" s="1" t="s">
-        <v>3923</v>
+        <v>3917</v>
       </c>
       <c r="B1313" t="s">
-        <v>3924</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="1314" spans="1:2">
       <c r="A1314" s="1" t="s">
-        <v>3925</v>
+        <v>3919</v>
       </c>
       <c r="B1314" t="s">
-        <v>3926</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="1315" spans="1:2">
       <c r="A1315" s="1" t="s">
-        <v>3927</v>
+        <v>3921</v>
       </c>
       <c r="B1315" t="s">
-        <v>3928</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="1316" spans="1:2">
       <c r="A1316" s="1" t="s">
-        <v>3929</v>
+        <v>3923</v>
       </c>
       <c r="B1316" t="s">
-        <v>3930</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="1317" spans="1:2">
       <c r="A1317" s="1" t="s">
-        <v>3931</v>
+        <v>3925</v>
       </c>
       <c r="B1317" t="s">
-        <v>3932</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="1318" spans="1:2">
       <c r="A1318" s="1" t="s">
-        <v>3933</v>
+        <v>3927</v>
       </c>
       <c r="B1318" t="s">
-        <v>3934</v>
+        <v>3928</v>
       </c>
     </row>
     <row r="1319" spans="1:2">
       <c r="A1319" s="1" t="s">
-        <v>3935</v>
+        <v>3929</v>
       </c>
       <c r="B1319" t="s">
-        <v>3936</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="1320" spans="1:2">
       <c r="A1320" s="1" t="s">
-        <v>3937</v>
+        <v>3931</v>
       </c>
       <c r="B1320" t="s">
-        <v>3938</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1321" spans="1:2">
       <c r="A1321" s="1" t="s">
-        <v>3939</v>
+        <v>3933</v>
       </c>
       <c r="B1321" t="s">
-        <v>3940</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="1322" spans="1:2">
       <c r="A1322" s="1" t="s">
-        <v>3941</v>
+        <v>3935</v>
       </c>
       <c r="B1322" t="s">
-        <v>3942</v>
+        <v>3936</v>
       </c>
     </row>
     <row r="1323" spans="1:2">
       <c r="A1323" s="1" t="s">
-        <v>3943</v>
+        <v>3937</v>
       </c>
       <c r="B1323" t="s">
-        <v>3944</v>
+        <v>3938</v>
       </c>
     </row>
     <row r="1324" spans="1:2">
       <c r="A1324" s="1" t="s">
-        <v>3945</v>
+        <v>3939</v>
       </c>
       <c r="B1324" t="s">
-        <v>3946</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="1325" spans="1:2">
       <c r="A1325" s="1" t="s">
-        <v>3947</v>
+        <v>3941</v>
       </c>
       <c r="B1325" t="s">
-        <v>3948</v>
+        <v>3942</v>
       </c>
     </row>
     <row r="1326" spans="1:2">
       <c r="A1326" s="1" t="s">
-        <v>3949</v>
+        <v>3943</v>
       </c>
       <c r="B1326" t="s">
-        <v>3950</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="1327" spans="1:2">
       <c r="A1327" s="1" t="s">
-        <v>3951</v>
+        <v>3945</v>
       </c>
       <c r="B1327" t="s">
-        <v>3952</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="1328" spans="1:2">
       <c r="A1328" s="1" t="s">
-        <v>3953</v>
+        <v>3947</v>
       </c>
       <c r="B1328" t="s">
-        <v>3954</v>
+        <v>3948</v>
       </c>
     </row>
     <row r="1329" spans="1:2">
       <c r="A1329" s="1" t="s">
-        <v>3955</v>
+        <v>3949</v>
       </c>
       <c r="B1329" t="s">
-        <v>3942</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="1330" spans="1:2">
       <c r="A1330" s="1" t="s">
-        <v>3956</v>
+        <v>3951</v>
       </c>
       <c r="B1330" t="s">
-        <v>3957</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="1331" spans="1:2">
       <c r="A1331" s="1" t="s">
-        <v>3958</v>
+        <v>3953</v>
       </c>
       <c r="B1331" t="s">
-        <v>3959</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1332" spans="1:2">
       <c r="A1332" s="1" t="s">
-        <v>3960</v>
+        <v>3955</v>
       </c>
       <c r="B1332" t="s">
-        <v>3961</v>
+        <v>3942</v>
       </c>
     </row>
     <row r="1333" spans="1:2">
       <c r="A1333" s="1" t="s">
-        <v>3962</v>
+        <v>3956</v>
       </c>
       <c r="B1333" t="s">
-        <v>3963</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="1334" spans="1:2">
       <c r="A1334" s="1" t="s">
-        <v>3964</v>
+        <v>3958</v>
       </c>
       <c r="B1334" t="s">
-        <v>3848</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1335" spans="1:2">
       <c r="A1335" s="1" t="s">
-        <v>3965</v>
+        <v>3960</v>
       </c>
       <c r="B1335" t="s">
-        <v>3966</v>
+        <v>3961</v>
       </c>
     </row>
     <row r="1336" spans="1:2">
       <c r="A1336" s="1" t="s">
-        <v>3967</v>
+        <v>3962</v>
       </c>
       <c r="B1336" t="s">
-        <v>3968</v>
+        <v>3963</v>
       </c>
     </row>
     <row r="1337" spans="1:2">
       <c r="A1337" s="1" t="s">
-        <v>3969</v>
+        <v>3964</v>
       </c>
       <c r="B1337" t="s">
-        <v>3970</v>
+        <v>3848</v>
       </c>
     </row>
     <row r="1338" spans="1:2">
       <c r="A1338" s="1" t="s">
-        <v>3971</v>
+        <v>3965</v>
       </c>
       <c r="B1338" t="s">
-        <v>3972</v>
+        <v>3966</v>
       </c>
     </row>
     <row r="1339" spans="1:2">
       <c r="A1339" s="1" t="s">
-        <v>3973</v>
+        <v>3967</v>
       </c>
       <c r="B1339" t="s">
-        <v>3974</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="1340" spans="1:2">
       <c r="A1340" s="1" t="s">
-        <v>3975</v>
+        <v>3969</v>
       </c>
       <c r="B1340" t="s">
-        <v>3976</v>
+        <v>3970</v>
       </c>
     </row>
     <row r="1341" spans="1:2">
       <c r="A1341" s="1" t="s">
-        <v>3977</v>
+        <v>3971</v>
       </c>
       <c r="B1341" t="s">
-        <v>3978</v>
+        <v>3972</v>
       </c>
     </row>
     <row r="1342" spans="1:2">
       <c r="A1342" s="1" t="s">
-        <v>3979</v>
+        <v>3973</v>
       </c>
       <c r="B1342" t="s">
-        <v>3980</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="1343" spans="1:2">
       <c r="A1343" s="1" t="s">
-        <v>3981</v>
+        <v>3975</v>
       </c>
       <c r="B1343" t="s">
-        <v>3982</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1344" spans="1:2">
       <c r="A1344" s="1" t="s">
-        <v>3983</v>
+        <v>3977</v>
       </c>
       <c r="B1344" t="s">
-        <v>3984</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="1345" spans="1:2">
       <c r="A1345" s="1" t="s">
-        <v>3985</v>
+        <v>3979</v>
       </c>
       <c r="B1345" t="s">
-        <v>3986</v>
+        <v>3980</v>
       </c>
     </row>
     <row r="1346" spans="1:2">
       <c r="A1346" s="1" t="s">
-        <v>3987</v>
+        <v>3981</v>
       </c>
       <c r="B1346" t="s">
-        <v>3988</v>
+        <v>3982</v>
       </c>
     </row>
     <row r="1347" spans="1:2">
       <c r="A1347" s="1" t="s">
-        <v>3989</v>
+        <v>3983</v>
       </c>
       <c r="B1347" t="s">
-        <v>3990</v>
+        <v>3984</v>
       </c>
     </row>
     <row r="1348" spans="1:2">
       <c r="A1348" s="1" t="s">
-        <v>3991</v>
+        <v>3985</v>
       </c>
       <c r="B1348" t="s">
-        <v>3992</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1349" spans="1:2">
       <c r="A1349" s="1" t="s">
-        <v>3993</v>
+        <v>3987</v>
       </c>
       <c r="B1349" t="s">
-        <v>3994</v>
+        <v>3988</v>
       </c>
     </row>
     <row r="1350" spans="1:2">
       <c r="A1350" s="1" t="s">
-        <v>3995</v>
+        <v>3989</v>
       </c>
       <c r="B1350" t="s">
-        <v>3996</v>
+        <v>3990</v>
       </c>
     </row>
     <row r="1351" spans="1:2">
       <c r="A1351" s="1" t="s">
-        <v>3997</v>
+        <v>3991</v>
       </c>
       <c r="B1351" t="s">
-        <v>3998</v>
+        <v>3992</v>
       </c>
     </row>
     <row r="1352" spans="1:2">
       <c r="A1352" s="1" t="s">
-        <v>3999</v>
+        <v>3993</v>
       </c>
       <c r="B1352" t="s">
-        <v>4000</v>
+        <v>3994</v>
       </c>
     </row>
     <row r="1353" spans="1:2">
       <c r="A1353" s="1" t="s">
-        <v>4001</v>
+        <v>3995</v>
       </c>
       <c r="B1353" t="s">
-        <v>4002</v>
+        <v>3996</v>
       </c>
     </row>
     <row r="1354" spans="1:2">
       <c r="A1354" s="1" t="s">
-        <v>4003</v>
+        <v>3997</v>
       </c>
       <c r="B1354" t="s">
-        <v>4004</v>
+        <v>3998</v>
       </c>
     </row>
     <row r="1355" spans="1:2">
       <c r="A1355" s="1" t="s">
-        <v>4005</v>
+        <v>3999</v>
       </c>
       <c r="B1355" t="s">
-        <v>4006</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1356" spans="1:2">
       <c r="A1356" s="1" t="s">
-        <v>4007</v>
+        <v>4001</v>
       </c>
       <c r="B1356" t="s">
-        <v>4008</v>
+        <v>4002</v>
       </c>
     </row>
     <row r="1357" spans="1:2">
       <c r="A1357" s="1" t="s">
-        <v>4009</v>
+        <v>4003</v>
       </c>
       <c r="B1357" t="s">
-        <v>4010</v>
+        <v>4004</v>
       </c>
     </row>
     <row r="1358" spans="1:2">
       <c r="A1358" s="1" t="s">
-        <v>4011</v>
+        <v>4005</v>
       </c>
       <c r="B1358" t="s">
-        <v>4012</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="1359" spans="1:2">
       <c r="A1359" s="1" t="s">
-        <v>4013</v>
+        <v>4007</v>
       </c>
       <c r="B1359" t="s">
-        <v>4014</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="1360" spans="1:2">
       <c r="A1360" s="1" t="s">
-        <v>4015</v>
+        <v>4009</v>
       </c>
       <c r="B1360" t="s">
-        <v>4016</v>
+        <v>4010</v>
       </c>
     </row>
     <row r="1361" spans="1:2">
       <c r="A1361" s="1" t="s">
-        <v>4017</v>
+        <v>4011</v>
       </c>
       <c r="B1361" t="s">
-        <v>4018</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="1362" spans="1:2">
       <c r="A1362" s="1" t="s">
-        <v>4019</v>
+        <v>4013</v>
       </c>
       <c r="B1362" t="s">
-        <v>4020</v>
+        <v>4014</v>
       </c>
     </row>
     <row r="1363" spans="1:2">
       <c r="A1363" s="1" t="s">
-        <v>4021</v>
+        <v>4015</v>
       </c>
       <c r="B1363" t="s">
-        <v>4022</v>
+        <v>4016</v>
       </c>
     </row>
     <row r="1364" spans="1:2">
       <c r="A1364" s="1" t="s">
-        <v>4023</v>
+        <v>4017</v>
       </c>
       <c r="B1364" t="s">
-        <v>4024</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="1365" spans="1:2">
       <c r="A1365" s="1" t="s">
-        <v>4025</v>
+        <v>4019</v>
       </c>
       <c r="B1365" t="s">
-        <v>4026</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1366" spans="1:2">
       <c r="A1366" s="1" t="s">
-        <v>4027</v>
+        <v>4021</v>
       </c>
       <c r="B1366" t="s">
-        <v>4028</v>
+        <v>4022</v>
       </c>
     </row>
     <row r="1367" spans="1:2">
       <c r="A1367" s="1" t="s">
-        <v>4029</v>
+        <v>4023</v>
       </c>
       <c r="B1367" t="s">
-        <v>4030</v>
+        <v>4024</v>
       </c>
     </row>
     <row r="1368" spans="1:2">
       <c r="A1368" s="1" t="s">
-        <v>4031</v>
+        <v>4025</v>
       </c>
       <c r="B1368" t="s">
-        <v>4032</v>
+        <v>4026</v>
       </c>
     </row>
     <row r="1369" spans="1:2">
       <c r="A1369" s="1" t="s">
-        <v>4033</v>
+        <v>4027</v>
       </c>
       <c r="B1369" t="s">
-        <v>4034</v>
+        <v>4028</v>
       </c>
     </row>
     <row r="1370" spans="1:2">
       <c r="A1370" s="1" t="s">
-        <v>4035</v>
+        <v>4029</v>
       </c>
       <c r="B1370" t="s">
-        <v>4036</v>
+        <v>4030</v>
       </c>
     </row>
     <row r="1371" spans="1:2">
       <c r="A1371" s="1" t="s">
-        <v>4037</v>
+        <v>4031</v>
       </c>
       <c r="B1371" t="s">
-        <v>4038</v>
+        <v>4032</v>
       </c>
     </row>
     <row r="1372" spans="1:2">
       <c r="A1372" s="1" t="s">
-        <v>4039</v>
+        <v>4033</v>
       </c>
       <c r="B1372" t="s">
-        <v>4040</v>
+        <v>4034</v>
       </c>
     </row>
     <row r="1373" spans="1:2">
       <c r="A1373" s="1" t="s">
-        <v>4041</v>
+        <v>4035</v>
       </c>
       <c r="B1373" t="s">
-        <v>4042</v>
+        <v>4036</v>
       </c>
     </row>
     <row r="1374" spans="1:2">
       <c r="A1374" s="1" t="s">
-        <v>4043</v>
+        <v>4037</v>
       </c>
       <c r="B1374" t="s">
-        <v>4044</v>
+        <v>4038</v>
       </c>
     </row>
     <row r="1375" spans="1:2">
       <c r="A1375" s="1" t="s">
-        <v>4045</v>
+        <v>4039</v>
       </c>
       <c r="B1375" t="s">
-        <v>4046</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1376" spans="1:2">
       <c r="A1376" s="1" t="s">
-        <v>4047</v>
+        <v>4041</v>
       </c>
       <c r="B1376" t="s">
-        <v>4048</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="1377" spans="1:2">
       <c r="A1377" s="1" t="s">
-        <v>4049</v>
+        <v>4043</v>
       </c>
       <c r="B1377" t="s">
-        <v>4050</v>
+        <v>4044</v>
       </c>
     </row>
     <row r="1378" spans="1:2">
       <c r="A1378" s="1" t="s">
-        <v>4051</v>
+        <v>4045</v>
       </c>
       <c r="B1378" t="s">
-        <v>4052</v>
+        <v>4046</v>
       </c>
     </row>
     <row r="1379" spans="1:2">
       <c r="A1379" s="1" t="s">
-        <v>4053</v>
+        <v>4047</v>
       </c>
       <c r="B1379" t="s">
-        <v>4054</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1380" spans="1:2">
       <c r="A1380" s="1" t="s">
-        <v>4055</v>
+        <v>4049</v>
       </c>
       <c r="B1380" t="s">
-        <v>4056</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="1381" spans="1:2">
       <c r="A1381" s="1" t="s">
-        <v>4057</v>
+        <v>4051</v>
       </c>
       <c r="B1381" t="s">
-        <v>4058</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="1382" spans="1:2">
       <c r="A1382" s="1" t="s">
-        <v>4059</v>
+        <v>4053</v>
       </c>
       <c r="B1382" t="s">
-        <v>4060</v>
+        <v>4054</v>
       </c>
     </row>
     <row r="1383" spans="1:2">
       <c r="A1383" s="1" t="s">
-        <v>4061</v>
+        <v>4055</v>
       </c>
       <c r="B1383" t="s">
-        <v>4062</v>
+        <v>4056</v>
       </c>
     </row>
     <row r="1384" spans="1:2">
       <c r="A1384" s="1" t="s">
-        <v>4063</v>
+        <v>4057</v>
       </c>
       <c r="B1384" t="s">
-        <v>4064</v>
+        <v>4058</v>
       </c>
     </row>
     <row r="1385" spans="1:2">
       <c r="A1385" s="1" t="s">
-        <v>4065</v>
+        <v>4059</v>
       </c>
       <c r="B1385" t="s">
-        <v>4066</v>
+        <v>4060</v>
       </c>
     </row>
     <row r="1386" spans="1:2">
       <c r="A1386" s="1" t="s">
-        <v>4067</v>
+        <v>4061</v>
       </c>
       <c r="B1386" t="s">
-        <v>4068</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="1387" spans="1:2">
       <c r="A1387" s="1" t="s">
-        <v>4069</v>
+        <v>4063</v>
       </c>
       <c r="B1387" t="s">
-        <v>4070</v>
+        <v>4064</v>
       </c>
     </row>
     <row r="1388" spans="1:2">
       <c r="A1388" s="1" t="s">
-        <v>4071</v>
+        <v>4065</v>
       </c>
       <c r="B1388" t="s">
-        <v>4072</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="1389" spans="1:2">
       <c r="A1389" s="1" t="s">
-        <v>4073</v>
+        <v>4067</v>
       </c>
       <c r="B1389" t="s">
-        <v>4074</v>
+        <v>4068</v>
       </c>
     </row>
     <row r="1390" spans="1:2">
       <c r="A1390" s="1" t="s">
-        <v>4075</v>
+        <v>4069</v>
       </c>
       <c r="B1390" t="s">
-        <v>4076</v>
+        <v>4070</v>
       </c>
     </row>
     <row r="1391" spans="1:2">
       <c r="A1391" s="1" t="s">
-        <v>4077</v>
+        <v>4071</v>
       </c>
       <c r="B1391" t="s">
-        <v>4078</v>
+        <v>4072</v>
       </c>
     </row>
     <row r="1392" spans="1:2">
       <c r="A1392" s="1" t="s">
-        <v>4079</v>
+        <v>4073</v>
       </c>
       <c r="B1392" t="s">
-        <v>4080</v>
+        <v>4074</v>
       </c>
     </row>
     <row r="1393" spans="1:2">
       <c r="A1393" s="1" t="s">
-        <v>4081</v>
+        <v>4075</v>
       </c>
       <c r="B1393" t="s">
-        <v>4082</v>
+        <v>4076</v>
       </c>
     </row>
     <row r="1394" spans="1:2">
       <c r="A1394" s="1" t="s">
-        <v>4083</v>
+        <v>4077</v>
       </c>
       <c r="B1394" t="s">
-        <v>4084</v>
+        <v>4078</v>
       </c>
     </row>
     <row r="1395" spans="1:2">
       <c r="A1395" s="1" t="s">
-        <v>4085</v>
+        <v>4079</v>
       </c>
       <c r="B1395" t="s">
-        <v>4086</v>
+        <v>4080</v>
       </c>
     </row>
     <row r="1396" spans="1:2">
       <c r="A1396" s="1" t="s">
-        <v>4087</v>
+        <v>4081</v>
       </c>
       <c r="B1396" t="s">
-        <v>4088</v>
+        <v>4082</v>
       </c>
     </row>
     <row r="1397" spans="1:2">
       <c r="A1397" s="1" t="s">
-        <v>4089</v>
+        <v>4083</v>
       </c>
       <c r="B1397" t="s">
-        <v>4090</v>
+        <v>4084</v>
       </c>
     </row>
     <row r="1398" spans="1:2">
       <c r="A1398" s="1" t="s">
-        <v>4091</v>
+        <v>4085</v>
       </c>
       <c r="B1398" t="s">
-        <v>4092</v>
+        <v>4086</v>
       </c>
     </row>
     <row r="1399" spans="1:2">
       <c r="A1399" s="1" t="s">
-        <v>4093</v>
+        <v>4087</v>
       </c>
       <c r="B1399" t="s">
-        <v>4094</v>
+        <v>4088</v>
       </c>
     </row>
     <row r="1400" spans="1:2">
       <c r="A1400" s="1" t="s">
-        <v>4095</v>
+        <v>4089</v>
       </c>
       <c r="B1400" t="s">
-        <v>4096</v>
+        <v>4090</v>
       </c>
     </row>
     <row r="1401" spans="1:2">
       <c r="A1401" s="1" t="s">
-        <v>4097</v>
+        <v>4091</v>
       </c>
       <c r="B1401" t="s">
-        <v>4098</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="1402" spans="1:2">
       <c r="A1402" s="1" t="s">
-        <v>4099</v>
+        <v>4093</v>
       </c>
       <c r="B1402" t="s">
-        <v>4100</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="1403" spans="1:2">
       <c r="A1403" s="1" t="s">
-        <v>4101</v>
+        <v>4095</v>
       </c>
       <c r="B1403" t="s">
-        <v>4102</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="1404" spans="1:2">
       <c r="A1404" s="1" t="s">
-        <v>4103</v>
+        <v>4097</v>
       </c>
       <c r="B1404" t="s">
-        <v>4104</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="1405" spans="1:2">
       <c r="A1405" s="1" t="s">
-        <v>4105</v>
+        <v>4099</v>
       </c>
       <c r="B1405" t="s">
-        <v>4106</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="1406" spans="1:2">
       <c r="A1406" s="1" t="s">
-        <v>4107</v>
+        <v>4101</v>
       </c>
       <c r="B1406" t="s">
-        <v>4108</v>
+        <v>4102</v>
       </c>
     </row>
     <row r="1407" spans="1:2">
       <c r="A1407" s="1" t="s">
-        <v>4109</v>
+        <v>4103</v>
       </c>
       <c r="B1407" t="s">
-        <v>4110</v>
+        <v>4104</v>
       </c>
     </row>
     <row r="1408" spans="1:2">
       <c r="A1408" s="1" t="s">
-        <v>4111</v>
+        <v>4105</v>
       </c>
       <c r="B1408" t="s">
-        <v>4112</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="1409" spans="1:2">
       <c r="A1409" s="1" t="s">
-        <v>4113</v>
+        <v>4107</v>
       </c>
       <c r="B1409" t="s">
-        <v>4114</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="1410" spans="1:2">
       <c r="A1410" s="1" t="s">
-        <v>4115</v>
+        <v>4109</v>
       </c>
       <c r="B1410" t="s">
-        <v>4116</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="1411" spans="1:2">
       <c r="A1411" s="1" t="s">
-        <v>4117</v>
+        <v>4111</v>
       </c>
       <c r="B1411" t="s">
-        <v>4118</v>
+        <v>4112</v>
       </c>
     </row>
     <row r="1412" spans="1:2">
       <c r="A1412" s="1" t="s">
-        <v>4119</v>
+        <v>4113</v>
       </c>
       <c r="B1412" t="s">
-        <v>4120</v>
+        <v>4114</v>
       </c>
     </row>
     <row r="1413" spans="1:2">
       <c r="A1413" s="1" t="s">
-        <v>4121</v>
+        <v>4115</v>
       </c>
       <c r="B1413" t="s">
-        <v>4122</v>
+        <v>4116</v>
       </c>
     </row>
     <row r="1414" spans="1:2">
       <c r="A1414" s="1" t="s">
-        <v>4123</v>
+        <v>4117</v>
       </c>
       <c r="B1414" t="s">
-        <v>4124</v>
+        <v>4118</v>
       </c>
     </row>
     <row r="1415" spans="1:2">
       <c r="A1415" s="1" t="s">
-        <v>4125</v>
+        <v>4119</v>
       </c>
       <c r="B1415" t="s">
-        <v>4126</v>
+        <v>4120</v>
       </c>
     </row>
     <row r="1416" spans="1:2">
       <c r="A1416" s="1" t="s">
-        <v>4127</v>
+        <v>4121</v>
       </c>
       <c r="B1416" t="s">
-        <v>4128</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="1417" spans="1:2">
       <c r="A1417" s="1" t="s">
-        <v>4129</v>
+        <v>4123</v>
       </c>
       <c r="B1417" t="s">
-        <v>4130</v>
+        <v>4124</v>
       </c>
     </row>
     <row r="1418" spans="1:2">
       <c r="A1418" s="1" t="s">
-        <v>4131</v>
+        <v>4125</v>
       </c>
       <c r="B1418" t="s">
-        <v>4132</v>
+        <v>4126</v>
       </c>
     </row>
     <row r="1419" spans="1:2">
       <c r="A1419" s="1" t="s">
-        <v>4133</v>
+        <v>4127</v>
       </c>
       <c r="B1419" t="s">
-        <v>4134</v>
+        <v>4128</v>
       </c>
     </row>
     <row r="1420" spans="1:2">
       <c r="A1420" s="1" t="s">
-        <v>4135</v>
+        <v>4129</v>
       </c>
       <c r="B1420" t="s">
-        <v>4136</v>
+        <v>4130</v>
       </c>
     </row>
     <row r="1421" spans="1:2">
       <c r="A1421" s="1" t="s">
-        <v>4137</v>
+        <v>4131</v>
       </c>
       <c r="B1421" t="s">
-        <v>4138</v>
+        <v>4132</v>
       </c>
     </row>
     <row r="1422" spans="1:2">
       <c r="A1422" s="1" t="s">
-        <v>4139</v>
+        <v>4133</v>
       </c>
       <c r="B1422" t="s">
-        <v>4140</v>
+        <v>4134</v>
       </c>
     </row>
     <row r="1423" spans="1:2">
       <c r="A1423" s="1" t="s">
-        <v>4141</v>
+        <v>4135</v>
       </c>
       <c r="B1423" t="s">
-        <v>4142</v>
+        <v>4136</v>
       </c>
     </row>
     <row r="1424" spans="1:2">
       <c r="A1424" s="1" t="s">
-        <v>4143</v>
+        <v>4137</v>
       </c>
       <c r="B1424" t="s">
-        <v>4144</v>
+        <v>4138</v>
       </c>
     </row>
     <row r="1425" spans="1:2">
       <c r="A1425" s="1" t="s">
-        <v>4423</v>
+        <v>4139</v>
       </c>
       <c r="B1425" t="s">
-        <v>4424</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="1426" spans="1:2">
       <c r="A1426" s="1" t="s">
-        <v>4145</v>
+        <v>4141</v>
       </c>
       <c r="B1426" t="s">
-        <v>4146</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="1427" spans="1:2">
       <c r="A1427" s="1" t="s">
-        <v>4147</v>
+        <v>4143</v>
       </c>
       <c r="B1427" t="s">
-        <v>4148</v>
+        <v>4144</v>
       </c>
     </row>
     <row r="1428" spans="1:2">
       <c r="A1428" s="1" t="s">
-        <v>4149</v>
+        <v>4423</v>
       </c>
       <c r="B1428" t="s">
-        <v>4150</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="1429" spans="1:2">
       <c r="A1429" s="1" t="s">
-        <v>4151</v>
+        <v>4145</v>
       </c>
       <c r="B1429" t="s">
-        <v>4152</v>
+        <v>4146</v>
       </c>
     </row>
     <row r="1430" spans="1:2">
       <c r="A1430" s="1" t="s">
-        <v>4153</v>
+        <v>4147</v>
       </c>
       <c r="B1430" t="s">
-        <v>4154</v>
+        <v>4148</v>
       </c>
     </row>
     <row r="1431" spans="1:2">
       <c r="A1431" s="1" t="s">
-        <v>4155</v>
+        <v>4149</v>
       </c>
       <c r="B1431" t="s">
-        <v>4156</v>
+        <v>4150</v>
       </c>
     </row>
     <row r="1432" spans="1:2">
       <c r="A1432" s="1" t="s">
-        <v>4157</v>
+        <v>4151</v>
       </c>
       <c r="B1432" t="s">
-        <v>4158</v>
+        <v>4152</v>
       </c>
     </row>
     <row r="1433" spans="1:2">
       <c r="A1433" s="1" t="s">
-        <v>4159</v>
+        <v>4153</v>
       </c>
       <c r="B1433" t="s">
-        <v>4160</v>
+        <v>4154</v>
       </c>
     </row>
     <row r="1434" spans="1:2">
       <c r="A1434" s="1" t="s">
-        <v>4161</v>
+        <v>4155</v>
       </c>
       <c r="B1434" t="s">
-        <v>4162</v>
+        <v>4156</v>
       </c>
     </row>
     <row r="1435" spans="1:2">
       <c r="A1435" s="1" t="s">
-        <v>4163</v>
+        <v>4157</v>
       </c>
       <c r="B1435" t="s">
-        <v>4164</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="1436" spans="1:2">
       <c r="A1436" s="1" t="s">
-        <v>4165</v>
+        <v>4159</v>
       </c>
       <c r="B1436" t="s">
-        <v>4166</v>
+        <v>4160</v>
       </c>
     </row>
     <row r="1437" spans="1:2">
       <c r="A1437" s="1" t="s">
-        <v>4167</v>
+        <v>4161</v>
       </c>
       <c r="B1437" t="s">
-        <v>4168</v>
+        <v>4162</v>
       </c>
     </row>
     <row r="1438" spans="1:2">
       <c r="A1438" s="1" t="s">
-        <v>4169</v>
+        <v>4163</v>
       </c>
       <c r="B1438" t="s">
-        <v>4170</v>
+        <v>4164</v>
       </c>
     </row>
     <row r="1439" spans="1:2">
       <c r="A1439" s="1" t="s">
-        <v>4171</v>
+        <v>4165</v>
       </c>
       <c r="B1439" t="s">
-        <v>4172</v>
+        <v>4166</v>
       </c>
     </row>
     <row r="1440" spans="1:2">
       <c r="A1440" s="1" t="s">
-        <v>4173</v>
+        <v>4167</v>
       </c>
       <c r="B1440" t="s">
-        <v>4174</v>
+        <v>4168</v>
       </c>
     </row>
     <row r="1441" spans="1:2">
       <c r="A1441" s="1" t="s">
-        <v>4175</v>
+        <v>4169</v>
       </c>
       <c r="B1441" t="s">
-        <v>4176</v>
+        <v>4170</v>
       </c>
     </row>
     <row r="1442" spans="1:2">
       <c r="A1442" s="1" t="s">
-        <v>4177</v>
+        <v>4171</v>
       </c>
       <c r="B1442" t="s">
-        <v>4178</v>
+        <v>4172</v>
       </c>
     </row>
     <row r="1443" spans="1:2">
       <c r="A1443" s="1" t="s">
-        <v>4179</v>
+        <v>4173</v>
       </c>
       <c r="B1443" t="s">
-        <v>4180</v>
+        <v>4174</v>
       </c>
     </row>
     <row r="1444" spans="1:2">
       <c r="A1444" s="1" t="s">
-        <v>4181</v>
+        <v>4175</v>
       </c>
       <c r="B1444" t="s">
-        <v>4182</v>
+        <v>4176</v>
       </c>
     </row>
     <row r="1445" spans="1:2">
       <c r="A1445" s="1" t="s">
-        <v>4183</v>
+        <v>4177</v>
       </c>
       <c r="B1445" t="s">
-        <v>4184</v>
+        <v>4178</v>
       </c>
     </row>
     <row r="1446" spans="1:2">
       <c r="A1446" s="1" t="s">
-        <v>4185</v>
+        <v>4179</v>
       </c>
       <c r="B1446" t="s">
-        <v>4186</v>
+        <v>4180</v>
       </c>
     </row>
     <row r="1447" spans="1:2">
       <c r="A1447" s="1" t="s">
-        <v>4187</v>
+        <v>4181</v>
       </c>
       <c r="B1447" t="s">
-        <v>4188</v>
+        <v>4182</v>
       </c>
     </row>
     <row r="1448" spans="1:2">
       <c r="A1448" s="1" t="s">
-        <v>4189</v>
+        <v>4183</v>
       </c>
       <c r="B1448" t="s">
-        <v>4190</v>
+        <v>4184</v>
       </c>
     </row>
     <row r="1449" spans="1:2">
       <c r="A1449" s="1" t="s">
-        <v>4191</v>
+        <v>4185</v>
       </c>
       <c r="B1449" t="s">
-        <v>4192</v>
+        <v>4186</v>
       </c>
     </row>
     <row r="1450" spans="1:2">
       <c r="A1450" s="1" t="s">
-        <v>4193</v>
+        <v>4187</v>
       </c>
       <c r="B1450" t="s">
-        <v>4194</v>
+        <v>4188</v>
       </c>
     </row>
     <row r="1451" spans="1:2">
       <c r="A1451" s="1" t="s">
-        <v>4195</v>
+        <v>4189</v>
       </c>
       <c r="B1451" t="s">
-        <v>4196</v>
+        <v>4190</v>
       </c>
     </row>
     <row r="1452" spans="1:2">
       <c r="A1452" s="1" t="s">
-        <v>4197</v>
+        <v>4191</v>
       </c>
       <c r="B1452" t="s">
-        <v>4198</v>
+        <v>4192</v>
       </c>
     </row>
     <row r="1453" spans="1:2">
       <c r="A1453" s="1" t="s">
-        <v>4199</v>
+        <v>4193</v>
       </c>
       <c r="B1453" t="s">
-        <v>4200</v>
+        <v>4194</v>
       </c>
     </row>
     <row r="1454" spans="1:2">
       <c r="A1454" s="1" t="s">
-        <v>4201</v>
+        <v>4195</v>
       </c>
       <c r="B1454" t="s">
-        <v>4202</v>
+        <v>4196</v>
       </c>
     </row>
     <row r="1455" spans="1:2">
       <c r="A1455" s="1" t="s">
-        <v>4203</v>
+        <v>4197</v>
       </c>
       <c r="B1455" t="s">
-        <v>4204</v>
+        <v>4198</v>
       </c>
     </row>
     <row r="1456" spans="1:2">
       <c r="A1456" s="1" t="s">
-        <v>4205</v>
+        <v>4199</v>
       </c>
       <c r="B1456" t="s">
-        <v>4206</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="1457" spans="1:2">
       <c r="A1457" s="1" t="s">
-        <v>4207</v>
+        <v>4201</v>
       </c>
       <c r="B1457" t="s">
-        <v>4208</v>
+        <v>4202</v>
       </c>
     </row>
     <row r="1458" spans="1:2">
       <c r="A1458" s="1" t="s">
-        <v>4209</v>
+        <v>4203</v>
       </c>
       <c r="B1458" t="s">
-        <v>4210</v>
+        <v>4204</v>
       </c>
     </row>
     <row r="1459" spans="1:2">
       <c r="A1459" s="1" t="s">
-        <v>4211</v>
+        <v>4205</v>
       </c>
       <c r="B1459" t="s">
-        <v>4212</v>
+        <v>4206</v>
       </c>
     </row>
     <row r="1460" spans="1:2">
       <c r="A1460" s="1" t="s">
-        <v>4213</v>
+        <v>4207</v>
       </c>
       <c r="B1460" t="s">
-        <v>4214</v>
+        <v>4208</v>
       </c>
     </row>
     <row r="1461" spans="1:2">
       <c r="A1461" s="1" t="s">
-        <v>4215</v>
+        <v>4209</v>
       </c>
       <c r="B1461" t="s">
-        <v>4216</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="1462" spans="1:2">
       <c r="A1462" s="1" t="s">
-        <v>4217</v>
+        <v>4211</v>
       </c>
       <c r="B1462" t="s">
-        <v>4218</v>
+        <v>4212</v>
       </c>
     </row>
     <row r="1463" spans="1:2">
       <c r="A1463" s="1" t="s">
-        <v>4219</v>
+        <v>4213</v>
       </c>
       <c r="B1463" t="s">
-        <v>4220</v>
+        <v>4214</v>
       </c>
     </row>
     <row r="1464" spans="1:2">
       <c r="A1464" s="1" t="s">
-        <v>4221</v>
+        <v>4215</v>
       </c>
       <c r="B1464" t="s">
-        <v>4222</v>
+        <v>4216</v>
       </c>
     </row>
     <row r="1465" spans="1:2">
       <c r="A1465" s="1" t="s">
-        <v>4223</v>
+        <v>4217</v>
       </c>
       <c r="B1465" t="s">
-        <v>4224</v>
+        <v>4218</v>
       </c>
     </row>
     <row r="1466" spans="1:2">
       <c r="A1466" s="1" t="s">
-        <v>4225</v>
+        <v>4219</v>
       </c>
       <c r="B1466" t="s">
-        <v>4226</v>
+        <v>4220</v>
       </c>
     </row>
     <row r="1467" spans="1:2">
       <c r="A1467" s="1" t="s">
-        <v>4227</v>
+        <v>4221</v>
       </c>
       <c r="B1467" t="s">
-        <v>4228</v>
+        <v>4222</v>
       </c>
     </row>
     <row r="1468" spans="1:2">
       <c r="A1468" s="1" t="s">
-        <v>4229</v>
+        <v>4223</v>
       </c>
       <c r="B1468" t="s">
-        <v>4230</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="1469" spans="1:2">
       <c r="A1469" s="1" t="s">
-        <v>4231</v>
+        <v>4225</v>
       </c>
       <c r="B1469" t="s">
-        <v>4232</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="1470" spans="1:2">
       <c r="A1470" s="1" t="s">
-        <v>4233</v>
+        <v>4227</v>
       </c>
       <c r="B1470" t="s">
-        <v>4234</v>
+        <v>4228</v>
       </c>
     </row>
     <row r="1471" spans="1:2">
       <c r="A1471" s="1" t="s">
-        <v>4235</v>
+        <v>4229</v>
       </c>
       <c r="B1471" t="s">
-        <v>4236</v>
+        <v>4230</v>
       </c>
     </row>
     <row r="1472" spans="1:2">
       <c r="A1472" s="1" t="s">
-        <v>4237</v>
+        <v>4231</v>
       </c>
       <c r="B1472" t="s">
-        <v>4238</v>
+        <v>4232</v>
       </c>
     </row>
     <row r="1473" spans="1:2">
       <c r="A1473" s="1" t="s">
-        <v>4239</v>
+        <v>4233</v>
       </c>
       <c r="B1473" t="s">
-        <v>4240</v>
+        <v>4234</v>
       </c>
     </row>
     <row r="1474" spans="1:2">
       <c r="A1474" s="1" t="s">
-        <v>4241</v>
+        <v>4235</v>
       </c>
       <c r="B1474" t="s">
-        <v>4242</v>
+        <v>4236</v>
       </c>
     </row>
     <row r="1475" spans="1:2">
       <c r="A1475" s="1" t="s">
-        <v>4243</v>
+        <v>4237</v>
       </c>
       <c r="B1475" t="s">
-        <v>4244</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="1476" spans="1:2">
       <c r="A1476" s="1" t="s">
-        <v>4245</v>
+        <v>4239</v>
       </c>
       <c r="B1476" t="s">
-        <v>4246</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="1477" spans="1:2">
       <c r="A1477" s="1" t="s">
-        <v>4247</v>
+        <v>4241</v>
       </c>
       <c r="B1477" t="s">
-        <v>4248</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="1478" spans="1:2">
       <c r="A1478" s="1" t="s">
-        <v>4249</v>
+        <v>4243</v>
       </c>
       <c r="B1478" t="s">
-        <v>4250</v>
+        <v>4244</v>
       </c>
     </row>
     <row r="1479" spans="1:2">
       <c r="A1479" s="1" t="s">
-        <v>4251</v>
+        <v>4245</v>
       </c>
       <c r="B1479" t="s">
-        <v>4252</v>
+        <v>4246</v>
       </c>
     </row>
     <row r="1480" spans="1:2">
       <c r="A1480" s="1" t="s">
-        <v>4253</v>
+        <v>4247</v>
       </c>
       <c r="B1480" t="s">
-        <v>4254</v>
+        <v>4248</v>
       </c>
     </row>
     <row r="1481" spans="1:2">
       <c r="A1481" s="1" t="s">
-        <v>4255</v>
+        <v>4249</v>
       </c>
       <c r="B1481" t="s">
-        <v>4256</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="1482" spans="1:2">
       <c r="A1482" s="1" t="s">
-        <v>4257</v>
+        <v>4251</v>
       </c>
       <c r="B1482" t="s">
-        <v>4258</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="1483" spans="1:2">
       <c r="A1483" s="1" t="s">
-        <v>4259</v>
+        <v>4253</v>
       </c>
       <c r="B1483" t="s">
-        <v>4260</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="1484" spans="1:2">
       <c r="A1484" s="1" t="s">
-        <v>4261</v>
+        <v>4255</v>
       </c>
       <c r="B1484" t="s">
-        <v>4262</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="1485" spans="1:2">
       <c r="A1485" s="1" t="s">
-        <v>4263</v>
+        <v>4257</v>
       </c>
       <c r="B1485" t="s">
-        <v>4264</v>
+        <v>4258</v>
       </c>
     </row>
     <row r="1486" spans="1:2">
       <c r="A1486" s="1" t="s">
-        <v>4265</v>
+        <v>4259</v>
       </c>
       <c r="B1486" t="s">
-        <v>4266</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="1487" spans="1:2">
       <c r="A1487" s="1" t="s">
-        <v>4267</v>
+        <v>4261</v>
       </c>
       <c r="B1487" t="s">
-        <v>4268</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="1488" spans="1:2">
       <c r="A1488" s="1" t="s">
-        <v>4269</v>
+        <v>4263</v>
       </c>
       <c r="B1488" t="s">
-        <v>4270</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="1489" spans="1:2">
       <c r="A1489" s="1" t="s">
-        <v>4271</v>
+        <v>4265</v>
       </c>
       <c r="B1489" t="s">
-        <v>4272</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="1490" spans="1:2">
       <c r="A1490" s="1" t="s">
-        <v>4273</v>
+        <v>4267</v>
       </c>
       <c r="B1490" t="s">
-        <v>4274</v>
+        <v>4268</v>
       </c>
     </row>
     <row r="1491" spans="1:2">
       <c r="A1491" s="1" t="s">
-        <v>4275</v>
+        <v>4269</v>
       </c>
       <c r="B1491" t="s">
-        <v>4276</v>
+        <v>4270</v>
       </c>
     </row>
     <row r="1492" spans="1:2">
       <c r="A1492" s="1" t="s">
-        <v>4277</v>
+        <v>4271</v>
       </c>
       <c r="B1492" t="s">
-        <v>4278</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="1493" spans="1:2">
       <c r="A1493" s="1" t="s">
-        <v>4279</v>
+        <v>4273</v>
       </c>
       <c r="B1493" t="s">
-        <v>4280</v>
+        <v>4274</v>
       </c>
     </row>
     <row r="1494" spans="1:2">
       <c r="A1494" s="1" t="s">
-        <v>4281</v>
+        <v>4275</v>
       </c>
       <c r="B1494" t="s">
-        <v>4282</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="1495" spans="1:2">
       <c r="A1495" s="1" t="s">
-        <v>4283</v>
+        <v>4277</v>
       </c>
       <c r="B1495" t="s">
-        <v>4284</v>
+        <v>4278</v>
       </c>
     </row>
     <row r="1496" spans="1:2">
       <c r="A1496" s="1" t="s">
-        <v>4285</v>
+        <v>4279</v>
       </c>
       <c r="B1496" t="s">
-        <v>4286</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="1497" spans="1:2">
       <c r="A1497" s="1" t="s">
-        <v>4287</v>
+        <v>4281</v>
       </c>
       <c r="B1497" t="s">
-        <v>4288</v>
+        <v>4282</v>
       </c>
     </row>
     <row r="1498" spans="1:2">
       <c r="A1498" s="1" t="s">
-        <v>4289</v>
+        <v>4283</v>
       </c>
       <c r="B1498" t="s">
-        <v>4290</v>
+        <v>4284</v>
       </c>
     </row>
     <row r="1499" spans="1:2">
       <c r="A1499" s="1" t="s">
-        <v>4291</v>
+        <v>4285</v>
       </c>
       <c r="B1499" t="s">
-        <v>4292</v>
+        <v>4286</v>
       </c>
     </row>
     <row r="1500" spans="1:2">
       <c r="A1500" s="1" t="s">
-        <v>4293</v>
+        <v>4287</v>
       </c>
       <c r="B1500" t="s">
-        <v>4294</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="1501" spans="1:2">
       <c r="A1501" s="1" t="s">
-        <v>4295</v>
+        <v>4289</v>
       </c>
       <c r="B1501" t="s">
-        <v>4296</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="1502" spans="1:2">
       <c r="A1502" s="1" t="s">
-        <v>4297</v>
+        <v>4291</v>
       </c>
       <c r="B1502" t="s">
-        <v>4298</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="1503" spans="1:2">
       <c r="A1503" s="1" t="s">
-        <v>4299</v>
+        <v>4293</v>
       </c>
       <c r="B1503" t="s">
-        <v>4300</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="1504" spans="1:2">
       <c r="A1504" s="1" t="s">
-        <v>4431</v>
+        <v>4295</v>
       </c>
       <c r="B1504" t="s">
-        <v>4432</v>
+        <v>4296</v>
       </c>
     </row>
     <row r="1505" spans="1:2">
       <c r="A1505" s="1" t="s">
-        <v>4301</v>
+        <v>4297</v>
       </c>
       <c r="B1505" t="s">
-        <v>4302</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="1506" spans="1:2">
       <c r="A1506" s="1" t="s">
-        <v>4303</v>
+        <v>4299</v>
       </c>
       <c r="B1506" t="s">
-        <v>4304</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="1507" spans="1:2">
       <c r="A1507" s="1" t="s">
-        <v>4305</v>
+        <v>4446</v>
       </c>
       <c r="B1507" t="s">
-        <v>4306</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="1508" spans="1:2">
       <c r="A1508" s="1" t="s">
-        <v>4307</v>
+        <v>4431</v>
       </c>
       <c r="B1508" t="s">
-        <v>4308</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="1509" spans="1:2">
       <c r="A1509" s="1" t="s">
-        <v>4309</v>
+        <v>4301</v>
       </c>
       <c r="B1509" t="s">
-        <v>4310</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="1510" spans="1:2">
       <c r="A1510" s="1" t="s">
-        <v>4311</v>
+        <v>4303</v>
       </c>
       <c r="B1510" t="s">
-        <v>4312</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="1511" spans="1:2">
       <c r="A1511" s="1" t="s">
-        <v>4313</v>
+        <v>4305</v>
       </c>
       <c r="B1511" t="s">
-        <v>4314</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="1512" spans="1:2">
       <c r="A1512" s="1" t="s">
-        <v>4315</v>
+        <v>4307</v>
       </c>
       <c r="B1512" t="s">
-        <v>4316</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="1513" spans="1:2">
       <c r="A1513" s="1" t="s">
-        <v>4317</v>
+        <v>4309</v>
       </c>
       <c r="B1513" t="s">
-        <v>4318</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="1514" spans="1:2">
       <c r="A1514" s="1" t="s">
-        <v>4319</v>
+        <v>4311</v>
       </c>
       <c r="B1514" t="s">
-        <v>4320</v>
+        <v>4312</v>
       </c>
     </row>
     <row r="1515" spans="1:2">
       <c r="A1515" s="1" t="s">
-        <v>4321</v>
+        <v>4313</v>
       </c>
       <c r="B1515" t="s">
-        <v>4322</v>
+        <v>4314</v>
       </c>
     </row>
     <row r="1516" spans="1:2">
       <c r="A1516" s="1" t="s">
-        <v>4323</v>
+        <v>4315</v>
       </c>
       <c r="B1516" t="s">
-        <v>4324</v>
+        <v>4316</v>
       </c>
     </row>
     <row r="1517" spans="1:2">
       <c r="A1517" s="1" t="s">
-        <v>4325</v>
+        <v>4317</v>
       </c>
       <c r="B1517" t="s">
-        <v>4326</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="1518" spans="1:2">
       <c r="A1518" s="1" t="s">
-        <v>4327</v>
+        <v>4319</v>
       </c>
       <c r="B1518" t="s">
-        <v>4328</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="1519" spans="1:2">
       <c r="A1519" s="1" t="s">
-        <v>4329</v>
+        <v>4321</v>
       </c>
       <c r="B1519" t="s">
-        <v>4330</v>
+        <v>4322</v>
       </c>
     </row>
     <row r="1520" spans="1:2">
       <c r="A1520" s="1" t="s">
-        <v>4331</v>
+        <v>4323</v>
       </c>
       <c r="B1520" t="s">
-        <v>4332</v>
+        <v>4324</v>
       </c>
     </row>
     <row r="1521" spans="1:2">
       <c r="A1521" s="1" t="s">
-        <v>4333</v>
+        <v>4325</v>
       </c>
       <c r="B1521" t="s">
-        <v>4334</v>
+        <v>4326</v>
       </c>
     </row>
     <row r="1522" spans="1:2">
       <c r="A1522" s="1" t="s">
-        <v>4335</v>
+        <v>4327</v>
       </c>
       <c r="B1522" t="s">
-        <v>4336</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="1523" spans="1:2">
       <c r="A1523" s="1" t="s">
-        <v>4337</v>
+        <v>4329</v>
       </c>
       <c r="B1523" t="s">
-        <v>4338</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="1524" spans="1:2">
       <c r="A1524" s="1" t="s">
-        <v>4339</v>
+        <v>4331</v>
       </c>
       <c r="B1524" t="s">
-        <v>4340</v>
+        <v>4332</v>
       </c>
     </row>
     <row r="1525" spans="1:2">
       <c r="A1525" s="1" t="s">
-        <v>4341</v>
+        <v>4333</v>
       </c>
       <c r="B1525" t="s">
-        <v>4342</v>
+        <v>4334</v>
       </c>
     </row>
     <row r="1526" spans="1:2">
       <c r="A1526" s="1" t="s">
-        <v>4343</v>
+        <v>4335</v>
       </c>
       <c r="B1526" t="s">
-        <v>4344</v>
+        <v>4336</v>
       </c>
     </row>
     <row r="1527" spans="1:2">
       <c r="A1527" s="1" t="s">
-        <v>4345</v>
+        <v>4337</v>
       </c>
       <c r="B1527" t="s">
-        <v>4346</v>
+        <v>4338</v>
       </c>
     </row>
     <row r="1528" spans="1:2">
       <c r="A1528" s="1" t="s">
-        <v>4347</v>
+        <v>4339</v>
       </c>
       <c r="B1528" t="s">
-        <v>4348</v>
+        <v>4340</v>
       </c>
     </row>
     <row r="1529" spans="1:2">
       <c r="A1529" s="1" t="s">
-        <v>4349</v>
+        <v>4341</v>
       </c>
       <c r="B1529" t="s">
-        <v>4350</v>
+        <v>4342</v>
       </c>
     </row>
     <row r="1530" spans="1:2">
       <c r="A1530" s="1" t="s">
-        <v>4351</v>
+        <v>4343</v>
       </c>
       <c r="B1530" t="s">
-        <v>4352</v>
+        <v>4344</v>
       </c>
     </row>
     <row r="1531" spans="1:2">
       <c r="A1531" s="1" t="s">
-        <v>4353</v>
+        <v>4345</v>
       </c>
       <c r="B1531" t="s">
-        <v>4354</v>
+        <v>4346</v>
       </c>
     </row>
     <row r="1532" spans="1:2">
       <c r="A1532" s="1" t="s">
-        <v>4355</v>
+        <v>4347</v>
       </c>
       <c r="B1532" t="s">
-        <v>4356</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="1533" spans="1:2">
       <c r="A1533" s="1" t="s">
-        <v>4357</v>
+        <v>4349</v>
       </c>
       <c r="B1533" t="s">
-        <v>4358</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="1534" spans="1:2">
       <c r="A1534" s="1" t="s">
-        <v>4359</v>
+        <v>4351</v>
       </c>
       <c r="B1534" t="s">
-        <v>4360</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="1535" spans="1:2">
       <c r="A1535" s="1" t="s">
-        <v>4361</v>
+        <v>4353</v>
       </c>
       <c r="B1535" t="s">
-        <v>4362</v>
+        <v>4354</v>
       </c>
     </row>
     <row r="1536" spans="1:2">
       <c r="A1536" s="1" t="s">
-        <v>4363</v>
+        <v>4355</v>
       </c>
       <c r="B1536" t="s">
-        <v>4364</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="1537" spans="1:2">
       <c r="A1537" s="1" t="s">
-        <v>4365</v>
+        <v>4357</v>
       </c>
       <c r="B1537" t="s">
-        <v>4366</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="1538" spans="1:2">
       <c r="A1538" s="1" t="s">
-        <v>4427</v>
+        <v>4359</v>
       </c>
       <c r="B1538" t="s">
-        <v>4428</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="1539" spans="1:2">
       <c r="A1539" s="1" t="s">
-        <v>4367</v>
+        <v>4361</v>
       </c>
       <c r="B1539" t="s">
-        <v>4368</v>
+        <v>4362</v>
       </c>
     </row>
     <row r="1540" spans="1:2">
       <c r="A1540" s="1" t="s">
-        <v>4369</v>
+        <v>4363</v>
       </c>
       <c r="B1540" t="s">
-        <v>4370</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="1541" spans="1:2">
       <c r="A1541" s="1" t="s">
-        <v>4371</v>
+        <v>4365</v>
       </c>
       <c r="B1541" t="s">
-        <v>4372</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="1542" spans="1:2">
       <c r="A1542" s="1" t="s">
-        <v>4373</v>
+        <v>4427</v>
       </c>
       <c r="B1542" t="s">
-        <v>4374</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="1543" spans="1:2">
       <c r="A1543" s="1" t="s">
-        <v>4375</v>
+        <v>4367</v>
       </c>
       <c r="B1543" t="s">
-        <v>4376</v>
+        <v>4368</v>
       </c>
     </row>
     <row r="1544" spans="1:2">
       <c r="A1544" s="1" t="s">
-        <v>4377</v>
+        <v>4369</v>
       </c>
       <c r="B1544" t="s">
-        <v>4378</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="1545" spans="1:2">
       <c r="A1545" s="1" t="s">
-        <v>4379</v>
+        <v>4371</v>
       </c>
       <c r="B1545" t="s">
-        <v>4380</v>
+        <v>4372</v>
       </c>
     </row>
     <row r="1546" spans="1:2">
       <c r="A1546" s="1" t="s">
-        <v>4438</v>
+        <v>4373</v>
       </c>
       <c r="B1546" t="s">
-        <v>4439</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="1547" spans="1:2">
       <c r="A1547" s="1" t="s">
-        <v>4381</v>
+        <v>4375</v>
       </c>
       <c r="B1547" t="s">
-        <v>4382</v>
+        <v>4376</v>
       </c>
     </row>
     <row r="1548" spans="1:2">
       <c r="A1548" s="1" t="s">
-        <v>4383</v>
+        <v>4377</v>
       </c>
       <c r="B1548" t="s">
-        <v>4384</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="1549" spans="1:2">
       <c r="A1549" s="1" t="s">
-        <v>4385</v>
+        <v>4379</v>
       </c>
       <c r="B1549" t="s">
-        <v>4386</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="1550" spans="1:2">
       <c r="A1550" s="1" t="s">
-        <v>4387</v>
+        <v>4438</v>
       </c>
       <c r="B1550" t="s">
-        <v>4388</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="1551" spans="1:2">
       <c r="A1551" s="1" t="s">
-        <v>4389</v>
+        <v>4381</v>
       </c>
       <c r="B1551" t="s">
-        <v>4390</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="1552" spans="1:2">
       <c r="A1552" s="1" t="s">
-        <v>4391</v>
+        <v>4383</v>
       </c>
       <c r="B1552" t="s">
-        <v>4392</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="1553" spans="1:2">
       <c r="A1553" s="1" t="s">
-        <v>4393</v>
+        <v>4385</v>
       </c>
       <c r="B1553" t="s">
-        <v>4394</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="1554" spans="1:2">
       <c r="A1554" s="1" t="s">
-        <v>4395</v>
+        <v>4387</v>
       </c>
       <c r="B1554" t="s">
-        <v>4396</v>
+        <v>4388</v>
       </c>
     </row>
     <row r="1555" spans="1:2">
       <c r="A1555" s="1" t="s">
-        <v>4397</v>
+        <v>4389</v>
       </c>
       <c r="B1555" t="s">
-        <v>4398</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="1556" spans="1:2">
       <c r="A1556" s="1" t="s">
-        <v>4399</v>
+        <v>4391</v>
       </c>
       <c r="B1556" t="s">
-        <v>4400</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="1557" spans="1:2">
       <c r="A1557" s="1" t="s">
-        <v>4401</v>
+        <v>4393</v>
       </c>
       <c r="B1557" t="s">
-        <v>4402</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="1558" spans="1:2">
       <c r="A1558" s="1" t="s">
-        <v>4403</v>
+        <v>4395</v>
       </c>
       <c r="B1558" t="s">
-        <v>4404</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="1559" spans="1:2">
       <c r="A1559" s="1" t="s">
-        <v>4405</v>
+        <v>4397</v>
       </c>
       <c r="B1559" t="s">
-        <v>4406</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="1560" spans="1:2">
       <c r="A1560" s="1" t="s">
+        <v>4399</v>
+      </c>
+      <c r="B1560" t="s">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:2">
+      <c r="A1561" s="1" t="s">
+        <v>4401</v>
+      </c>
+      <c r="B1561" t="s">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:2">
+      <c r="A1562" s="1" t="s">
+        <v>4403</v>
+      </c>
+      <c r="B1562" t="s">
+        <v>4404</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:2">
+      <c r="A1563" s="1" t="s">
+        <v>4405</v>
+      </c>
+      <c r="B1563" t="s">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:2">
+      <c r="A1564" s="1" t="s">
         <v>4407</v>
       </c>
-      <c r="B1560" t="s">
+      <c r="B1564" t="s">
         <v>4408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: update a document
</commit_message>
<xml_diff>
--- a/public/6. COA.xlsx
+++ b/public/6. COA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patience.uwase\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E1781F2-D358-4C20-A65D-F1F4AB24A345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45E948A4-F7DF-4CA5-B4D1-8F6F027474FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier Details" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4487" uniqueCount="4450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4488" uniqueCount="4451">
   <si>
     <t>ACCESS BANK -USD</t>
   </si>
@@ -13395,6 +13395,9 @@
   </si>
   <si>
     <t>PUMA SOUTH AFRICA</t>
+  </si>
+  <si>
+    <t>Photo Copiers and Fax Equipment rentals</t>
   </si>
 </sst>
 </file>
@@ -13654,7 +13657,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -13769,13 +13772,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -14090,8 +14107,8 @@
   </sheetPr>
   <dimension ref="A1:B1564"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1254" workbookViewId="0">
-      <selection activeCell="B1271" sqref="B1271"/>
+    <sheetView topLeftCell="A1255" workbookViewId="0">
+      <selection activeCell="A1268" sqref="A1268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -26613,6 +26630,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -27869,10 +27889,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B1386"/>
+  <dimension ref="A1:B1387"/>
   <sheetViews>
-    <sheetView topLeftCell="A989" workbookViewId="0">
-      <selection activeCell="B1017" sqref="B1017"/>
+    <sheetView tabSelected="1" topLeftCell="A890" workbookViewId="0">
+      <selection activeCell="B902" sqref="B902"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35139,999 +35159,1003 @@
     </row>
     <row r="908" spans="1:2" s="8" customFormat="1">
       <c r="A908" s="6">
-        <v>5751</v>
-      </c>
-      <c r="B908" s="7" t="s">
-        <v>904</v>
+        <v>5733</v>
+      </c>
+      <c r="B908" s="72" t="s">
+        <v>4450</v>
       </c>
     </row>
     <row r="909" spans="1:2" s="8" customFormat="1">
       <c r="A909" s="6">
-        <v>5752</v>
+        <v>5751</v>
       </c>
       <c r="B909" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="910" spans="1:2" s="8" customFormat="1">
       <c r="A910" s="6">
-        <v>5753</v>
+        <v>5752</v>
       </c>
       <c r="B910" s="7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="911" spans="1:2" s="8" customFormat="1">
       <c r="A911" s="6">
-        <v>5754</v>
+        <v>5753</v>
       </c>
       <c r="B911" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="912" spans="1:2" s="8" customFormat="1">
       <c r="A912" s="6">
-        <v>5755</v>
+        <v>5754</v>
       </c>
       <c r="B912" s="7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="913" spans="1:2" s="8" customFormat="1">
       <c r="A913" s="6">
-        <v>5756</v>
+        <v>5755</v>
       </c>
       <c r="B913" s="7" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="914" spans="1:2" s="8" customFormat="1">
       <c r="A914" s="6">
-        <v>5757</v>
+        <v>5756</v>
       </c>
       <c r="B914" s="7" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="915" spans="1:2" s="8" customFormat="1">
       <c r="A915" s="6">
-        <v>5761</v>
+        <v>5757</v>
       </c>
       <c r="B915" s="7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="916" spans="1:2" s="8" customFormat="1">
       <c r="A916" s="6">
-        <v>5762</v>
+        <v>5761</v>
       </c>
       <c r="B916" s="7" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="917" spans="1:2" s="8" customFormat="1">
       <c r="A917" s="6">
-        <v>5763</v>
+        <v>5762</v>
       </c>
       <c r="B917" s="7" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="918" spans="1:2" s="8" customFormat="1">
       <c r="A918" s="6">
-        <v>5764</v>
+        <v>5763</v>
       </c>
       <c r="B918" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="919" spans="1:2" s="8" customFormat="1">
       <c r="A919" s="6">
-        <v>5765</v>
+        <v>5764</v>
       </c>
       <c r="B919" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="920" spans="1:2" s="8" customFormat="1">
       <c r="A920" s="6">
-        <v>5766</v>
+        <v>5765</v>
       </c>
       <c r="B920" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="921" spans="1:2" s="8" customFormat="1">
       <c r="A921" s="6">
-        <v>5767</v>
+        <v>5766</v>
       </c>
       <c r="B921" s="7" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="922" spans="1:2" s="8" customFormat="1">
       <c r="A922" s="6">
-        <v>5768</v>
+        <v>5767</v>
       </c>
       <c r="B922" s="7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="923" spans="1:2" s="8" customFormat="1">
       <c r="A923" s="6">
-        <v>5769</v>
+        <v>5768</v>
       </c>
       <c r="B923" s="7" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="924" spans="1:2" s="8" customFormat="1">
       <c r="A924" s="6">
-        <v>5771</v>
+        <v>5769</v>
       </c>
       <c r="B924" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="925" spans="1:2" s="8" customFormat="1">
       <c r="A925" s="6">
-        <v>5772</v>
+        <v>5771</v>
       </c>
       <c r="B925" s="7" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="926" spans="1:2" s="8" customFormat="1">
       <c r="A926" s="6">
-        <v>5773</v>
+        <v>5772</v>
       </c>
       <c r="B926" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="927" spans="1:2" s="8" customFormat="1">
       <c r="A927" s="6">
-        <v>5774</v>
+        <v>5773</v>
       </c>
       <c r="B927" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="928" spans="1:2" s="8" customFormat="1">
       <c r="A928" s="6">
-        <v>5775</v>
+        <v>5774</v>
       </c>
       <c r="B928" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="929" spans="1:2" s="8" customFormat="1">
       <c r="A929" s="6">
-        <v>5776</v>
+        <v>5775</v>
       </c>
       <c r="B929" s="7" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="930" spans="1:2" s="8" customFormat="1">
       <c r="A930" s="6">
-        <v>5777</v>
+        <v>5776</v>
       </c>
       <c r="B930" s="7" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="931" spans="1:2" s="8" customFormat="1">
       <c r="A931" s="6">
-        <v>5791</v>
+        <v>5777</v>
       </c>
       <c r="B931" s="7" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="932" spans="1:2" s="8" customFormat="1">
       <c r="A932" s="6">
-        <v>5792</v>
+        <v>5791</v>
       </c>
       <c r="B932" s="7" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="933" spans="1:2" s="8" customFormat="1">
       <c r="A933" s="6">
-        <v>5793</v>
+        <v>5792</v>
       </c>
       <c r="B933" s="7" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="934" spans="1:2" s="8" customFormat="1">
       <c r="A934" s="6">
-        <v>5794</v>
+        <v>5793</v>
       </c>
       <c r="B934" s="7" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="935" spans="1:2" s="8" customFormat="1">
       <c r="A935" s="6">
-        <v>5795</v>
+        <v>5794</v>
       </c>
       <c r="B935" s="7" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="936" spans="1:2" s="8" customFormat="1">
       <c r="A936" s="6">
-        <v>5796</v>
+        <v>5795</v>
       </c>
       <c r="B936" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="937" spans="1:2" s="8" customFormat="1">
       <c r="A937" s="6">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="B937" s="7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="938" spans="1:2" s="8" customFormat="1">
       <c r="A938" s="6">
-        <v>5798</v>
+        <v>5797</v>
       </c>
       <c r="B938" s="7" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="939" spans="1:2" s="8" customFormat="1">
       <c r="A939" s="6">
-        <v>5799</v>
+        <v>5798</v>
       </c>
       <c r="B939" s="7" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="940" spans="1:2" s="8" customFormat="1">
       <c r="A940" s="6">
-        <v>5800</v>
+        <v>5799</v>
       </c>
       <c r="B940" s="7" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="941" spans="1:2" s="8" customFormat="1">
       <c r="A941" s="6">
-        <v>5801</v>
+        <v>5800</v>
       </c>
       <c r="B941" s="7" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="942" spans="1:2" s="8" customFormat="1">
       <c r="A942" s="6">
-        <v>5802</v>
+        <v>5801</v>
       </c>
       <c r="B942" s="7" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="943" spans="1:2" s="8" customFormat="1">
       <c r="A943" s="6">
-        <v>5803</v>
+        <v>5802</v>
       </c>
       <c r="B943" s="7" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="944" spans="1:2" s="8" customFormat="1">
       <c r="A944" s="6">
-        <v>5804</v>
+        <v>5803</v>
       </c>
       <c r="B944" s="7" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="945" spans="1:2" s="8" customFormat="1">
       <c r="A945" s="6">
-        <v>5821</v>
+        <v>5804</v>
       </c>
       <c r="B945" s="7" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="946" spans="1:2" s="8" customFormat="1">
       <c r="A946" s="6">
-        <v>5822</v>
+        <v>5821</v>
       </c>
       <c r="B946" s="7" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="947" spans="1:2" s="8" customFormat="1">
       <c r="A947" s="6">
-        <v>5823</v>
+        <v>5822</v>
       </c>
       <c r="B947" s="7" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="948" spans="1:2" s="8" customFormat="1">
       <c r="A948" s="6">
-        <v>5824</v>
+        <v>5823</v>
       </c>
       <c r="B948" s="7" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="949" spans="1:2" s="8" customFormat="1">
       <c r="A949" s="6">
-        <v>5825</v>
+        <v>5824</v>
       </c>
       <c r="B949" s="7" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="950" spans="1:2" s="8" customFormat="1">
       <c r="A950" s="6">
-        <v>5826</v>
+        <v>5825</v>
       </c>
       <c r="B950" s="7" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="951" spans="1:2" s="8" customFormat="1">
       <c r="A951" s="6">
-        <v>5827</v>
+        <v>5826</v>
       </c>
       <c r="B951" s="7" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="952" spans="1:2" s="8" customFormat="1">
       <c r="A952" s="6">
-        <v>5828</v>
+        <v>5827</v>
       </c>
       <c r="B952" s="7" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="953" spans="1:2" s="8" customFormat="1">
       <c r="A953" s="6">
-        <v>5829</v>
+        <v>5828</v>
       </c>
       <c r="B953" s="7" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="954" spans="1:2" s="8" customFormat="1">
       <c r="A954" s="6">
-        <v>5830</v>
+        <v>5829</v>
       </c>
       <c r="B954" s="7" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="955" spans="1:2" s="8" customFormat="1">
       <c r="A955" s="6">
-        <v>5831</v>
+        <v>5830</v>
       </c>
       <c r="B955" s="7" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="956" spans="1:2" s="8" customFormat="1">
       <c r="A956" s="6">
-        <v>5832</v>
+        <v>5831</v>
       </c>
       <c r="B956" s="7" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="957" spans="1:2" s="8" customFormat="1">
       <c r="A957" s="6">
-        <v>5841</v>
+        <v>5832</v>
       </c>
       <c r="B957" s="7" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="958" spans="1:2" s="8" customFormat="1">
       <c r="A958" s="6">
-        <v>5842</v>
+        <v>5841</v>
       </c>
       <c r="B958" s="7" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="959" spans="1:2" s="8" customFormat="1">
       <c r="A959" s="6">
-        <v>5843</v>
+        <v>5842</v>
       </c>
       <c r="B959" s="7" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="960" spans="1:2" s="8" customFormat="1">
       <c r="A960" s="6">
-        <v>5851</v>
+        <v>5843</v>
       </c>
       <c r="B960" s="7" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="961" spans="1:2" s="8" customFormat="1">
       <c r="A961" s="6">
-        <v>5852</v>
+        <v>5851</v>
       </c>
       <c r="B961" s="7" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="962" spans="1:2" s="8" customFormat="1">
       <c r="A962" s="6">
-        <v>5853</v>
+        <v>5852</v>
       </c>
       <c r="B962" s="7" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="963" spans="1:2" s="8" customFormat="1">
       <c r="A963" s="6">
-        <v>5854</v>
+        <v>5853</v>
       </c>
       <c r="B963" s="7" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="964" spans="1:2" s="8" customFormat="1">
       <c r="A964" s="6">
-        <v>5855</v>
+        <v>5854</v>
       </c>
       <c r="B964" s="7" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="965" spans="1:2" s="8" customFormat="1">
       <c r="A965" s="6">
-        <v>5856</v>
+        <v>5855</v>
       </c>
       <c r="B965" s="7" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="966" spans="1:2" s="8" customFormat="1">
       <c r="A966" s="6">
-        <v>5857</v>
+        <v>5856</v>
       </c>
       <c r="B966" s="7" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="967" spans="1:2" s="8" customFormat="1">
       <c r="A967" s="6">
-        <v>5871</v>
+        <v>5857</v>
       </c>
       <c r="B967" s="7" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="968" spans="1:2" s="8" customFormat="1">
       <c r="A968" s="6">
-        <v>5872</v>
+        <v>5871</v>
       </c>
       <c r="B968" s="7" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="969" spans="1:2" s="8" customFormat="1">
       <c r="A969" s="6">
-        <v>5873</v>
+        <v>5872</v>
       </c>
       <c r="B969" s="7" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="970" spans="1:2" s="8" customFormat="1">
       <c r="A970" s="6">
-        <v>5874</v>
+        <v>5873</v>
       </c>
       <c r="B970" s="7" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="971" spans="1:2" s="8" customFormat="1">
       <c r="A971" s="6">
-        <v>5875</v>
+        <v>5874</v>
       </c>
       <c r="B971" s="7" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="972" spans="1:2" s="8" customFormat="1">
       <c r="A972" s="6">
-        <v>5876</v>
+        <v>5875</v>
       </c>
       <c r="B972" s="7" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="973" spans="1:2" s="8" customFormat="1">
       <c r="A973" s="6">
-        <v>5877</v>
+        <v>5876</v>
       </c>
       <c r="B973" s="7" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="974" spans="1:2" s="8" customFormat="1">
       <c r="A974" s="6">
-        <v>5878</v>
+        <v>5877</v>
       </c>
       <c r="B974" s="7" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="975" spans="1:2" s="8" customFormat="1">
       <c r="A975" s="6">
-        <v>5879</v>
+        <v>5878</v>
       </c>
       <c r="B975" s="7" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="976" spans="1:2" s="8" customFormat="1">
       <c r="A976" s="6">
-        <v>5880</v>
+        <v>5879</v>
       </c>
       <c r="B976" s="7" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="977" spans="1:2" s="8" customFormat="1">
       <c r="A977" s="6">
-        <v>5881</v>
+        <v>5880</v>
       </c>
       <c r="B977" s="7" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="978" spans="1:2" s="8" customFormat="1">
       <c r="A978" s="6">
-        <v>5882</v>
+        <v>5881</v>
       </c>
       <c r="B978" s="7" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="979" spans="1:2" s="8" customFormat="1">
       <c r="A979" s="6">
-        <v>5883</v>
+        <v>5882</v>
       </c>
       <c r="B979" s="7" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="980" spans="1:2" s="8" customFormat="1">
       <c r="A980" s="6">
-        <v>5884</v>
+        <v>5883</v>
       </c>
       <c r="B980" s="7" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="981" spans="1:2" s="8" customFormat="1">
       <c r="A981" s="6">
-        <v>5885</v>
+        <v>5884</v>
       </c>
       <c r="B981" s="7" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="982" spans="1:2" s="8" customFormat="1">
       <c r="A982" s="6">
-        <v>5886</v>
+        <v>5885</v>
       </c>
       <c r="B982" s="7" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="983" spans="1:2" s="8" customFormat="1">
       <c r="A983" s="6">
-        <v>5887</v>
+        <v>5886</v>
       </c>
       <c r="B983" s="7" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="984" spans="1:2" s="8" customFormat="1">
       <c r="A984" s="6">
-        <v>5888</v>
+        <v>5887</v>
       </c>
       <c r="B984" s="7" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="985" spans="1:2" s="8" customFormat="1">
       <c r="A985" s="6">
-        <v>5889</v>
+        <v>5888</v>
       </c>
       <c r="B985" s="7" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="986" spans="1:2" s="8" customFormat="1">
       <c r="A986" s="6">
-        <v>5890</v>
+        <v>5889</v>
       </c>
       <c r="B986" s="7" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="987" spans="1:2" s="8" customFormat="1">
       <c r="A987" s="6">
-        <v>5891</v>
+        <v>5890</v>
       </c>
       <c r="B987" s="7" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="988" spans="1:2" s="8" customFormat="1">
       <c r="A988" s="6">
-        <v>5892</v>
+        <v>5891</v>
       </c>
       <c r="B988" s="7" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="989" spans="1:2" s="8" customFormat="1">
       <c r="A989" s="6">
-        <v>5893</v>
+        <v>5892</v>
       </c>
       <c r="B989" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="990" spans="1:2" s="8" customFormat="1">
       <c r="A990" s="6">
-        <v>5894</v>
+        <v>5893</v>
       </c>
       <c r="B990" s="7" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="991" spans="1:2" s="8" customFormat="1">
       <c r="A991" s="6">
-        <v>5895</v>
+        <v>5894</v>
       </c>
       <c r="B991" s="7" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="992" spans="1:2" s="8" customFormat="1">
       <c r="A992" s="6">
-        <v>5896</v>
+        <v>5895</v>
       </c>
       <c r="B992" s="7" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="993" spans="1:2" s="8" customFormat="1">
       <c r="A993" s="6">
-        <v>5897</v>
+        <v>5896</v>
       </c>
       <c r="B993" s="7" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="994" spans="1:2" s="8" customFormat="1">
       <c r="A994" s="6">
-        <v>5898</v>
+        <v>5897</v>
       </c>
       <c r="B994" s="7" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="995" spans="1:2" s="8" customFormat="1">
       <c r="A995" s="6">
-        <v>5899</v>
+        <v>5898</v>
       </c>
       <c r="B995" s="7" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="996" spans="1:2" s="8" customFormat="1">
       <c r="A996" s="6">
-        <v>5900</v>
+        <v>5899</v>
       </c>
       <c r="B996" s="7" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="997" spans="1:2" s="8" customFormat="1">
       <c r="A997" s="6">
-        <v>5901</v>
+        <v>5900</v>
       </c>
       <c r="B997" s="7" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="998" spans="1:2" s="8" customFormat="1">
       <c r="A998" s="6">
-        <v>5902</v>
+        <v>5901</v>
       </c>
       <c r="B998" s="7" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="999" spans="1:2" s="8" customFormat="1">
       <c r="A999" s="6">
-        <v>5903</v>
+        <v>5902</v>
       </c>
       <c r="B999" s="7" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="1000" spans="1:2" s="8" customFormat="1">
       <c r="A1000" s="6">
-        <v>5904</v>
+        <v>5903</v>
       </c>
       <c r="B1000" s="7" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="1001" spans="1:2" s="8" customFormat="1">
       <c r="A1001" s="6">
-        <v>5905</v>
+        <v>5904</v>
       </c>
       <c r="B1001" s="7" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="1002" spans="1:2" s="8" customFormat="1">
       <c r="A1002" s="6">
-        <v>5906</v>
+        <v>5905</v>
       </c>
       <c r="B1002" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="1003" spans="1:2" s="8" customFormat="1">
       <c r="A1003" s="6">
-        <v>5907</v>
+        <v>5906</v>
       </c>
       <c r="B1003" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="1004" spans="1:2" s="8" customFormat="1">
       <c r="A1004" s="6">
-        <v>5908</v>
+        <v>5907</v>
       </c>
       <c r="B1004" s="7" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="1005" spans="1:2" s="8" customFormat="1">
       <c r="A1005" s="6">
-        <v>5909</v>
+        <v>5908</v>
       </c>
       <c r="B1005" s="7" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="1006" spans="1:2" s="8" customFormat="1">
       <c r="A1006" s="6">
-        <v>5910</v>
+        <v>5909</v>
       </c>
       <c r="B1006" s="7" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="1007" spans="1:2" s="8" customFormat="1">
       <c r="A1007" s="6">
-        <v>6111</v>
+        <v>5910</v>
       </c>
       <c r="B1007" s="7" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="1008" spans="1:2" s="8" customFormat="1">
       <c r="A1008" s="6">
-        <v>6112</v>
+        <v>6111</v>
       </c>
       <c r="B1008" s="7" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="1009" spans="1:2" s="8" customFormat="1">
       <c r="A1009" s="6">
-        <v>6113</v>
+        <v>6112</v>
       </c>
       <c r="B1009" s="7" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="1010" spans="1:2" s="8" customFormat="1">
       <c r="A1010" s="6">
-        <v>6114</v>
+        <v>6113</v>
       </c>
       <c r="B1010" s="7" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="1011" spans="1:2" s="8" customFormat="1">
       <c r="A1011" s="6">
-        <v>6115</v>
+        <v>6114</v>
       </c>
       <c r="B1011" s="7" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="1012" spans="1:2" s="8" customFormat="1">
       <c r="A1012" s="6">
-        <v>6116</v>
+        <v>6115</v>
       </c>
       <c r="B1012" s="7" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="1013" spans="1:2" s="8" customFormat="1">
       <c r="A1013" s="6">
-        <v>6117</v>
+        <v>6116</v>
       </c>
       <c r="B1013" s="7" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="1014" spans="1:2" s="8" customFormat="1">
       <c r="A1014" s="6">
-        <v>6118</v>
+        <v>6117</v>
       </c>
       <c r="B1014" s="7" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="1015" spans="1:2" s="8" customFormat="1">
       <c r="A1015" s="6">
-        <v>6119</v>
+        <v>6118</v>
       </c>
       <c r="B1015" s="7" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="1016" spans="1:2" s="8" customFormat="1">
       <c r="A1016" s="6">
-        <v>6120</v>
+        <v>6119</v>
       </c>
       <c r="B1016" s="7" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="1017" spans="1:2" s="8" customFormat="1">
       <c r="A1017" s="6">
-        <v>6121</v>
+        <v>6120</v>
       </c>
       <c r="B1017" s="7" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="1018" spans="1:2" s="8" customFormat="1">
       <c r="A1018" s="6">
-        <v>6131</v>
+        <v>6121</v>
       </c>
       <c r="B1018" s="7" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="1019" spans="1:2" s="8" customFormat="1">
       <c r="A1019" s="6">
-        <v>6151</v>
+        <v>6131</v>
       </c>
       <c r="B1019" s="7" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="1020" spans="1:2" s="8" customFormat="1">
       <c r="A1020" s="6">
-        <v>6152</v>
+        <v>6151</v>
       </c>
       <c r="B1020" s="7" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="1021" spans="1:2" s="8" customFormat="1">
       <c r="A1021" s="6">
-        <v>6153</v>
+        <v>6152</v>
       </c>
       <c r="B1021" s="7" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="1022" spans="1:2" s="8" customFormat="1">
       <c r="A1022" s="6">
-        <v>6171</v>
+        <v>6153</v>
       </c>
       <c r="B1022" s="7" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="1023" spans="1:2" s="8" customFormat="1">
       <c r="A1023" s="6">
-        <v>6172</v>
+        <v>6171</v>
       </c>
       <c r="B1023" s="7" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="1024" spans="1:2" s="8" customFormat="1">
       <c r="A1024" s="6">
-        <v>6173</v>
+        <v>6172</v>
       </c>
       <c r="B1024" s="7" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="1025" spans="1:2" s="8" customFormat="1">
       <c r="A1025" s="6">
-        <v>6174</v>
+        <v>6173</v>
       </c>
       <c r="B1025" s="7" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="1026" spans="1:2" s="8" customFormat="1">
       <c r="A1026" s="6">
-        <v>6191</v>
+        <v>6174</v>
       </c>
       <c r="B1026" s="7" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="1027" spans="1:2" s="8" customFormat="1">
       <c r="A1027" s="6">
-        <v>6192</v>
+        <v>6191</v>
       </c>
       <c r="B1027" s="7" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="1028" spans="1:2" s="8" customFormat="1">
       <c r="A1028" s="6">
-        <v>7201</v>
+        <v>6192</v>
       </c>
       <c r="B1028" s="7" t="s">
-        <v>535</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="1029" spans="1:2" s="8" customFormat="1">
       <c r="A1029" s="6">
-        <v>7202</v>
+        <v>7201</v>
       </c>
       <c r="B1029" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="1030" spans="1:2" s="8" customFormat="1">
       <c r="A1030" s="6">
-        <v>7203</v>
+        <v>7202</v>
       </c>
       <c r="B1030" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="1031" spans="1:2" s="8" customFormat="1">
       <c r="A1031" s="6">
+        <v>7203</v>
+      </c>
+      <c r="B1031" s="7" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:2" s="8" customFormat="1">
+      <c r="A1032" s="6">
         <v>7301</v>
       </c>
-      <c r="B1031" s="7" t="s">
+      <c r="B1032" s="7" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="1032" spans="1:2">
-      <c r="A1032"/>
-      <c r="B1032"/>
     </row>
     <row r="1033" spans="1:2">
       <c r="A1033"/>
@@ -36165,1390 +36189,353 @@
       <c r="A1040"/>
       <c r="B1040"/>
     </row>
-    <row r="1041" spans="1:2">
-      <c r="A1041"/>
-      <c r="B1041"/>
-    </row>
-    <row r="1042" spans="1:2">
-      <c r="A1042"/>
-      <c r="B1042"/>
-    </row>
-    <row r="1043" spans="1:2">
-      <c r="A1043"/>
-      <c r="B1043"/>
-    </row>
-    <row r="1044" spans="1:2">
-      <c r="A1044"/>
-      <c r="B1044"/>
-    </row>
-    <row r="1045" spans="1:2">
-      <c r="A1045"/>
-      <c r="B1045"/>
-    </row>
-    <row r="1046" spans="1:2">
-      <c r="A1046"/>
-      <c r="B1046"/>
-    </row>
-    <row r="1047" spans="1:2">
-      <c r="A1047"/>
-      <c r="B1047"/>
-    </row>
-    <row r="1048" spans="1:2">
-      <c r="A1048"/>
-      <c r="B1048"/>
-    </row>
-    <row r="1049" spans="1:2">
-      <c r="A1049"/>
-      <c r="B1049"/>
-    </row>
-    <row r="1050" spans="1:2">
-      <c r="A1050"/>
-      <c r="B1050"/>
-    </row>
-    <row r="1051" spans="1:2">
-      <c r="A1051"/>
-      <c r="B1051"/>
-    </row>
-    <row r="1052" spans="1:2">
-      <c r="A1052"/>
-      <c r="B1052"/>
-    </row>
-    <row r="1053" spans="1:2">
-      <c r="A1053"/>
-      <c r="B1053"/>
-    </row>
-    <row r="1054" spans="1:2">
-      <c r="A1054"/>
-      <c r="B1054"/>
-    </row>
-    <row r="1055" spans="1:2">
-      <c r="A1055"/>
-      <c r="B1055"/>
-    </row>
-    <row r="1056" spans="1:2">
-      <c r="A1056"/>
-      <c r="B1056"/>
-    </row>
-    <row r="1057" spans="1:2">
-      <c r="A1057"/>
-      <c r="B1057"/>
-    </row>
-    <row r="1058" spans="1:2">
-      <c r="A1058"/>
-      <c r="B1058"/>
-    </row>
-    <row r="1059" spans="1:2">
-      <c r="A1059"/>
-      <c r="B1059"/>
-    </row>
-    <row r="1060" spans="1:2">
-      <c r="A1060"/>
-      <c r="B1060"/>
-    </row>
-    <row r="1061" spans="1:2">
-      <c r="A1061"/>
-      <c r="B1061"/>
-    </row>
-    <row r="1062" spans="1:2">
-      <c r="A1062"/>
-      <c r="B1062"/>
-    </row>
-    <row r="1063" spans="1:2">
-      <c r="A1063"/>
-      <c r="B1063"/>
-    </row>
-    <row r="1064" spans="1:2">
-      <c r="A1064"/>
-      <c r="B1064"/>
-    </row>
-    <row r="1065" spans="1:2">
-      <c r="A1065"/>
-      <c r="B1065"/>
-    </row>
-    <row r="1066" spans="1:2">
-      <c r="A1066"/>
-      <c r="B1066"/>
-    </row>
-    <row r="1067" spans="1:2">
-      <c r="A1067"/>
-      <c r="B1067"/>
-    </row>
-    <row r="1068" spans="1:2">
-      <c r="A1068"/>
-      <c r="B1068"/>
-    </row>
-    <row r="1069" spans="1:2">
-      <c r="A1069"/>
-      <c r="B1069"/>
-    </row>
-    <row r="1070" spans="1:2">
-      <c r="A1070"/>
-      <c r="B1070"/>
-    </row>
-    <row r="1071" spans="1:2">
-      <c r="A1071"/>
-      <c r="B1071"/>
-    </row>
-    <row r="1072" spans="1:2">
-      <c r="A1072"/>
-      <c r="B1072"/>
-    </row>
-    <row r="1073" spans="1:2">
-      <c r="A1073"/>
-      <c r="B1073"/>
-    </row>
-    <row r="1074" spans="1:2">
-      <c r="A1074"/>
-      <c r="B1074"/>
-    </row>
-    <row r="1075" spans="1:2">
-      <c r="A1075"/>
-      <c r="B1075"/>
-    </row>
-    <row r="1076" spans="1:2">
-      <c r="A1076"/>
-      <c r="B1076"/>
-    </row>
-    <row r="1077" spans="1:2">
-      <c r="A1077"/>
-      <c r="B1077"/>
-    </row>
-    <row r="1078" spans="1:2">
-      <c r="A1078"/>
-      <c r="B1078"/>
-    </row>
-    <row r="1079" spans="1:2">
-      <c r="A1079"/>
-      <c r="B1079"/>
-    </row>
-    <row r="1080" spans="1:2">
-      <c r="A1080"/>
-      <c r="B1080"/>
-    </row>
-    <row r="1081" spans="1:2">
-      <c r="A1081"/>
-      <c r="B1081"/>
-    </row>
-    <row r="1082" spans="1:2">
-      <c r="A1082"/>
-      <c r="B1082"/>
-    </row>
-    <row r="1083" spans="1:2">
-      <c r="A1083"/>
-      <c r="B1083"/>
-    </row>
-    <row r="1084" spans="1:2">
-      <c r="A1084"/>
-      <c r="B1084"/>
-    </row>
-    <row r="1085" spans="1:2">
-      <c r="A1085"/>
-      <c r="B1085"/>
-    </row>
-    <row r="1086" spans="1:2">
-      <c r="A1086"/>
-      <c r="B1086"/>
-    </row>
-    <row r="1087" spans="1:2">
-      <c r="A1087"/>
-      <c r="B1087"/>
-    </row>
-    <row r="1088" spans="1:2">
-      <c r="A1088"/>
-      <c r="B1088"/>
-    </row>
-    <row r="1089" spans="1:2">
-      <c r="A1089"/>
-      <c r="B1089"/>
-    </row>
-    <row r="1090" spans="1:2">
-      <c r="A1090"/>
-      <c r="B1090"/>
-    </row>
-    <row r="1091" spans="1:2">
-      <c r="A1091"/>
-      <c r="B1091"/>
-    </row>
-    <row r="1092" spans="1:2">
-      <c r="A1092"/>
-      <c r="B1092"/>
-    </row>
-    <row r="1093" spans="1:2">
-      <c r="A1093"/>
-      <c r="B1093"/>
-    </row>
-    <row r="1094" spans="1:2">
-      <c r="A1094"/>
-      <c r="B1094"/>
-    </row>
-    <row r="1095" spans="1:2">
-      <c r="A1095"/>
-      <c r="B1095"/>
-    </row>
-    <row r="1096" spans="1:2">
-      <c r="A1096"/>
-      <c r="B1096"/>
-    </row>
-    <row r="1097" spans="1:2">
-      <c r="A1097"/>
-      <c r="B1097"/>
-    </row>
-    <row r="1098" spans="1:2">
-      <c r="A1098"/>
-      <c r="B1098"/>
-    </row>
-    <row r="1099" spans="1:2">
-      <c r="A1099"/>
-      <c r="B1099"/>
-    </row>
-    <row r="1100" spans="1:2">
-      <c r="A1100"/>
-      <c r="B1100"/>
-    </row>
-    <row r="1101" spans="1:2">
-      <c r="A1101"/>
-      <c r="B1101"/>
-    </row>
-    <row r="1102" spans="1:2">
-      <c r="A1102"/>
-      <c r="B1102"/>
-    </row>
-    <row r="1103" spans="1:2">
-      <c r="A1103"/>
-      <c r="B1103"/>
-    </row>
-    <row r="1104" spans="1:2">
-      <c r="A1104"/>
-      <c r="B1104"/>
-    </row>
-    <row r="1105" spans="1:2">
-      <c r="A1105"/>
-      <c r="B1105"/>
-    </row>
-    <row r="1106" spans="1:2">
-      <c r="A1106"/>
-      <c r="B1106"/>
-    </row>
-    <row r="1107" spans="1:2">
-      <c r="A1107"/>
-      <c r="B1107"/>
-    </row>
-    <row r="1108" spans="1:2">
-      <c r="A1108"/>
-      <c r="B1108"/>
-    </row>
-    <row r="1109" spans="1:2">
-      <c r="A1109"/>
-      <c r="B1109"/>
-    </row>
-    <row r="1110" spans="1:2">
-      <c r="A1110"/>
-      <c r="B1110"/>
-    </row>
-    <row r="1111" spans="1:2">
-      <c r="A1111"/>
-      <c r="B1111"/>
-    </row>
-    <row r="1112" spans="1:2">
-      <c r="A1112"/>
-      <c r="B1112"/>
-    </row>
-    <row r="1113" spans="1:2">
-      <c r="A1113"/>
-      <c r="B1113"/>
-    </row>
-    <row r="1114" spans="1:2">
-      <c r="A1114"/>
-      <c r="B1114"/>
-    </row>
-    <row r="1115" spans="1:2">
-      <c r="A1115"/>
-      <c r="B1115"/>
-    </row>
-    <row r="1116" spans="1:2">
-      <c r="A1116"/>
-      <c r="B1116"/>
-    </row>
-    <row r="1117" spans="1:2">
-      <c r="A1117"/>
-      <c r="B1117"/>
-    </row>
-    <row r="1118" spans="1:2">
-      <c r="A1118"/>
-      <c r="B1118"/>
-    </row>
-    <row r="1119" spans="1:2">
-      <c r="A1119"/>
-      <c r="B1119"/>
-    </row>
-    <row r="1120" spans="1:2">
-      <c r="A1120"/>
-      <c r="B1120"/>
-    </row>
-    <row r="1121" spans="1:2">
-      <c r="A1121"/>
-      <c r="B1121"/>
-    </row>
-    <row r="1122" spans="1:2">
-      <c r="A1122"/>
-      <c r="B1122"/>
-    </row>
-    <row r="1123" spans="1:2">
-      <c r="A1123"/>
-      <c r="B1123"/>
-    </row>
-    <row r="1124" spans="1:2">
-      <c r="A1124"/>
-      <c r="B1124"/>
-    </row>
-    <row r="1125" spans="1:2">
-      <c r="A1125"/>
-      <c r="B1125"/>
-    </row>
-    <row r="1126" spans="1:2">
-      <c r="A1126"/>
-      <c r="B1126"/>
-    </row>
-    <row r="1127" spans="1:2">
-      <c r="A1127"/>
-      <c r="B1127"/>
-    </row>
-    <row r="1128" spans="1:2">
-      <c r="A1128"/>
-      <c r="B1128"/>
-    </row>
-    <row r="1129" spans="1:2">
-      <c r="A1129"/>
-      <c r="B1129"/>
-    </row>
-    <row r="1130" spans="1:2">
-      <c r="A1130"/>
-      <c r="B1130"/>
-    </row>
-    <row r="1131" spans="1:2">
-      <c r="A1131"/>
-      <c r="B1131"/>
-    </row>
-    <row r="1132" spans="1:2">
-      <c r="A1132"/>
-      <c r="B1132"/>
-    </row>
-    <row r="1133" spans="1:2">
-      <c r="A1133"/>
-      <c r="B1133"/>
-    </row>
-    <row r="1134" spans="1:2">
-      <c r="A1134"/>
-      <c r="B1134"/>
-    </row>
-    <row r="1135" spans="1:2">
-      <c r="A1135"/>
-      <c r="B1135"/>
-    </row>
-    <row r="1136" spans="1:2">
-      <c r="A1136"/>
-      <c r="B1136"/>
-    </row>
-    <row r="1137" spans="1:2">
-      <c r="A1137"/>
-      <c r="B1137"/>
-    </row>
-    <row r="1138" spans="1:2">
-      <c r="A1138"/>
-      <c r="B1138"/>
-    </row>
-    <row r="1139" spans="1:2">
-      <c r="A1139"/>
-      <c r="B1139"/>
-    </row>
-    <row r="1140" spans="1:2">
-      <c r="A1140"/>
-      <c r="B1140"/>
-    </row>
-    <row r="1141" spans="1:2">
-      <c r="A1141"/>
-      <c r="B1141"/>
-    </row>
-    <row r="1142" spans="1:2">
-      <c r="A1142"/>
-      <c r="B1142"/>
-    </row>
-    <row r="1143" spans="1:2">
-      <c r="A1143"/>
-      <c r="B1143"/>
-    </row>
-    <row r="1144" spans="1:2">
-      <c r="A1144"/>
-      <c r="B1144"/>
-    </row>
-    <row r="1145" spans="1:2">
-      <c r="A1145"/>
-      <c r="B1145"/>
-    </row>
-    <row r="1146" spans="1:2">
-      <c r="A1146"/>
-      <c r="B1146"/>
-    </row>
-    <row r="1147" spans="1:2">
-      <c r="A1147"/>
-      <c r="B1147"/>
-    </row>
-    <row r="1148" spans="1:2">
-      <c r="A1148"/>
-      <c r="B1148"/>
-    </row>
-    <row r="1149" spans="1:2">
-      <c r="A1149"/>
-      <c r="B1149"/>
-    </row>
-    <row r="1150" spans="1:2">
-      <c r="A1150"/>
-      <c r="B1150"/>
-    </row>
-    <row r="1151" spans="1:2">
-      <c r="A1151"/>
-      <c r="B1151"/>
-    </row>
-    <row r="1152" spans="1:2">
-      <c r="A1152"/>
-      <c r="B1152"/>
-    </row>
-    <row r="1153" spans="1:2">
-      <c r="A1153"/>
-      <c r="B1153"/>
-    </row>
-    <row r="1154" spans="1:2">
-      <c r="A1154"/>
-      <c r="B1154"/>
-    </row>
-    <row r="1155" spans="1:2">
-      <c r="A1155"/>
-      <c r="B1155"/>
-    </row>
-    <row r="1156" spans="1:2">
-      <c r="A1156"/>
-      <c r="B1156"/>
-    </row>
-    <row r="1157" spans="1:2">
-      <c r="A1157"/>
-      <c r="B1157"/>
-    </row>
-    <row r="1158" spans="1:2">
-      <c r="A1158"/>
-      <c r="B1158"/>
-    </row>
-    <row r="1159" spans="1:2">
-      <c r="A1159"/>
-      <c r="B1159"/>
-    </row>
-    <row r="1160" spans="1:2">
-      <c r="A1160"/>
-      <c r="B1160"/>
-    </row>
-    <row r="1161" spans="1:2">
-      <c r="A1161"/>
-      <c r="B1161"/>
-    </row>
-    <row r="1162" spans="1:2">
-      <c r="A1162"/>
-      <c r="B1162"/>
-    </row>
-    <row r="1163" spans="1:2">
-      <c r="A1163"/>
-      <c r="B1163"/>
-    </row>
-    <row r="1164" spans="1:2">
-      <c r="A1164"/>
-      <c r="B1164"/>
-    </row>
-    <row r="1165" spans="1:2">
-      <c r="A1165"/>
-      <c r="B1165"/>
-    </row>
-    <row r="1166" spans="1:2">
-      <c r="A1166"/>
-      <c r="B1166"/>
-    </row>
-    <row r="1167" spans="1:2">
-      <c r="A1167"/>
-      <c r="B1167"/>
-    </row>
-    <row r="1168" spans="1:2">
-      <c r="A1168"/>
-      <c r="B1168"/>
-    </row>
-    <row r="1169" spans="1:2">
-      <c r="A1169"/>
-      <c r="B1169"/>
-    </row>
-    <row r="1170" spans="1:2">
-      <c r="A1170"/>
-      <c r="B1170"/>
-    </row>
-    <row r="1171" spans="1:2">
-      <c r="A1171"/>
-      <c r="B1171"/>
-    </row>
-    <row r="1172" spans="1:2">
-      <c r="A1172"/>
-      <c r="B1172"/>
-    </row>
-    <row r="1173" spans="1:2">
-      <c r="A1173"/>
-      <c r="B1173"/>
-    </row>
-    <row r="1174" spans="1:2">
-      <c r="A1174"/>
-      <c r="B1174"/>
-    </row>
-    <row r="1175" spans="1:2">
-      <c r="A1175"/>
-      <c r="B1175"/>
-    </row>
-    <row r="1176" spans="1:2">
-      <c r="A1176"/>
-      <c r="B1176"/>
-    </row>
-    <row r="1177" spans="1:2">
-      <c r="A1177"/>
-      <c r="B1177"/>
-    </row>
-    <row r="1178" spans="1:2">
-      <c r="A1178"/>
-      <c r="B1178"/>
-    </row>
-    <row r="1179" spans="1:2">
-      <c r="A1179"/>
-      <c r="B1179"/>
-    </row>
-    <row r="1180" spans="1:2">
-      <c r="A1180"/>
-      <c r="B1180"/>
-    </row>
-    <row r="1181" spans="1:2">
-      <c r="A1181"/>
-      <c r="B1181"/>
-    </row>
-    <row r="1182" spans="1:2">
-      <c r="A1182"/>
-      <c r="B1182"/>
-    </row>
-    <row r="1183" spans="1:2">
-      <c r="A1183"/>
-      <c r="B1183"/>
-    </row>
-    <row r="1184" spans="1:2">
-      <c r="A1184"/>
-      <c r="B1184"/>
-    </row>
-    <row r="1185" spans="1:2">
-      <c r="A1185"/>
-      <c r="B1185"/>
-    </row>
-    <row r="1186" spans="1:2">
-      <c r="A1186"/>
-      <c r="B1186"/>
-    </row>
-    <row r="1187" spans="1:2">
-      <c r="A1187"/>
-      <c r="B1187"/>
-    </row>
-    <row r="1188" spans="1:2">
-      <c r="A1188"/>
-      <c r="B1188"/>
-    </row>
-    <row r="1189" spans="1:2">
-      <c r="A1189"/>
-      <c r="B1189"/>
-    </row>
-    <row r="1190" spans="1:2">
-      <c r="A1190"/>
-      <c r="B1190"/>
-    </row>
-    <row r="1191" spans="1:2">
-      <c r="A1191"/>
-      <c r="B1191"/>
-    </row>
-    <row r="1192" spans="1:2">
-      <c r="A1192"/>
-      <c r="B1192"/>
-    </row>
-    <row r="1193" spans="1:2">
-      <c r="A1193"/>
-      <c r="B1193"/>
-    </row>
-    <row r="1194" spans="1:2">
-      <c r="A1194"/>
-      <c r="B1194"/>
-    </row>
-    <row r="1195" spans="1:2">
-      <c r="A1195"/>
-      <c r="B1195"/>
-    </row>
-    <row r="1196" spans="1:2">
-      <c r="A1196"/>
-      <c r="B1196"/>
-    </row>
-    <row r="1197" spans="1:2">
-      <c r="A1197"/>
-      <c r="B1197"/>
-    </row>
-    <row r="1198" spans="1:2">
-      <c r="A1198"/>
-      <c r="B1198"/>
-    </row>
-    <row r="1199" spans="1:2">
-      <c r="A1199"/>
-      <c r="B1199"/>
-    </row>
-    <row r="1200" spans="1:2">
-      <c r="A1200"/>
-      <c r="B1200"/>
-    </row>
-    <row r="1201" spans="1:2">
-      <c r="A1201"/>
-      <c r="B1201"/>
-    </row>
-    <row r="1202" spans="1:2">
-      <c r="A1202"/>
-      <c r="B1202"/>
-    </row>
-    <row r="1203" spans="1:2">
-      <c r="A1203"/>
-      <c r="B1203"/>
-    </row>
-    <row r="1204" spans="1:2">
-      <c r="A1204"/>
-      <c r="B1204"/>
-    </row>
-    <row r="1205" spans="1:2">
-      <c r="A1205"/>
-      <c r="B1205"/>
-    </row>
-    <row r="1206" spans="1:2">
-      <c r="A1206"/>
-      <c r="B1206"/>
-    </row>
-    <row r="1207" spans="1:2">
-      <c r="A1207"/>
-      <c r="B1207"/>
-    </row>
-    <row r="1208" spans="1:2">
-      <c r="A1208"/>
-      <c r="B1208"/>
-    </row>
-    <row r="1209" spans="1:2">
-      <c r="A1209"/>
-      <c r="B1209"/>
-    </row>
-    <row r="1210" spans="1:2">
-      <c r="A1210"/>
-      <c r="B1210"/>
-    </row>
-    <row r="1211" spans="1:2">
-      <c r="A1211"/>
-      <c r="B1211"/>
-    </row>
-    <row r="1212" spans="1:2">
-      <c r="A1212"/>
-      <c r="B1212"/>
-    </row>
-    <row r="1213" spans="1:2">
-      <c r="A1213"/>
-      <c r="B1213"/>
-    </row>
-    <row r="1214" spans="1:2">
-      <c r="A1214"/>
-      <c r="B1214"/>
-    </row>
-    <row r="1215" spans="1:2">
-      <c r="A1215"/>
-      <c r="B1215"/>
-    </row>
-    <row r="1216" spans="1:2">
-      <c r="A1216"/>
-      <c r="B1216"/>
-    </row>
-    <row r="1217" spans="1:2">
-      <c r="A1217"/>
-      <c r="B1217"/>
-    </row>
-    <row r="1218" spans="1:2">
-      <c r="A1218"/>
-      <c r="B1218"/>
-    </row>
-    <row r="1219" spans="1:2">
-      <c r="A1219"/>
-      <c r="B1219"/>
-    </row>
-    <row r="1220" spans="1:2">
-      <c r="A1220"/>
-      <c r="B1220"/>
-    </row>
-    <row r="1221" spans="1:2">
-      <c r="A1221"/>
-      <c r="B1221"/>
-    </row>
-    <row r="1222" spans="1:2">
-      <c r="A1222"/>
-      <c r="B1222"/>
-    </row>
-    <row r="1223" spans="1:2">
-      <c r="A1223"/>
-      <c r="B1223"/>
-    </row>
-    <row r="1224" spans="1:2">
-      <c r="A1224"/>
-      <c r="B1224"/>
-    </row>
-    <row r="1225" spans="1:2">
-      <c r="A1225"/>
-      <c r="B1225"/>
-    </row>
-    <row r="1226" spans="1:2">
-      <c r="A1226"/>
-      <c r="B1226"/>
-    </row>
-    <row r="1227" spans="1:2">
-      <c r="A1227"/>
-      <c r="B1227"/>
-    </row>
-    <row r="1228" spans="1:2">
-      <c r="A1228"/>
-      <c r="B1228"/>
-    </row>
-    <row r="1229" spans="1:2">
-      <c r="A1229"/>
-      <c r="B1229"/>
-    </row>
-    <row r="1230" spans="1:2">
-      <c r="A1230"/>
-      <c r="B1230"/>
-    </row>
-    <row r="1231" spans="1:2">
-      <c r="A1231"/>
-      <c r="B1231"/>
-    </row>
-    <row r="1232" spans="1:2">
-      <c r="A1232"/>
-      <c r="B1232"/>
-    </row>
-    <row r="1233" spans="1:2">
-      <c r="A1233"/>
-      <c r="B1233"/>
-    </row>
-    <row r="1234" spans="1:2">
-      <c r="A1234"/>
-      <c r="B1234"/>
-    </row>
-    <row r="1235" spans="1:2">
-      <c r="A1235"/>
-      <c r="B1235"/>
-    </row>
-    <row r="1236" spans="1:2">
-      <c r="A1236"/>
-      <c r="B1236"/>
-    </row>
-    <row r="1237" spans="1:2">
-      <c r="A1237"/>
-      <c r="B1237"/>
-    </row>
-    <row r="1238" spans="1:2">
-      <c r="A1238"/>
-      <c r="B1238"/>
-    </row>
-    <row r="1239" spans="1:2">
-      <c r="A1239"/>
-      <c r="B1239"/>
-    </row>
-    <row r="1240" spans="1:2">
-      <c r="A1240"/>
-      <c r="B1240"/>
-    </row>
-    <row r="1241" spans="1:2">
-      <c r="A1241"/>
-      <c r="B1241"/>
-    </row>
-    <row r="1242" spans="1:2">
-      <c r="A1242"/>
-      <c r="B1242"/>
-    </row>
-    <row r="1243" spans="1:2">
-      <c r="A1243"/>
-      <c r="B1243"/>
-    </row>
-    <row r="1244" spans="1:2">
-      <c r="A1244"/>
-      <c r="B1244"/>
-    </row>
-    <row r="1245" spans="1:2">
-      <c r="A1245"/>
-      <c r="B1245"/>
-    </row>
-    <row r="1246" spans="1:2">
-      <c r="A1246"/>
-      <c r="B1246"/>
-    </row>
-    <row r="1247" spans="1:2">
-      <c r="A1247"/>
-      <c r="B1247"/>
-    </row>
-    <row r="1248" spans="1:2">
-      <c r="A1248"/>
-      <c r="B1248"/>
-    </row>
-    <row r="1249" spans="1:2">
-      <c r="A1249"/>
-      <c r="B1249"/>
-    </row>
-    <row r="1250" spans="1:2">
-      <c r="A1250"/>
-      <c r="B1250"/>
-    </row>
-    <row r="1251" spans="1:2">
-      <c r="A1251"/>
-      <c r="B1251"/>
-    </row>
-    <row r="1252" spans="1:2">
-      <c r="A1252"/>
-      <c r="B1252"/>
-    </row>
-    <row r="1253" spans="1:2">
-      <c r="A1253"/>
-      <c r="B1253"/>
-    </row>
-    <row r="1254" spans="1:2">
-      <c r="A1254"/>
-      <c r="B1254"/>
-    </row>
-    <row r="1255" spans="1:2">
-      <c r="A1255"/>
-      <c r="B1255"/>
-    </row>
-    <row r="1256" spans="1:2">
-      <c r="A1256"/>
-      <c r="B1256"/>
-    </row>
-    <row r="1257" spans="1:2">
-      <c r="A1257"/>
-      <c r="B1257"/>
-    </row>
-    <row r="1258" spans="1:2">
-      <c r="A1258"/>
-      <c r="B1258"/>
-    </row>
-    <row r="1259" spans="1:2">
-      <c r="A1259"/>
-      <c r="B1259"/>
-    </row>
-    <row r="1260" spans="1:2">
-      <c r="A1260"/>
-      <c r="B1260"/>
-    </row>
-    <row r="1261" spans="1:2">
-      <c r="A1261"/>
-      <c r="B1261"/>
-    </row>
-    <row r="1262" spans="1:2">
-      <c r="A1262"/>
-      <c r="B1262"/>
-    </row>
-    <row r="1263" spans="1:2">
-      <c r="A1263"/>
-      <c r="B1263"/>
-    </row>
-    <row r="1264" spans="1:2">
-      <c r="A1264"/>
-      <c r="B1264"/>
-    </row>
-    <row r="1265" spans="1:2">
-      <c r="A1265"/>
-      <c r="B1265"/>
-    </row>
-    <row r="1266" spans="1:2">
-      <c r="A1266"/>
-      <c r="B1266"/>
-    </row>
-    <row r="1267" spans="1:2">
-      <c r="A1267"/>
-      <c r="B1267"/>
-    </row>
-    <row r="1268" spans="1:2">
-      <c r="A1268"/>
-      <c r="B1268"/>
-    </row>
-    <row r="1269" spans="1:2">
-      <c r="A1269"/>
-      <c r="B1269"/>
-    </row>
-    <row r="1270" spans="1:2">
-      <c r="A1270"/>
-      <c r="B1270"/>
-    </row>
-    <row r="1271" spans="1:2">
-      <c r="A1271"/>
-      <c r="B1271"/>
-    </row>
-    <row r="1272" spans="1:2">
-      <c r="A1272"/>
-      <c r="B1272"/>
-    </row>
-    <row r="1273" spans="1:2">
-      <c r="A1273"/>
-      <c r="B1273"/>
-    </row>
-    <row r="1274" spans="1:2">
-      <c r="A1274"/>
-      <c r="B1274"/>
-    </row>
-    <row r="1275" spans="1:2">
-      <c r="A1275"/>
-      <c r="B1275"/>
-    </row>
-    <row r="1276" spans="1:2">
-      <c r="A1276"/>
-      <c r="B1276"/>
-    </row>
-    <row r="1277" spans="1:2">
-      <c r="A1277"/>
-      <c r="B1277"/>
-    </row>
-    <row r="1278" spans="1:2">
-      <c r="A1278"/>
-      <c r="B1278"/>
-    </row>
-    <row r="1279" spans="1:2">
-      <c r="A1279"/>
-      <c r="B1279"/>
-    </row>
-    <row r="1280" spans="1:2">
-      <c r="A1280"/>
-      <c r="B1280"/>
-    </row>
-    <row r="1281" spans="1:2">
-      <c r="A1281"/>
-      <c r="B1281"/>
-    </row>
-    <row r="1282" spans="1:2">
-      <c r="A1282"/>
-      <c r="B1282"/>
-    </row>
-    <row r="1283" spans="1:2">
-      <c r="A1283"/>
-      <c r="B1283"/>
-    </row>
-    <row r="1284" spans="1:2">
-      <c r="A1284"/>
-      <c r="B1284"/>
-    </row>
-    <row r="1285" spans="1:2">
-      <c r="A1285"/>
-      <c r="B1285"/>
-    </row>
-    <row r="1286" spans="1:2">
-      <c r="A1286"/>
-      <c r="B1286"/>
-    </row>
-    <row r="1287" spans="1:2">
-      <c r="A1287"/>
-      <c r="B1287"/>
-    </row>
-    <row r="1288" spans="1:2">
-      <c r="A1288"/>
-      <c r="B1288"/>
-    </row>
-    <row r="1289" spans="1:2">
-      <c r="A1289"/>
-      <c r="B1289"/>
-    </row>
-    <row r="1290" spans="1:2">
-      <c r="A1290"/>
-      <c r="B1290"/>
-    </row>
-    <row r="1291" spans="1:2">
-      <c r="A1291"/>
-      <c r="B1291"/>
-    </row>
-    <row r="1292" spans="1:2">
-      <c r="A1292"/>
-      <c r="B1292"/>
-    </row>
-    <row r="1293" spans="1:2">
-      <c r="A1293"/>
-      <c r="B1293"/>
-    </row>
-    <row r="1294" spans="1:2">
-      <c r="A1294"/>
-      <c r="B1294"/>
-    </row>
-    <row r="1295" spans="1:2">
-      <c r="A1295"/>
-      <c r="B1295"/>
-    </row>
-    <row r="1296" spans="1:2">
-      <c r="A1296"/>
-      <c r="B1296"/>
-    </row>
-    <row r="1297" spans="1:2">
-      <c r="A1297"/>
-      <c r="B1297"/>
-    </row>
-    <row r="1298" spans="1:2">
-      <c r="A1298"/>
-      <c r="B1298"/>
-    </row>
-    <row r="1299" spans="1:2">
-      <c r="A1299"/>
-      <c r="B1299"/>
-    </row>
-    <row r="1300" spans="1:2">
-      <c r="A1300"/>
-      <c r="B1300"/>
-    </row>
-    <row r="1301" spans="1:2">
-      <c r="A1301"/>
-      <c r="B1301"/>
-    </row>
-    <row r="1302" spans="1:2">
-      <c r="A1302"/>
-      <c r="B1302"/>
-    </row>
-    <row r="1303" spans="1:2">
-      <c r="A1303"/>
-      <c r="B1303"/>
-    </row>
-    <row r="1304" spans="1:2">
-      <c r="A1304"/>
-      <c r="B1304"/>
-    </row>
-    <row r="1305" spans="1:2">
-      <c r="A1305"/>
-      <c r="B1305"/>
-    </row>
-    <row r="1306" spans="1:2">
-      <c r="A1306"/>
-      <c r="B1306"/>
-    </row>
-    <row r="1307" spans="1:2">
-      <c r="A1307"/>
-      <c r="B1307"/>
-    </row>
-    <row r="1308" spans="1:2">
-      <c r="A1308"/>
-      <c r="B1308"/>
-    </row>
-    <row r="1309" spans="1:2">
-      <c r="A1309"/>
-      <c r="B1309"/>
-    </row>
-    <row r="1310" spans="1:2">
-      <c r="A1310"/>
-      <c r="B1310"/>
-    </row>
-    <row r="1311" spans="1:2">
-      <c r="A1311"/>
-      <c r="B1311"/>
-    </row>
-    <row r="1312" spans="1:2">
-      <c r="A1312"/>
-      <c r="B1312"/>
-    </row>
-    <row r="1313" spans="1:2">
-      <c r="A1313"/>
-      <c r="B1313"/>
-    </row>
-    <row r="1314" spans="1:2">
-      <c r="A1314"/>
-      <c r="B1314"/>
-    </row>
-    <row r="1315" spans="1:2">
-      <c r="A1315"/>
-      <c r="B1315"/>
-    </row>
-    <row r="1316" spans="1:2">
-      <c r="A1316"/>
-      <c r="B1316"/>
-    </row>
-    <row r="1317" spans="1:2">
-      <c r="A1317"/>
-      <c r="B1317"/>
-    </row>
-    <row r="1318" spans="1:2">
-      <c r="A1318"/>
-      <c r="B1318"/>
-    </row>
-    <row r="1319" spans="1:2">
-      <c r="A1319"/>
-      <c r="B1319"/>
-    </row>
-    <row r="1320" spans="1:2">
-      <c r="A1320"/>
-      <c r="B1320"/>
-    </row>
-    <row r="1321" spans="1:2">
-      <c r="A1321"/>
-      <c r="B1321"/>
-    </row>
-    <row r="1322" spans="1:2">
-      <c r="A1322"/>
-      <c r="B1322"/>
-    </row>
-    <row r="1323" spans="1:2">
-      <c r="A1323"/>
-      <c r="B1323"/>
-    </row>
-    <row r="1324" spans="1:2">
-      <c r="A1324"/>
-      <c r="B1324"/>
-    </row>
-    <row r="1325" spans="1:2">
-      <c r="A1325"/>
-      <c r="B1325"/>
-    </row>
-    <row r="1326" spans="1:2">
-      <c r="A1326"/>
-      <c r="B1326"/>
-    </row>
-    <row r="1327" spans="1:2">
-      <c r="A1327"/>
-      <c r="B1327"/>
-    </row>
-    <row r="1328" spans="1:2">
-      <c r="A1328"/>
-      <c r="B1328"/>
-    </row>
-    <row r="1329" spans="1:2">
-      <c r="A1329"/>
-      <c r="B1329"/>
-    </row>
-    <row r="1330" spans="1:2">
-      <c r="A1330"/>
-      <c r="B1330"/>
-    </row>
-    <row r="1331" spans="1:2">
-      <c r="A1331"/>
-      <c r="B1331"/>
-    </row>
-    <row r="1332" spans="1:2">
-      <c r="A1332"/>
-      <c r="B1332"/>
-    </row>
-    <row r="1333" spans="1:2">
-      <c r="A1333"/>
-      <c r="B1333"/>
-    </row>
-    <row r="1334" spans="1:2">
-      <c r="A1334"/>
-      <c r="B1334"/>
-    </row>
-    <row r="1335" spans="1:2">
-      <c r="A1335"/>
-      <c r="B1335"/>
-    </row>
-    <row r="1336" spans="1:2">
-      <c r="A1336"/>
-      <c r="B1336"/>
-    </row>
-    <row r="1337" spans="1:2">
-      <c r="A1337"/>
-      <c r="B1337"/>
-    </row>
-    <row r="1338" spans="1:2">
-      <c r="A1338"/>
-      <c r="B1338"/>
-    </row>
-    <row r="1339" spans="1:2">
-      <c r="A1339"/>
-      <c r="B1339"/>
-    </row>
-    <row r="1340" spans="1:2">
-      <c r="A1340"/>
-      <c r="B1340"/>
-    </row>
-    <row r="1341" spans="1:2">
-      <c r="A1341"/>
-      <c r="B1341"/>
-    </row>
-    <row r="1342" spans="1:2">
-      <c r="A1342"/>
-      <c r="B1342"/>
-    </row>
-    <row r="1343" spans="1:2">
-      <c r="A1343"/>
-      <c r="B1343"/>
-    </row>
-    <row r="1344" spans="1:2">
-      <c r="A1344"/>
-      <c r="B1344"/>
-    </row>
-    <row r="1345" spans="1:2">
-      <c r="A1345"/>
-      <c r="B1345"/>
-    </row>
-    <row r="1346" spans="1:2">
-      <c r="A1346"/>
-      <c r="B1346"/>
-    </row>
-    <row r="1347" spans="1:2">
-      <c r="A1347"/>
-      <c r="B1347"/>
-    </row>
-    <row r="1348" spans="1:2">
-      <c r="A1348"/>
-      <c r="B1348"/>
-    </row>
-    <row r="1349" spans="1:2">
-      <c r="A1349"/>
-      <c r="B1349"/>
-    </row>
-    <row r="1350" spans="1:2">
-      <c r="A1350"/>
-      <c r="B1350"/>
-    </row>
-    <row r="1351" spans="1:2">
-      <c r="A1351"/>
-      <c r="B1351"/>
-    </row>
-    <row r="1352" spans="1:2">
-      <c r="A1352"/>
-      <c r="B1352"/>
-    </row>
-    <row r="1353" spans="1:2">
-      <c r="A1353"/>
-      <c r="B1353"/>
-    </row>
-    <row r="1354" spans="1:2">
-      <c r="A1354"/>
-      <c r="B1354"/>
-    </row>
-    <row r="1355" spans="1:2">
-      <c r="A1355"/>
-      <c r="B1355"/>
-    </row>
-    <row r="1356" spans="1:2">
-      <c r="A1356"/>
-      <c r="B1356"/>
-    </row>
-    <row r="1357" spans="1:2">
-      <c r="A1357"/>
-      <c r="B1357"/>
-    </row>
-    <row r="1358" spans="1:2">
-      <c r="A1358"/>
-      <c r="B1358"/>
-    </row>
-    <row r="1359" spans="1:2">
-      <c r="A1359"/>
-      <c r="B1359"/>
-    </row>
-    <row r="1360" spans="1:2">
-      <c r="A1360"/>
-      <c r="B1360"/>
-    </row>
-    <row r="1361" spans="1:2">
-      <c r="A1361"/>
-      <c r="B1361"/>
-    </row>
-    <row r="1362" spans="1:2">
-      <c r="A1362"/>
-      <c r="B1362"/>
-    </row>
-    <row r="1363" spans="1:2">
-      <c r="A1363"/>
-      <c r="B1363"/>
-    </row>
-    <row r="1364" spans="1:2">
-      <c r="A1364"/>
-      <c r="B1364"/>
-    </row>
-    <row r="1365" spans="1:2">
-      <c r="A1365"/>
-      <c r="B1365"/>
-    </row>
-    <row r="1366" spans="1:2">
-      <c r="A1366"/>
-      <c r="B1366"/>
-    </row>
-    <row r="1367" spans="1:2">
-      <c r="A1367"/>
-      <c r="B1367"/>
-    </row>
-    <row r="1368" spans="1:2">
-      <c r="A1368"/>
-      <c r="B1368"/>
-    </row>
-    <row r="1369" spans="1:2">
-      <c r="A1369"/>
-      <c r="B1369"/>
-    </row>
-    <row r="1370" spans="1:2">
-      <c r="A1370"/>
-      <c r="B1370"/>
-    </row>
-    <row r="1371" spans="1:2">
-      <c r="A1371"/>
-      <c r="B1371"/>
-    </row>
-    <row r="1372" spans="1:2">
-      <c r="A1372"/>
-      <c r="B1372"/>
-    </row>
-    <row r="1373" spans="1:2">
-      <c r="A1373"/>
-      <c r="B1373"/>
-    </row>
-    <row r="1374" spans="1:2">
-      <c r="A1374"/>
-      <c r="B1374"/>
-    </row>
-    <row r="1375" spans="1:2">
-      <c r="A1375"/>
-      <c r="B1375"/>
-    </row>
-    <row r="1376" spans="1:2">
-      <c r="A1376"/>
-      <c r="B1376"/>
-    </row>
-    <row r="1377" spans="1:2">
-      <c r="A1377"/>
-      <c r="B1377"/>
-    </row>
-    <row r="1378" spans="1:2">
-      <c r="A1378"/>
-      <c r="B1378"/>
-    </row>
-    <row r="1379" spans="1:2">
-      <c r="A1379"/>
-      <c r="B1379"/>
-    </row>
-    <row r="1380" spans="1:2">
-      <c r="A1380"/>
-      <c r="B1380"/>
-    </row>
-    <row r="1381" spans="1:2">
-      <c r="A1381"/>
-      <c r="B1381"/>
-    </row>
-    <row r="1382" spans="1:2">
-      <c r="A1382"/>
-      <c r="B1382"/>
-    </row>
-    <row r="1383" spans="1:2">
-      <c r="A1383"/>
-      <c r="B1383"/>
-    </row>
-    <row r="1384" spans="1:2">
-      <c r="A1384"/>
-      <c r="B1384"/>
-    </row>
-    <row r="1385" spans="1:2">
-      <c r="A1385"/>
-      <c r="B1385"/>
-    </row>
-    <row r="1386" spans="1:2">
-      <c r="A1386"/>
-      <c r="B1386"/>
-    </row>
+    <row r="1041" customFormat="1"/>
+    <row r="1042" customFormat="1"/>
+    <row r="1043" customFormat="1"/>
+    <row r="1044" customFormat="1"/>
+    <row r="1045" customFormat="1"/>
+    <row r="1046" customFormat="1"/>
+    <row r="1047" customFormat="1"/>
+    <row r="1048" customFormat="1"/>
+    <row r="1049" customFormat="1"/>
+    <row r="1050" customFormat="1"/>
+    <row r="1051" customFormat="1"/>
+    <row r="1052" customFormat="1"/>
+    <row r="1053" customFormat="1"/>
+    <row r="1054" customFormat="1"/>
+    <row r="1055" customFormat="1"/>
+    <row r="1056" customFormat="1"/>
+    <row r="1057" customFormat="1"/>
+    <row r="1058" customFormat="1"/>
+    <row r="1059" customFormat="1"/>
+    <row r="1060" customFormat="1"/>
+    <row r="1061" customFormat="1"/>
+    <row r="1062" customFormat="1"/>
+    <row r="1063" customFormat="1"/>
+    <row r="1064" customFormat="1"/>
+    <row r="1065" customFormat="1"/>
+    <row r="1066" customFormat="1"/>
+    <row r="1067" customFormat="1"/>
+    <row r="1068" customFormat="1"/>
+    <row r="1069" customFormat="1"/>
+    <row r="1070" customFormat="1"/>
+    <row r="1071" customFormat="1"/>
+    <row r="1072" customFormat="1"/>
+    <row r="1073" customFormat="1"/>
+    <row r="1074" customFormat="1"/>
+    <row r="1075" customFormat="1"/>
+    <row r="1076" customFormat="1"/>
+    <row r="1077" customFormat="1"/>
+    <row r="1078" customFormat="1"/>
+    <row r="1079" customFormat="1"/>
+    <row r="1080" customFormat="1"/>
+    <row r="1081" customFormat="1"/>
+    <row r="1082" customFormat="1"/>
+    <row r="1083" customFormat="1"/>
+    <row r="1084" customFormat="1"/>
+    <row r="1085" customFormat="1"/>
+    <row r="1086" customFormat="1"/>
+    <row r="1087" customFormat="1"/>
+    <row r="1088" customFormat="1"/>
+    <row r="1089" customFormat="1"/>
+    <row r="1090" customFormat="1"/>
+    <row r="1091" customFormat="1"/>
+    <row r="1092" customFormat="1"/>
+    <row r="1093" customFormat="1"/>
+    <row r="1094" customFormat="1"/>
+    <row r="1095" customFormat="1"/>
+    <row r="1096" customFormat="1"/>
+    <row r="1097" customFormat="1"/>
+    <row r="1098" customFormat="1"/>
+    <row r="1099" customFormat="1"/>
+    <row r="1100" customFormat="1"/>
+    <row r="1101" customFormat="1"/>
+    <row r="1102" customFormat="1"/>
+    <row r="1103" customFormat="1"/>
+    <row r="1104" customFormat="1"/>
+    <row r="1105" customFormat="1"/>
+    <row r="1106" customFormat="1"/>
+    <row r="1107" customFormat="1"/>
+    <row r="1108" customFormat="1"/>
+    <row r="1109" customFormat="1"/>
+    <row r="1110" customFormat="1"/>
+    <row r="1111" customFormat="1"/>
+    <row r="1112" customFormat="1"/>
+    <row r="1113" customFormat="1"/>
+    <row r="1114" customFormat="1"/>
+    <row r="1115" customFormat="1"/>
+    <row r="1116" customFormat="1"/>
+    <row r="1117" customFormat="1"/>
+    <row r="1118" customFormat="1"/>
+    <row r="1119" customFormat="1"/>
+    <row r="1120" customFormat="1"/>
+    <row r="1121" customFormat="1"/>
+    <row r="1122" customFormat="1"/>
+    <row r="1123" customFormat="1"/>
+    <row r="1124" customFormat="1"/>
+    <row r="1125" customFormat="1"/>
+    <row r="1126" customFormat="1"/>
+    <row r="1127" customFormat="1"/>
+    <row r="1128" customFormat="1"/>
+    <row r="1129" customFormat="1"/>
+    <row r="1130" customFormat="1"/>
+    <row r="1131" customFormat="1"/>
+    <row r="1132" customFormat="1"/>
+    <row r="1133" customFormat="1"/>
+    <row r="1134" customFormat="1"/>
+    <row r="1135" customFormat="1"/>
+    <row r="1136" customFormat="1"/>
+    <row r="1137" customFormat="1"/>
+    <row r="1138" customFormat="1"/>
+    <row r="1139" customFormat="1"/>
+    <row r="1140" customFormat="1"/>
+    <row r="1141" customFormat="1"/>
+    <row r="1142" customFormat="1"/>
+    <row r="1143" customFormat="1"/>
+    <row r="1144" customFormat="1"/>
+    <row r="1145" customFormat="1"/>
+    <row r="1146" customFormat="1"/>
+    <row r="1147" customFormat="1"/>
+    <row r="1148" customFormat="1"/>
+    <row r="1149" customFormat="1"/>
+    <row r="1150" customFormat="1"/>
+    <row r="1151" customFormat="1"/>
+    <row r="1152" customFormat="1"/>
+    <row r="1153" customFormat="1"/>
+    <row r="1154" customFormat="1"/>
+    <row r="1155" customFormat="1"/>
+    <row r="1156" customFormat="1"/>
+    <row r="1157" customFormat="1"/>
+    <row r="1158" customFormat="1"/>
+    <row r="1159" customFormat="1"/>
+    <row r="1160" customFormat="1"/>
+    <row r="1161" customFormat="1"/>
+    <row r="1162" customFormat="1"/>
+    <row r="1163" customFormat="1"/>
+    <row r="1164" customFormat="1"/>
+    <row r="1165" customFormat="1"/>
+    <row r="1166" customFormat="1"/>
+    <row r="1167" customFormat="1"/>
+    <row r="1168" customFormat="1"/>
+    <row r="1169" customFormat="1"/>
+    <row r="1170" customFormat="1"/>
+    <row r="1171" customFormat="1"/>
+    <row r="1172" customFormat="1"/>
+    <row r="1173" customFormat="1"/>
+    <row r="1174" customFormat="1"/>
+    <row r="1175" customFormat="1"/>
+    <row r="1176" customFormat="1"/>
+    <row r="1177" customFormat="1"/>
+    <row r="1178" customFormat="1"/>
+    <row r="1179" customFormat="1"/>
+    <row r="1180" customFormat="1"/>
+    <row r="1181" customFormat="1"/>
+    <row r="1182" customFormat="1"/>
+    <row r="1183" customFormat="1"/>
+    <row r="1184" customFormat="1"/>
+    <row r="1185" customFormat="1"/>
+    <row r="1186" customFormat="1"/>
+    <row r="1187" customFormat="1"/>
+    <row r="1188" customFormat="1"/>
+    <row r="1189" customFormat="1"/>
+    <row r="1190" customFormat="1"/>
+    <row r="1191" customFormat="1"/>
+    <row r="1192" customFormat="1"/>
+    <row r="1193" customFormat="1"/>
+    <row r="1194" customFormat="1"/>
+    <row r="1195" customFormat="1"/>
+    <row r="1196" customFormat="1"/>
+    <row r="1197" customFormat="1"/>
+    <row r="1198" customFormat="1"/>
+    <row r="1199" customFormat="1"/>
+    <row r="1200" customFormat="1"/>
+    <row r="1201" customFormat="1"/>
+    <row r="1202" customFormat="1"/>
+    <row r="1203" customFormat="1"/>
+    <row r="1204" customFormat="1"/>
+    <row r="1205" customFormat="1"/>
+    <row r="1206" customFormat="1"/>
+    <row r="1207" customFormat="1"/>
+    <row r="1208" customFormat="1"/>
+    <row r="1209" customFormat="1"/>
+    <row r="1210" customFormat="1"/>
+    <row r="1211" customFormat="1"/>
+    <row r="1212" customFormat="1"/>
+    <row r="1213" customFormat="1"/>
+    <row r="1214" customFormat="1"/>
+    <row r="1215" customFormat="1"/>
+    <row r="1216" customFormat="1"/>
+    <row r="1217" customFormat="1"/>
+    <row r="1218" customFormat="1"/>
+    <row r="1219" customFormat="1"/>
+    <row r="1220" customFormat="1"/>
+    <row r="1221" customFormat="1"/>
+    <row r="1222" customFormat="1"/>
+    <row r="1223" customFormat="1"/>
+    <row r="1224" customFormat="1"/>
+    <row r="1225" customFormat="1"/>
+    <row r="1226" customFormat="1"/>
+    <row r="1227" customFormat="1"/>
+    <row r="1228" customFormat="1"/>
+    <row r="1229" customFormat="1"/>
+    <row r="1230" customFormat="1"/>
+    <row r="1231" customFormat="1"/>
+    <row r="1232" customFormat="1"/>
+    <row r="1233" customFormat="1"/>
+    <row r="1234" customFormat="1"/>
+    <row r="1235" customFormat="1"/>
+    <row r="1236" customFormat="1"/>
+    <row r="1237" customFormat="1"/>
+    <row r="1238" customFormat="1"/>
+    <row r="1239" customFormat="1"/>
+    <row r="1240" customFormat="1"/>
+    <row r="1241" customFormat="1"/>
+    <row r="1242" customFormat="1"/>
+    <row r="1243" customFormat="1"/>
+    <row r="1244" customFormat="1"/>
+    <row r="1245" customFormat="1"/>
+    <row r="1246" customFormat="1"/>
+    <row r="1247" customFormat="1"/>
+    <row r="1248" customFormat="1"/>
+    <row r="1249" customFormat="1"/>
+    <row r="1250" customFormat="1"/>
+    <row r="1251" customFormat="1"/>
+    <row r="1252" customFormat="1"/>
+    <row r="1253" customFormat="1"/>
+    <row r="1254" customFormat="1"/>
+    <row r="1255" customFormat="1"/>
+    <row r="1256" customFormat="1"/>
+    <row r="1257" customFormat="1"/>
+    <row r="1258" customFormat="1"/>
+    <row r="1259" customFormat="1"/>
+    <row r="1260" customFormat="1"/>
+    <row r="1261" customFormat="1"/>
+    <row r="1262" customFormat="1"/>
+    <row r="1263" customFormat="1"/>
+    <row r="1264" customFormat="1"/>
+    <row r="1265" customFormat="1"/>
+    <row r="1266" customFormat="1"/>
+    <row r="1267" customFormat="1"/>
+    <row r="1268" customFormat="1"/>
+    <row r="1269" customFormat="1"/>
+    <row r="1270" customFormat="1"/>
+    <row r="1271" customFormat="1"/>
+    <row r="1272" customFormat="1"/>
+    <row r="1273" customFormat="1"/>
+    <row r="1274" customFormat="1"/>
+    <row r="1275" customFormat="1"/>
+    <row r="1276" customFormat="1"/>
+    <row r="1277" customFormat="1"/>
+    <row r="1278" customFormat="1"/>
+    <row r="1279" customFormat="1"/>
+    <row r="1280" customFormat="1"/>
+    <row r="1281" customFormat="1"/>
+    <row r="1282" customFormat="1"/>
+    <row r="1283" customFormat="1"/>
+    <row r="1284" customFormat="1"/>
+    <row r="1285" customFormat="1"/>
+    <row r="1286" customFormat="1"/>
+    <row r="1287" customFormat="1"/>
+    <row r="1288" customFormat="1"/>
+    <row r="1289" customFormat="1"/>
+    <row r="1290" customFormat="1"/>
+    <row r="1291" customFormat="1"/>
+    <row r="1292" customFormat="1"/>
+    <row r="1293" customFormat="1"/>
+    <row r="1294" customFormat="1"/>
+    <row r="1295" customFormat="1"/>
+    <row r="1296" customFormat="1"/>
+    <row r="1297" customFormat="1"/>
+    <row r="1298" customFormat="1"/>
+    <row r="1299" customFormat="1"/>
+    <row r="1300" customFormat="1"/>
+    <row r="1301" customFormat="1"/>
+    <row r="1302" customFormat="1"/>
+    <row r="1303" customFormat="1"/>
+    <row r="1304" customFormat="1"/>
+    <row r="1305" customFormat="1"/>
+    <row r="1306" customFormat="1"/>
+    <row r="1307" customFormat="1"/>
+    <row r="1308" customFormat="1"/>
+    <row r="1309" customFormat="1"/>
+    <row r="1310" customFormat="1"/>
+    <row r="1311" customFormat="1"/>
+    <row r="1312" customFormat="1"/>
+    <row r="1313" customFormat="1"/>
+    <row r="1314" customFormat="1"/>
+    <row r="1315" customFormat="1"/>
+    <row r="1316" customFormat="1"/>
+    <row r="1317" customFormat="1"/>
+    <row r="1318" customFormat="1"/>
+    <row r="1319" customFormat="1"/>
+    <row r="1320" customFormat="1"/>
+    <row r="1321" customFormat="1"/>
+    <row r="1322" customFormat="1"/>
+    <row r="1323" customFormat="1"/>
+    <row r="1324" customFormat="1"/>
+    <row r="1325" customFormat="1"/>
+    <row r="1326" customFormat="1"/>
+    <row r="1327" customFormat="1"/>
+    <row r="1328" customFormat="1"/>
+    <row r="1329" customFormat="1"/>
+    <row r="1330" customFormat="1"/>
+    <row r="1331" customFormat="1"/>
+    <row r="1332" customFormat="1"/>
+    <row r="1333" customFormat="1"/>
+    <row r="1334" customFormat="1"/>
+    <row r="1335" customFormat="1"/>
+    <row r="1336" customFormat="1"/>
+    <row r="1337" customFormat="1"/>
+    <row r="1338" customFormat="1"/>
+    <row r="1339" customFormat="1"/>
+    <row r="1340" customFormat="1"/>
+    <row r="1341" customFormat="1"/>
+    <row r="1342" customFormat="1"/>
+    <row r="1343" customFormat="1"/>
+    <row r="1344" customFormat="1"/>
+    <row r="1345" customFormat="1"/>
+    <row r="1346" customFormat="1"/>
+    <row r="1347" customFormat="1"/>
+    <row r="1348" customFormat="1"/>
+    <row r="1349" customFormat="1"/>
+    <row r="1350" customFormat="1"/>
+    <row r="1351" customFormat="1"/>
+    <row r="1352" customFormat="1"/>
+    <row r="1353" customFormat="1"/>
+    <row r="1354" customFormat="1"/>
+    <row r="1355" customFormat="1"/>
+    <row r="1356" customFormat="1"/>
+    <row r="1357" customFormat="1"/>
+    <row r="1358" customFormat="1"/>
+    <row r="1359" customFormat="1"/>
+    <row r="1360" customFormat="1"/>
+    <row r="1361" customFormat="1"/>
+    <row r="1362" customFormat="1"/>
+    <row r="1363" customFormat="1"/>
+    <row r="1364" customFormat="1"/>
+    <row r="1365" customFormat="1"/>
+    <row r="1366" customFormat="1"/>
+    <row r="1367" customFormat="1"/>
+    <row r="1368" customFormat="1"/>
+    <row r="1369" customFormat="1"/>
+    <row r="1370" customFormat="1"/>
+    <row r="1371" customFormat="1"/>
+    <row r="1372" customFormat="1"/>
+    <row r="1373" customFormat="1"/>
+    <row r="1374" customFormat="1"/>
+    <row r="1375" customFormat="1"/>
+    <row r="1376" customFormat="1"/>
+    <row r="1377" customFormat="1"/>
+    <row r="1378" customFormat="1"/>
+    <row r="1379" customFormat="1"/>
+    <row r="1380" customFormat="1"/>
+    <row r="1381" customFormat="1"/>
+    <row r="1382" customFormat="1"/>
+    <row r="1383" customFormat="1"/>
+    <row r="1384" customFormat="1"/>
+    <row r="1385" customFormat="1"/>
+    <row r="1386" customFormat="1"/>
+    <row r="1387" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: add supplier in the file
</commit_message>
<xml_diff>
--- a/public/6. COA.xlsx
+++ b/public/6. COA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WB\Project\invoice-management-frontend\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patience.uwase\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58089D24-4DDC-47DA-BB87-A4A6F1F6EC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier Details" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Route!$A$4:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4490" uniqueCount="4453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4492" uniqueCount="4455">
   <si>
     <t>ACCESS BANK -USD</t>
   </si>
@@ -13399,16 +13400,22 @@
     <t>Photo Copiers and Fax Equipment rentals</t>
   </si>
   <si>
+    <t>ATTACHED GLOBAL COMMUNICATION</t>
+  </si>
+  <si>
     <t>S0204</t>
   </si>
   <si>
-    <t xml:space="preserve">ATTACHED GLOBAL COMMUNICATION </t>
+    <t>S0053</t>
+  </si>
+  <si>
+    <t>SOCOMAT S.A.R.L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17">
     <font>
       <sz val="11"/>
@@ -13783,8 +13790,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -14106,14 +14113,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B1565"/>
+  <dimension ref="A1:B1566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1424" workbookViewId="0">
-      <selection activeCell="B1459" sqref="B1459"/>
+    <sheetView tabSelected="1" topLeftCell="A1108" workbookViewId="0">
+      <selection activeCell="B1366" sqref="B1366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -25028,1617 +25035,1625 @@
     </row>
     <row r="1364" spans="1:2">
       <c r="A1364" s="1" t="s">
-        <v>4017</v>
+        <v>4453</v>
       </c>
       <c r="B1364" t="s">
-        <v>4018</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="1365" spans="1:2">
       <c r="A1365" s="1" t="s">
-        <v>4019</v>
+        <v>4017</v>
       </c>
       <c r="B1365" t="s">
-        <v>4020</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="1366" spans="1:2">
       <c r="A1366" s="1" t="s">
-        <v>4021</v>
+        <v>4019</v>
       </c>
       <c r="B1366" t="s">
-        <v>4022</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1367" spans="1:2">
       <c r="A1367" s="1" t="s">
-        <v>4023</v>
+        <v>4021</v>
       </c>
       <c r="B1367" t="s">
-        <v>4024</v>
+        <v>4022</v>
       </c>
     </row>
     <row r="1368" spans="1:2">
       <c r="A1368" s="1" t="s">
-        <v>4025</v>
+        <v>4023</v>
       </c>
       <c r="B1368" t="s">
-        <v>4026</v>
+        <v>4024</v>
       </c>
     </row>
     <row r="1369" spans="1:2">
       <c r="A1369" s="1" t="s">
-        <v>4027</v>
+        <v>4025</v>
       </c>
       <c r="B1369" t="s">
-        <v>4028</v>
+        <v>4026</v>
       </c>
     </row>
     <row r="1370" spans="1:2">
       <c r="A1370" s="1" t="s">
-        <v>4029</v>
+        <v>4027</v>
       </c>
       <c r="B1370" t="s">
-        <v>4030</v>
+        <v>4028</v>
       </c>
     </row>
     <row r="1371" spans="1:2">
       <c r="A1371" s="1" t="s">
-        <v>4031</v>
+        <v>4029</v>
       </c>
       <c r="B1371" t="s">
-        <v>4032</v>
+        <v>4030</v>
       </c>
     </row>
     <row r="1372" spans="1:2">
       <c r="A1372" s="1" t="s">
-        <v>4033</v>
+        <v>4031</v>
       </c>
       <c r="B1372" t="s">
-        <v>4034</v>
+        <v>4032</v>
       </c>
     </row>
     <row r="1373" spans="1:2">
       <c r="A1373" s="1" t="s">
-        <v>4035</v>
+        <v>4033</v>
       </c>
       <c r="B1373" t="s">
-        <v>4036</v>
+        <v>4034</v>
       </c>
     </row>
     <row r="1374" spans="1:2">
       <c r="A1374" s="1" t="s">
-        <v>4037</v>
+        <v>4035</v>
       </c>
       <c r="B1374" t="s">
-        <v>4038</v>
+        <v>4036</v>
       </c>
     </row>
     <row r="1375" spans="1:2">
       <c r="A1375" s="1" t="s">
-        <v>4039</v>
+        <v>4037</v>
       </c>
       <c r="B1375" t="s">
-        <v>4040</v>
+        <v>4038</v>
       </c>
     </row>
     <row r="1376" spans="1:2">
       <c r="A1376" s="1" t="s">
-        <v>4041</v>
+        <v>4039</v>
       </c>
       <c r="B1376" t="s">
-        <v>4042</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1377" spans="1:2">
       <c r="A1377" s="1" t="s">
-        <v>4043</v>
+        <v>4041</v>
       </c>
       <c r="B1377" t="s">
-        <v>4044</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="1378" spans="1:2">
       <c r="A1378" s="1" t="s">
-        <v>4045</v>
+        <v>4043</v>
       </c>
       <c r="B1378" t="s">
-        <v>4046</v>
+        <v>4044</v>
       </c>
     </row>
     <row r="1379" spans="1:2">
       <c r="A1379" s="1" t="s">
-        <v>4047</v>
+        <v>4045</v>
       </c>
       <c r="B1379" t="s">
-        <v>4048</v>
+        <v>4046</v>
       </c>
     </row>
     <row r="1380" spans="1:2">
       <c r="A1380" s="1" t="s">
-        <v>4049</v>
+        <v>4047</v>
       </c>
       <c r="B1380" t="s">
-        <v>4050</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1381" spans="1:2">
       <c r="A1381" s="1" t="s">
-        <v>4051</v>
+        <v>4049</v>
       </c>
       <c r="B1381" t="s">
-        <v>4052</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="1382" spans="1:2">
       <c r="A1382" s="1" t="s">
-        <v>4053</v>
+        <v>4051</v>
       </c>
       <c r="B1382" t="s">
-        <v>4054</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="1383" spans="1:2">
       <c r="A1383" s="1" t="s">
-        <v>4055</v>
+        <v>4053</v>
       </c>
       <c r="B1383" t="s">
-        <v>4056</v>
+        <v>4054</v>
       </c>
     </row>
     <row r="1384" spans="1:2">
       <c r="A1384" s="1" t="s">
-        <v>4057</v>
+        <v>4055</v>
       </c>
       <c r="B1384" t="s">
-        <v>4058</v>
+        <v>4056</v>
       </c>
     </row>
     <row r="1385" spans="1:2">
       <c r="A1385" s="1" t="s">
-        <v>4059</v>
+        <v>4057</v>
       </c>
       <c r="B1385" t="s">
-        <v>4060</v>
+        <v>4058</v>
       </c>
     </row>
     <row r="1386" spans="1:2">
       <c r="A1386" s="1" t="s">
-        <v>4061</v>
+        <v>4059</v>
       </c>
       <c r="B1386" t="s">
-        <v>4062</v>
+        <v>4060</v>
       </c>
     </row>
     <row r="1387" spans="1:2">
       <c r="A1387" s="1" t="s">
-        <v>4063</v>
+        <v>4061</v>
       </c>
       <c r="B1387" t="s">
-        <v>4064</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="1388" spans="1:2">
       <c r="A1388" s="1" t="s">
-        <v>4065</v>
+        <v>4063</v>
       </c>
       <c r="B1388" t="s">
-        <v>4066</v>
+        <v>4064</v>
       </c>
     </row>
     <row r="1389" spans="1:2">
       <c r="A1389" s="1" t="s">
-        <v>4067</v>
+        <v>4065</v>
       </c>
       <c r="B1389" t="s">
-        <v>4068</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="1390" spans="1:2">
       <c r="A1390" s="1" t="s">
-        <v>4069</v>
+        <v>4067</v>
       </c>
       <c r="B1390" t="s">
-        <v>4070</v>
+        <v>4068</v>
       </c>
     </row>
     <row r="1391" spans="1:2">
       <c r="A1391" s="1" t="s">
-        <v>4071</v>
+        <v>4069</v>
       </c>
       <c r="B1391" t="s">
-        <v>4072</v>
+        <v>4070</v>
       </c>
     </row>
     <row r="1392" spans="1:2">
       <c r="A1392" s="1" t="s">
-        <v>4073</v>
+        <v>4071</v>
       </c>
       <c r="B1392" t="s">
-        <v>4074</v>
+        <v>4072</v>
       </c>
     </row>
     <row r="1393" spans="1:2">
       <c r="A1393" s="1" t="s">
-        <v>4075</v>
+        <v>4073</v>
       </c>
       <c r="B1393" t="s">
-        <v>4076</v>
+        <v>4074</v>
       </c>
     </row>
     <row r="1394" spans="1:2">
       <c r="A1394" s="1" t="s">
-        <v>4077</v>
+        <v>4075</v>
       </c>
       <c r="B1394" t="s">
-        <v>4078</v>
+        <v>4076</v>
       </c>
     </row>
     <row r="1395" spans="1:2">
       <c r="A1395" s="1" t="s">
-        <v>4079</v>
+        <v>4077</v>
       </c>
       <c r="B1395" t="s">
-        <v>4080</v>
+        <v>4078</v>
       </c>
     </row>
     <row r="1396" spans="1:2">
       <c r="A1396" s="1" t="s">
-        <v>4081</v>
+        <v>4079</v>
       </c>
       <c r="B1396" t="s">
-        <v>4082</v>
+        <v>4080</v>
       </c>
     </row>
     <row r="1397" spans="1:2">
       <c r="A1397" s="1" t="s">
-        <v>4083</v>
+        <v>4081</v>
       </c>
       <c r="B1397" t="s">
-        <v>4084</v>
+        <v>4082</v>
       </c>
     </row>
     <row r="1398" spans="1:2">
       <c r="A1398" s="1" t="s">
-        <v>4085</v>
+        <v>4083</v>
       </c>
       <c r="B1398" t="s">
-        <v>4086</v>
+        <v>4084</v>
       </c>
     </row>
     <row r="1399" spans="1:2">
       <c r="A1399" s="1" t="s">
-        <v>4087</v>
+        <v>4085</v>
       </c>
       <c r="B1399" t="s">
-        <v>4088</v>
+        <v>4086</v>
       </c>
     </row>
     <row r="1400" spans="1:2">
       <c r="A1400" s="1" t="s">
-        <v>4089</v>
+        <v>4087</v>
       </c>
       <c r="B1400" t="s">
-        <v>4090</v>
+        <v>4088</v>
       </c>
     </row>
     <row r="1401" spans="1:2">
       <c r="A1401" s="1" t="s">
-        <v>4091</v>
+        <v>4089</v>
       </c>
       <c r="B1401" t="s">
-        <v>4092</v>
+        <v>4090</v>
       </c>
     </row>
     <row r="1402" spans="1:2">
       <c r="A1402" s="1" t="s">
-        <v>4093</v>
+        <v>4091</v>
       </c>
       <c r="B1402" t="s">
-        <v>4094</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="1403" spans="1:2">
       <c r="A1403" s="1" t="s">
-        <v>4095</v>
+        <v>4093</v>
       </c>
       <c r="B1403" t="s">
-        <v>4096</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="1404" spans="1:2">
       <c r="A1404" s="1" t="s">
-        <v>4097</v>
+        <v>4095</v>
       </c>
       <c r="B1404" t="s">
-        <v>4098</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="1405" spans="1:2">
       <c r="A1405" s="1" t="s">
-        <v>4099</v>
+        <v>4097</v>
       </c>
       <c r="B1405" t="s">
-        <v>4100</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="1406" spans="1:2">
       <c r="A1406" s="1" t="s">
-        <v>4101</v>
+        <v>4099</v>
       </c>
       <c r="B1406" t="s">
-        <v>4102</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="1407" spans="1:2">
       <c r="A1407" s="1" t="s">
-        <v>4103</v>
+        <v>4101</v>
       </c>
       <c r="B1407" t="s">
-        <v>4104</v>
+        <v>4102</v>
       </c>
     </row>
     <row r="1408" spans="1:2">
       <c r="A1408" s="1" t="s">
-        <v>4105</v>
+        <v>4103</v>
       </c>
       <c r="B1408" t="s">
-        <v>4106</v>
+        <v>4104</v>
       </c>
     </row>
     <row r="1409" spans="1:2">
       <c r="A1409" s="1" t="s">
-        <v>4107</v>
+        <v>4105</v>
       </c>
       <c r="B1409" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="1410" spans="1:2">
       <c r="A1410" s="1" t="s">
-        <v>4109</v>
+        <v>4107</v>
       </c>
       <c r="B1410" t="s">
-        <v>4110</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="1411" spans="1:2">
       <c r="A1411" s="1" t="s">
-        <v>4111</v>
+        <v>4109</v>
       </c>
       <c r="B1411" t="s">
-        <v>4112</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="1412" spans="1:2">
       <c r="A1412" s="1" t="s">
-        <v>4113</v>
+        <v>4111</v>
       </c>
       <c r="B1412" t="s">
-        <v>4114</v>
+        <v>4112</v>
       </c>
     </row>
     <row r="1413" spans="1:2">
       <c r="A1413" s="1" t="s">
-        <v>4115</v>
+        <v>4113</v>
       </c>
       <c r="B1413" t="s">
-        <v>4116</v>
+        <v>4114</v>
       </c>
     </row>
     <row r="1414" spans="1:2">
       <c r="A1414" s="1" t="s">
-        <v>4117</v>
+        <v>4115</v>
       </c>
       <c r="B1414" t="s">
-        <v>4118</v>
+        <v>4116</v>
       </c>
     </row>
     <row r="1415" spans="1:2">
       <c r="A1415" s="1" t="s">
-        <v>4119</v>
+        <v>4117</v>
       </c>
       <c r="B1415" t="s">
-        <v>4120</v>
+        <v>4118</v>
       </c>
     </row>
     <row r="1416" spans="1:2">
       <c r="A1416" s="1" t="s">
-        <v>4121</v>
+        <v>4119</v>
       </c>
       <c r="B1416" t="s">
-        <v>4122</v>
+        <v>4120</v>
       </c>
     </row>
     <row r="1417" spans="1:2">
       <c r="A1417" s="1" t="s">
-        <v>4123</v>
+        <v>4121</v>
       </c>
       <c r="B1417" t="s">
-        <v>4124</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="1418" spans="1:2">
       <c r="A1418" s="1" t="s">
-        <v>4125</v>
+        <v>4123</v>
       </c>
       <c r="B1418" t="s">
-        <v>4126</v>
+        <v>4124</v>
       </c>
     </row>
     <row r="1419" spans="1:2">
       <c r="A1419" s="1" t="s">
-        <v>4127</v>
+        <v>4125</v>
       </c>
       <c r="B1419" t="s">
-        <v>4128</v>
+        <v>4126</v>
       </c>
     </row>
     <row r="1420" spans="1:2">
       <c r="A1420" s="1" t="s">
-        <v>4129</v>
+        <v>4127</v>
       </c>
       <c r="B1420" t="s">
-        <v>4130</v>
+        <v>4128</v>
       </c>
     </row>
     <row r="1421" spans="1:2">
       <c r="A1421" s="1" t="s">
-        <v>4131</v>
+        <v>4129</v>
       </c>
       <c r="B1421" t="s">
-        <v>4132</v>
+        <v>4130</v>
       </c>
     </row>
     <row r="1422" spans="1:2">
       <c r="A1422" s="1" t="s">
-        <v>4133</v>
+        <v>4131</v>
       </c>
       <c r="B1422" t="s">
-        <v>4134</v>
+        <v>4132</v>
       </c>
     </row>
     <row r="1423" spans="1:2">
       <c r="A1423" s="1" t="s">
-        <v>4135</v>
+        <v>4133</v>
       </c>
       <c r="B1423" t="s">
-        <v>4136</v>
+        <v>4134</v>
       </c>
     </row>
     <row r="1424" spans="1:2">
       <c r="A1424" s="1" t="s">
-        <v>4137</v>
+        <v>4135</v>
       </c>
       <c r="B1424" t="s">
-        <v>4138</v>
+        <v>4136</v>
       </c>
     </row>
     <row r="1425" spans="1:2">
       <c r="A1425" s="1" t="s">
-        <v>4139</v>
+        <v>4137</v>
       </c>
       <c r="B1425" t="s">
-        <v>4140</v>
+        <v>4138</v>
       </c>
     </row>
     <row r="1426" spans="1:2">
       <c r="A1426" s="1" t="s">
-        <v>4141</v>
+        <v>4139</v>
       </c>
       <c r="B1426" t="s">
-        <v>4142</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="1427" spans="1:2">
       <c r="A1427" s="1" t="s">
-        <v>4143</v>
+        <v>4141</v>
       </c>
       <c r="B1427" t="s">
-        <v>4144</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="1428" spans="1:2">
       <c r="A1428" s="1" t="s">
-        <v>4423</v>
+        <v>4143</v>
       </c>
       <c r="B1428" t="s">
-        <v>4424</v>
+        <v>4144</v>
       </c>
     </row>
     <row r="1429" spans="1:2">
       <c r="A1429" s="1" t="s">
-        <v>4145</v>
+        <v>4423</v>
       </c>
       <c r="B1429" t="s">
-        <v>4146</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="1430" spans="1:2">
       <c r="A1430" s="1" t="s">
-        <v>4147</v>
+        <v>4145</v>
       </c>
       <c r="B1430" t="s">
-        <v>4148</v>
+        <v>4146</v>
       </c>
     </row>
     <row r="1431" spans="1:2">
       <c r="A1431" s="1" t="s">
-        <v>4149</v>
+        <v>4147</v>
       </c>
       <c r="B1431" t="s">
-        <v>4150</v>
+        <v>4148</v>
       </c>
     </row>
     <row r="1432" spans="1:2">
       <c r="A1432" s="1" t="s">
-        <v>4151</v>
+        <v>4149</v>
       </c>
       <c r="B1432" t="s">
-        <v>4152</v>
+        <v>4150</v>
       </c>
     </row>
     <row r="1433" spans="1:2">
       <c r="A1433" s="1" t="s">
-        <v>4153</v>
+        <v>4151</v>
       </c>
       <c r="B1433" t="s">
-        <v>4154</v>
+        <v>4152</v>
       </c>
     </row>
     <row r="1434" spans="1:2">
       <c r="A1434" s="1" t="s">
-        <v>4155</v>
+        <v>4153</v>
       </c>
       <c r="B1434" t="s">
-        <v>4156</v>
+        <v>4154</v>
       </c>
     </row>
     <row r="1435" spans="1:2">
       <c r="A1435" s="1" t="s">
-        <v>4157</v>
+        <v>4155</v>
       </c>
       <c r="B1435" t="s">
-        <v>4158</v>
+        <v>4156</v>
       </c>
     </row>
     <row r="1436" spans="1:2">
       <c r="A1436" s="1" t="s">
-        <v>4159</v>
+        <v>4157</v>
       </c>
       <c r="B1436" t="s">
-        <v>4160</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="1437" spans="1:2">
       <c r="A1437" s="1" t="s">
-        <v>4161</v>
+        <v>4159</v>
       </c>
       <c r="B1437" t="s">
-        <v>4162</v>
+        <v>4160</v>
       </c>
     </row>
     <row r="1438" spans="1:2">
       <c r="A1438" s="1" t="s">
-        <v>4163</v>
+        <v>4161</v>
       </c>
       <c r="B1438" t="s">
-        <v>4164</v>
+        <v>4162</v>
       </c>
     </row>
     <row r="1439" spans="1:2">
       <c r="A1439" s="1" t="s">
-        <v>4165</v>
+        <v>4163</v>
       </c>
       <c r="B1439" t="s">
-        <v>4166</v>
+        <v>4164</v>
       </c>
     </row>
     <row r="1440" spans="1:2">
       <c r="A1440" s="1" t="s">
-        <v>4167</v>
+        <v>4165</v>
       </c>
       <c r="B1440" t="s">
-        <v>4168</v>
+        <v>4166</v>
       </c>
     </row>
     <row r="1441" spans="1:2">
       <c r="A1441" s="1" t="s">
-        <v>4169</v>
+        <v>4167</v>
       </c>
       <c r="B1441" t="s">
-        <v>4170</v>
+        <v>4168</v>
       </c>
     </row>
     <row r="1442" spans="1:2">
       <c r="A1442" s="1" t="s">
-        <v>4171</v>
+        <v>4169</v>
       </c>
       <c r="B1442" t="s">
-        <v>4172</v>
+        <v>4170</v>
       </c>
     </row>
     <row r="1443" spans="1:2">
       <c r="A1443" s="1" t="s">
-        <v>4173</v>
+        <v>4171</v>
       </c>
       <c r="B1443" t="s">
-        <v>4174</v>
+        <v>4172</v>
       </c>
     </row>
     <row r="1444" spans="1:2">
       <c r="A1444" s="1" t="s">
-        <v>4175</v>
+        <v>4173</v>
       </c>
       <c r="B1444" t="s">
-        <v>4176</v>
+        <v>4174</v>
       </c>
     </row>
     <row r="1445" spans="1:2">
       <c r="A1445" s="1" t="s">
-        <v>4177</v>
+        <v>4175</v>
       </c>
       <c r="B1445" t="s">
-        <v>4178</v>
+        <v>4176</v>
       </c>
     </row>
     <row r="1446" spans="1:2">
       <c r="A1446" s="1" t="s">
-        <v>4179</v>
+        <v>4452</v>
       </c>
       <c r="B1446" t="s">
-        <v>4180</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="1447" spans="1:2">
       <c r="A1447" s="1" t="s">
-        <v>4181</v>
+        <v>4177</v>
       </c>
       <c r="B1447" t="s">
-        <v>4182</v>
+        <v>4178</v>
       </c>
     </row>
     <row r="1448" spans="1:2">
       <c r="A1448" s="1" t="s">
-        <v>4183</v>
+        <v>4179</v>
       </c>
       <c r="B1448" t="s">
-        <v>4184</v>
+        <v>4180</v>
       </c>
     </row>
     <row r="1449" spans="1:2">
       <c r="A1449" s="1" t="s">
-        <v>4185</v>
+        <v>4181</v>
       </c>
       <c r="B1449" t="s">
-        <v>4186</v>
+        <v>4182</v>
       </c>
     </row>
     <row r="1450" spans="1:2">
       <c r="A1450" s="1" t="s">
-        <v>4187</v>
+        <v>4183</v>
       </c>
       <c r="B1450" t="s">
-        <v>4188</v>
+        <v>4184</v>
       </c>
     </row>
     <row r="1451" spans="1:2">
       <c r="A1451" s="1" t="s">
-        <v>4189</v>
+        <v>4185</v>
       </c>
       <c r="B1451" t="s">
-        <v>4190</v>
+        <v>4186</v>
       </c>
     </row>
     <row r="1452" spans="1:2">
       <c r="A1452" s="1" t="s">
-        <v>4191</v>
+        <v>4187</v>
       </c>
       <c r="B1452" t="s">
-        <v>4192</v>
+        <v>4188</v>
       </c>
     </row>
     <row r="1453" spans="1:2">
       <c r="A1453" s="1" t="s">
-        <v>4193</v>
+        <v>4189</v>
       </c>
       <c r="B1453" t="s">
-        <v>4194</v>
+        <v>4190</v>
       </c>
     </row>
     <row r="1454" spans="1:2">
       <c r="A1454" s="1" t="s">
-        <v>4451</v>
+        <v>4191</v>
       </c>
       <c r="B1454" t="s">
-        <v>4452</v>
+        <v>4192</v>
       </c>
     </row>
     <row r="1455" spans="1:2">
       <c r="A1455" s="1" t="s">
-        <v>4195</v>
+        <v>4193</v>
       </c>
       <c r="B1455" t="s">
-        <v>4196</v>
+        <v>4194</v>
       </c>
     </row>
     <row r="1456" spans="1:2">
       <c r="A1456" s="1" t="s">
-        <v>4197</v>
+        <v>4195</v>
       </c>
       <c r="B1456" t="s">
-        <v>4198</v>
+        <v>4196</v>
       </c>
     </row>
     <row r="1457" spans="1:2">
       <c r="A1457" s="1" t="s">
-        <v>4199</v>
+        <v>4197</v>
       </c>
       <c r="B1457" t="s">
-        <v>4200</v>
+        <v>4198</v>
       </c>
     </row>
     <row r="1458" spans="1:2">
       <c r="A1458" s="1" t="s">
-        <v>4201</v>
+        <v>4199</v>
       </c>
       <c r="B1458" t="s">
-        <v>4202</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="1459" spans="1:2">
       <c r="A1459" s="1" t="s">
-        <v>4203</v>
+        <v>4201</v>
       </c>
       <c r="B1459" t="s">
-        <v>4204</v>
+        <v>4202</v>
       </c>
     </row>
     <row r="1460" spans="1:2">
       <c r="A1460" s="1" t="s">
-        <v>4205</v>
+        <v>4203</v>
       </c>
       <c r="B1460" t="s">
-        <v>4206</v>
+        <v>4204</v>
       </c>
     </row>
     <row r="1461" spans="1:2">
       <c r="A1461" s="1" t="s">
-        <v>4207</v>
+        <v>4205</v>
       </c>
       <c r="B1461" t="s">
-        <v>4208</v>
+        <v>4206</v>
       </c>
     </row>
     <row r="1462" spans="1:2">
       <c r="A1462" s="1" t="s">
-        <v>4209</v>
+        <v>4207</v>
       </c>
       <c r="B1462" t="s">
-        <v>4210</v>
+        <v>4208</v>
       </c>
     </row>
     <row r="1463" spans="1:2">
       <c r="A1463" s="1" t="s">
-        <v>4211</v>
+        <v>4209</v>
       </c>
       <c r="B1463" t="s">
-        <v>4212</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="1464" spans="1:2">
       <c r="A1464" s="1" t="s">
-        <v>4213</v>
+        <v>4211</v>
       </c>
       <c r="B1464" t="s">
-        <v>4214</v>
+        <v>4212</v>
       </c>
     </row>
     <row r="1465" spans="1:2">
       <c r="A1465" s="1" t="s">
-        <v>4215</v>
+        <v>4213</v>
       </c>
       <c r="B1465" t="s">
-        <v>4216</v>
+        <v>4214</v>
       </c>
     </row>
     <row r="1466" spans="1:2">
       <c r="A1466" s="1" t="s">
-        <v>4217</v>
+        <v>4215</v>
       </c>
       <c r="B1466" t="s">
-        <v>4218</v>
+        <v>4216</v>
       </c>
     </row>
     <row r="1467" spans="1:2">
       <c r="A1467" s="1" t="s">
-        <v>4219</v>
+        <v>4217</v>
       </c>
       <c r="B1467" t="s">
-        <v>4220</v>
+        <v>4218</v>
       </c>
     </row>
     <row r="1468" spans="1:2">
       <c r="A1468" s="1" t="s">
-        <v>4221</v>
+        <v>4219</v>
       </c>
       <c r="B1468" t="s">
-        <v>4222</v>
+        <v>4220</v>
       </c>
     </row>
     <row r="1469" spans="1:2">
       <c r="A1469" s="1" t="s">
-        <v>4223</v>
+        <v>4221</v>
       </c>
       <c r="B1469" t="s">
-        <v>4224</v>
+        <v>4222</v>
       </c>
     </row>
     <row r="1470" spans="1:2">
       <c r="A1470" s="1" t="s">
-        <v>4225</v>
+        <v>4223</v>
       </c>
       <c r="B1470" t="s">
-        <v>4226</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="1471" spans="1:2">
       <c r="A1471" s="1" t="s">
-        <v>4227</v>
+        <v>4225</v>
       </c>
       <c r="B1471" t="s">
-        <v>4228</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="1472" spans="1:2">
       <c r="A1472" s="1" t="s">
-        <v>4229</v>
+        <v>4227</v>
       </c>
       <c r="B1472" t="s">
-        <v>4230</v>
+        <v>4228</v>
       </c>
     </row>
     <row r="1473" spans="1:2">
       <c r="A1473" s="1" t="s">
-        <v>4231</v>
+        <v>4229</v>
       </c>
       <c r="B1473" t="s">
-        <v>4232</v>
+        <v>4230</v>
       </c>
     </row>
     <row r="1474" spans="1:2">
       <c r="A1474" s="1" t="s">
-        <v>4233</v>
+        <v>4231</v>
       </c>
       <c r="B1474" t="s">
-        <v>4234</v>
+        <v>4232</v>
       </c>
     </row>
     <row r="1475" spans="1:2">
       <c r="A1475" s="1" t="s">
-        <v>4235</v>
+        <v>4233</v>
       </c>
       <c r="B1475" t="s">
-        <v>4236</v>
+        <v>4234</v>
       </c>
     </row>
     <row r="1476" spans="1:2">
       <c r="A1476" s="1" t="s">
-        <v>4237</v>
+        <v>4235</v>
       </c>
       <c r="B1476" t="s">
-        <v>4238</v>
+        <v>4236</v>
       </c>
     </row>
     <row r="1477" spans="1:2">
       <c r="A1477" s="1" t="s">
-        <v>4239</v>
+        <v>4237</v>
       </c>
       <c r="B1477" t="s">
-        <v>4240</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="1478" spans="1:2">
       <c r="A1478" s="1" t="s">
-        <v>4241</v>
+        <v>4239</v>
       </c>
       <c r="B1478" t="s">
-        <v>4242</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="1479" spans="1:2">
       <c r="A1479" s="1" t="s">
-        <v>4243</v>
+        <v>4241</v>
       </c>
       <c r="B1479" t="s">
-        <v>4244</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="1480" spans="1:2">
       <c r="A1480" s="1" t="s">
-        <v>4245</v>
+        <v>4243</v>
       </c>
       <c r="B1480" t="s">
-        <v>4246</v>
+        <v>4244</v>
       </c>
     </row>
     <row r="1481" spans="1:2">
       <c r="A1481" s="1" t="s">
-        <v>4247</v>
+        <v>4245</v>
       </c>
       <c r="B1481" t="s">
-        <v>4248</v>
+        <v>4246</v>
       </c>
     </row>
     <row r="1482" spans="1:2">
       <c r="A1482" s="1" t="s">
-        <v>4249</v>
+        <v>4247</v>
       </c>
       <c r="B1482" t="s">
-        <v>4250</v>
+        <v>4248</v>
       </c>
     </row>
     <row r="1483" spans="1:2">
       <c r="A1483" s="1" t="s">
-        <v>4251</v>
+        <v>4249</v>
       </c>
       <c r="B1483" t="s">
-        <v>4252</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="1484" spans="1:2">
       <c r="A1484" s="1" t="s">
-        <v>4253</v>
+        <v>4251</v>
       </c>
       <c r="B1484" t="s">
-        <v>4254</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="1485" spans="1:2">
       <c r="A1485" s="1" t="s">
-        <v>4255</v>
+        <v>4253</v>
       </c>
       <c r="B1485" t="s">
-        <v>4256</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="1486" spans="1:2">
       <c r="A1486" s="1" t="s">
-        <v>4257</v>
+        <v>4255</v>
       </c>
       <c r="B1486" t="s">
-        <v>4258</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="1487" spans="1:2">
       <c r="A1487" s="1" t="s">
-        <v>4259</v>
+        <v>4257</v>
       </c>
       <c r="B1487" t="s">
-        <v>4260</v>
+        <v>4258</v>
       </c>
     </row>
     <row r="1488" spans="1:2">
       <c r="A1488" s="1" t="s">
-        <v>4261</v>
+        <v>4259</v>
       </c>
       <c r="B1488" t="s">
-        <v>4262</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="1489" spans="1:2">
       <c r="A1489" s="1" t="s">
-        <v>4263</v>
+        <v>4261</v>
       </c>
       <c r="B1489" t="s">
-        <v>4264</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="1490" spans="1:2">
       <c r="A1490" s="1" t="s">
-        <v>4265</v>
+        <v>4263</v>
       </c>
       <c r="B1490" t="s">
-        <v>4266</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="1491" spans="1:2">
       <c r="A1491" s="1" t="s">
-        <v>4267</v>
+        <v>4265</v>
       </c>
       <c r="B1491" t="s">
-        <v>4268</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="1492" spans="1:2">
       <c r="A1492" s="1" t="s">
-        <v>4269</v>
+        <v>4267</v>
       </c>
       <c r="B1492" t="s">
-        <v>4270</v>
+        <v>4268</v>
       </c>
     </row>
     <row r="1493" spans="1:2">
       <c r="A1493" s="1" t="s">
-        <v>4271</v>
+        <v>4269</v>
       </c>
       <c r="B1493" t="s">
-        <v>4272</v>
+        <v>4270</v>
       </c>
     </row>
     <row r="1494" spans="1:2">
       <c r="A1494" s="1" t="s">
-        <v>4273</v>
+        <v>4271</v>
       </c>
       <c r="B1494" t="s">
-        <v>4274</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="1495" spans="1:2">
       <c r="A1495" s="1" t="s">
-        <v>4275</v>
+        <v>4273</v>
       </c>
       <c r="B1495" t="s">
-        <v>4276</v>
+        <v>4274</v>
       </c>
     </row>
     <row r="1496" spans="1:2">
       <c r="A1496" s="1" t="s">
-        <v>4277</v>
+        <v>4275</v>
       </c>
       <c r="B1496" t="s">
-        <v>4278</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="1497" spans="1:2">
       <c r="A1497" s="1" t="s">
-        <v>4279</v>
+        <v>4277</v>
       </c>
       <c r="B1497" t="s">
-        <v>4280</v>
+        <v>4278</v>
       </c>
     </row>
     <row r="1498" spans="1:2">
       <c r="A1498" s="1" t="s">
-        <v>4281</v>
+        <v>4279</v>
       </c>
       <c r="B1498" t="s">
-        <v>4282</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="1499" spans="1:2">
       <c r="A1499" s="1" t="s">
-        <v>4283</v>
+        <v>4281</v>
       </c>
       <c r="B1499" t="s">
-        <v>4284</v>
+        <v>4282</v>
       </c>
     </row>
     <row r="1500" spans="1:2">
       <c r="A1500" s="1" t="s">
-        <v>4285</v>
+        <v>4283</v>
       </c>
       <c r="B1500" t="s">
-        <v>4286</v>
+        <v>4284</v>
       </c>
     </row>
     <row r="1501" spans="1:2">
       <c r="A1501" s="1" t="s">
-        <v>4287</v>
+        <v>4285</v>
       </c>
       <c r="B1501" t="s">
-        <v>4288</v>
+        <v>4286</v>
       </c>
     </row>
     <row r="1502" spans="1:2">
       <c r="A1502" s="1" t="s">
-        <v>4289</v>
+        <v>4287</v>
       </c>
       <c r="B1502" t="s">
-        <v>4290</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="1503" spans="1:2">
       <c r="A1503" s="1" t="s">
-        <v>4291</v>
+        <v>4289</v>
       </c>
       <c r="B1503" t="s">
-        <v>4292</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="1504" spans="1:2">
       <c r="A1504" s="1" t="s">
-        <v>4293</v>
+        <v>4291</v>
       </c>
       <c r="B1504" t="s">
-        <v>4294</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="1505" spans="1:2">
       <c r="A1505" s="1" t="s">
-        <v>4295</v>
+        <v>4293</v>
       </c>
       <c r="B1505" t="s">
-        <v>4296</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="1506" spans="1:2">
       <c r="A1506" s="1" t="s">
-        <v>4297</v>
+        <v>4295</v>
       </c>
       <c r="B1506" t="s">
-        <v>4298</v>
+        <v>4296</v>
       </c>
     </row>
     <row r="1507" spans="1:2">
       <c r="A1507" s="1" t="s">
-        <v>4299</v>
+        <v>4297</v>
       </c>
       <c r="B1507" t="s">
-        <v>4300</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="1508" spans="1:2">
       <c r="A1508" s="1" t="s">
-        <v>4446</v>
+        <v>4299</v>
       </c>
       <c r="B1508" t="s">
-        <v>4447</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="1509" spans="1:2">
       <c r="A1509" s="1" t="s">
-        <v>4431</v>
+        <v>4446</v>
       </c>
       <c r="B1509" t="s">
-        <v>4432</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="1510" spans="1:2">
       <c r="A1510" s="1" t="s">
-        <v>4301</v>
+        <v>4431</v>
       </c>
       <c r="B1510" t="s">
-        <v>4302</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="1511" spans="1:2">
       <c r="A1511" s="1" t="s">
-        <v>4303</v>
+        <v>4301</v>
       </c>
       <c r="B1511" t="s">
-        <v>4304</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="1512" spans="1:2">
       <c r="A1512" s="1" t="s">
-        <v>4305</v>
+        <v>4303</v>
       </c>
       <c r="B1512" t="s">
-        <v>4306</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="1513" spans="1:2">
       <c r="A1513" s="1" t="s">
-        <v>4307</v>
+        <v>4305</v>
       </c>
       <c r="B1513" t="s">
-        <v>4308</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="1514" spans="1:2">
       <c r="A1514" s="1" t="s">
-        <v>4309</v>
+        <v>4307</v>
       </c>
       <c r="B1514" t="s">
-        <v>4310</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="1515" spans="1:2">
       <c r="A1515" s="1" t="s">
-        <v>4311</v>
+        <v>4309</v>
       </c>
       <c r="B1515" t="s">
-        <v>4312</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="1516" spans="1:2">
       <c r="A1516" s="1" t="s">
-        <v>4313</v>
+        <v>4311</v>
       </c>
       <c r="B1516" t="s">
-        <v>4314</v>
+        <v>4312</v>
       </c>
     </row>
     <row r="1517" spans="1:2">
       <c r="A1517" s="1" t="s">
-        <v>4315</v>
+        <v>4313</v>
       </c>
       <c r="B1517" t="s">
-        <v>4316</v>
+        <v>4314</v>
       </c>
     </row>
     <row r="1518" spans="1:2">
       <c r="A1518" s="1" t="s">
-        <v>4317</v>
+        <v>4315</v>
       </c>
       <c r="B1518" t="s">
-        <v>4318</v>
+        <v>4316</v>
       </c>
     </row>
     <row r="1519" spans="1:2">
       <c r="A1519" s="1" t="s">
-        <v>4319</v>
+        <v>4317</v>
       </c>
       <c r="B1519" t="s">
-        <v>4320</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="1520" spans="1:2">
       <c r="A1520" s="1" t="s">
-        <v>4321</v>
+        <v>4319</v>
       </c>
       <c r="B1520" t="s">
-        <v>4322</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="1521" spans="1:2">
       <c r="A1521" s="1" t="s">
-        <v>4323</v>
+        <v>4321</v>
       </c>
       <c r="B1521" t="s">
-        <v>4324</v>
+        <v>4322</v>
       </c>
     </row>
     <row r="1522" spans="1:2">
       <c r="A1522" s="1" t="s">
-        <v>4325</v>
+        <v>4323</v>
       </c>
       <c r="B1522" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
     </row>
     <row r="1523" spans="1:2">
       <c r="A1523" s="1" t="s">
-        <v>4327</v>
+        <v>4325</v>
       </c>
       <c r="B1523" t="s">
-        <v>4328</v>
+        <v>4326</v>
       </c>
     </row>
     <row r="1524" spans="1:2">
       <c r="A1524" s="1" t="s">
-        <v>4329</v>
+        <v>4327</v>
       </c>
       <c r="B1524" t="s">
-        <v>4330</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="1525" spans="1:2">
       <c r="A1525" s="1" t="s">
-        <v>4331</v>
+        <v>4329</v>
       </c>
       <c r="B1525" t="s">
-        <v>4332</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="1526" spans="1:2">
       <c r="A1526" s="1" t="s">
-        <v>4333</v>
+        <v>4331</v>
       </c>
       <c r="B1526" t="s">
-        <v>4334</v>
+        <v>4332</v>
       </c>
     </row>
     <row r="1527" spans="1:2">
       <c r="A1527" s="1" t="s">
-        <v>4335</v>
+        <v>4333</v>
       </c>
       <c r="B1527" t="s">
-        <v>4336</v>
+        <v>4334</v>
       </c>
     </row>
     <row r="1528" spans="1:2">
       <c r="A1528" s="1" t="s">
-        <v>4337</v>
+        <v>4335</v>
       </c>
       <c r="B1528" t="s">
-        <v>4338</v>
+        <v>4336</v>
       </c>
     </row>
     <row r="1529" spans="1:2">
       <c r="A1529" s="1" t="s">
-        <v>4339</v>
+        <v>4337</v>
       </c>
       <c r="B1529" t="s">
-        <v>4340</v>
+        <v>4338</v>
       </c>
     </row>
     <row r="1530" spans="1:2">
       <c r="A1530" s="1" t="s">
-        <v>4341</v>
+        <v>4339</v>
       </c>
       <c r="B1530" t="s">
-        <v>4342</v>
+        <v>4340</v>
       </c>
     </row>
     <row r="1531" spans="1:2">
       <c r="A1531" s="1" t="s">
-        <v>4343</v>
+        <v>4341</v>
       </c>
       <c r="B1531" t="s">
-        <v>4344</v>
+        <v>4342</v>
       </c>
     </row>
     <row r="1532" spans="1:2">
       <c r="A1532" s="1" t="s">
-        <v>4345</v>
+        <v>4343</v>
       </c>
       <c r="B1532" t="s">
-        <v>4346</v>
+        <v>4344</v>
       </c>
     </row>
     <row r="1533" spans="1:2">
       <c r="A1533" s="1" t="s">
-        <v>4347</v>
+        <v>4345</v>
       </c>
       <c r="B1533" t="s">
-        <v>4348</v>
+        <v>4346</v>
       </c>
     </row>
     <row r="1534" spans="1:2">
       <c r="A1534" s="1" t="s">
-        <v>4349</v>
+        <v>4347</v>
       </c>
       <c r="B1534" t="s">
-        <v>4350</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="1535" spans="1:2">
       <c r="A1535" s="1" t="s">
-        <v>4351</v>
+        <v>4349</v>
       </c>
       <c r="B1535" t="s">
-        <v>4352</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="1536" spans="1:2">
       <c r="A1536" s="1" t="s">
-        <v>4353</v>
+        <v>4351</v>
       </c>
       <c r="B1536" t="s">
-        <v>4354</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="1537" spans="1:2">
       <c r="A1537" s="1" t="s">
-        <v>4355</v>
+        <v>4353</v>
       </c>
       <c r="B1537" t="s">
-        <v>4356</v>
+        <v>4354</v>
       </c>
     </row>
     <row r="1538" spans="1:2">
       <c r="A1538" s="1" t="s">
-        <v>4357</v>
+        <v>4355</v>
       </c>
       <c r="B1538" t="s">
-        <v>4358</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="1539" spans="1:2">
       <c r="A1539" s="1" t="s">
-        <v>4359</v>
+        <v>4357</v>
       </c>
       <c r="B1539" t="s">
-        <v>4360</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="1540" spans="1:2">
       <c r="A1540" s="1" t="s">
-        <v>4361</v>
+        <v>4359</v>
       </c>
       <c r="B1540" t="s">
-        <v>4362</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="1541" spans="1:2">
       <c r="A1541" s="1" t="s">
-        <v>4363</v>
+        <v>4361</v>
       </c>
       <c r="B1541" t="s">
-        <v>4364</v>
+        <v>4362</v>
       </c>
     </row>
     <row r="1542" spans="1:2">
       <c r="A1542" s="1" t="s">
-        <v>4365</v>
+        <v>4363</v>
       </c>
       <c r="B1542" t="s">
-        <v>4366</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="1543" spans="1:2">
       <c r="A1543" s="1" t="s">
-        <v>4427</v>
+        <v>4365</v>
       </c>
       <c r="B1543" t="s">
-        <v>4428</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="1544" spans="1:2">
       <c r="A1544" s="1" t="s">
-        <v>4367</v>
+        <v>4427</v>
       </c>
       <c r="B1544" t="s">
-        <v>4368</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="1545" spans="1:2">
       <c r="A1545" s="1" t="s">
-        <v>4369</v>
+        <v>4367</v>
       </c>
       <c r="B1545" t="s">
-        <v>4370</v>
+        <v>4368</v>
       </c>
     </row>
     <row r="1546" spans="1:2">
       <c r="A1546" s="1" t="s">
-        <v>4371</v>
+        <v>4369</v>
       </c>
       <c r="B1546" t="s">
-        <v>4372</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="1547" spans="1:2">
       <c r="A1547" s="1" t="s">
-        <v>4373</v>
+        <v>4371</v>
       </c>
       <c r="B1547" t="s">
-        <v>4374</v>
+        <v>4372</v>
       </c>
     </row>
     <row r="1548" spans="1:2">
       <c r="A1548" s="1" t="s">
-        <v>4375</v>
+        <v>4373</v>
       </c>
       <c r="B1548" t="s">
-        <v>4376</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="1549" spans="1:2">
       <c r="A1549" s="1" t="s">
-        <v>4377</v>
+        <v>4375</v>
       </c>
       <c r="B1549" t="s">
-        <v>4378</v>
+        <v>4376</v>
       </c>
     </row>
     <row r="1550" spans="1:2">
       <c r="A1550" s="1" t="s">
-        <v>4379</v>
+        <v>4377</v>
       </c>
       <c r="B1550" t="s">
-        <v>4380</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="1551" spans="1:2">
       <c r="A1551" s="1" t="s">
-        <v>4438</v>
+        <v>4379</v>
       </c>
       <c r="B1551" t="s">
-        <v>4439</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="1552" spans="1:2">
       <c r="A1552" s="1" t="s">
-        <v>4381</v>
+        <v>4438</v>
       </c>
       <c r="B1552" t="s">
-        <v>4382</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="1553" spans="1:2">
       <c r="A1553" s="1" t="s">
-        <v>4383</v>
+        <v>4381</v>
       </c>
       <c r="B1553" t="s">
-        <v>4384</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="1554" spans="1:2">
       <c r="A1554" s="1" t="s">
-        <v>4385</v>
+        <v>4383</v>
       </c>
       <c r="B1554" t="s">
-        <v>4386</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="1555" spans="1:2">
       <c r="A1555" s="1" t="s">
-        <v>4387</v>
+        <v>4385</v>
       </c>
       <c r="B1555" t="s">
-        <v>4388</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="1556" spans="1:2">
       <c r="A1556" s="1" t="s">
-        <v>4389</v>
+        <v>4387</v>
       </c>
       <c r="B1556" t="s">
-        <v>4390</v>
+        <v>4388</v>
       </c>
     </row>
     <row r="1557" spans="1:2">
       <c r="A1557" s="1" t="s">
-        <v>4391</v>
+        <v>4389</v>
       </c>
       <c r="B1557" t="s">
-        <v>4392</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="1558" spans="1:2">
       <c r="A1558" s="1" t="s">
-        <v>4393</v>
+        <v>4391</v>
       </c>
       <c r="B1558" t="s">
-        <v>4394</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="1559" spans="1:2">
       <c r="A1559" s="1" t="s">
-        <v>4395</v>
+        <v>4393</v>
       </c>
       <c r="B1559" t="s">
-        <v>4396</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="1560" spans="1:2">
       <c r="A1560" s="1" t="s">
-        <v>4397</v>
+        <v>4395</v>
       </c>
       <c r="B1560" t="s">
-        <v>4398</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="1561" spans="1:2">
       <c r="A1561" s="1" t="s">
-        <v>4399</v>
+        <v>4397</v>
       </c>
       <c r="B1561" t="s">
-        <v>4400</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="1562" spans="1:2">
       <c r="A1562" s="1" t="s">
-        <v>4401</v>
+        <v>4399</v>
       </c>
       <c r="B1562" t="s">
-        <v>4402</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="1563" spans="1:2">
       <c r="A1563" s="1" t="s">
-        <v>4403</v>
+        <v>4401</v>
       </c>
       <c r="B1563" t="s">
-        <v>4404</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="1564" spans="1:2">
       <c r="A1564" s="1" t="s">
-        <v>4405</v>
+        <v>4403</v>
       </c>
       <c r="B1564" t="s">
-        <v>4406</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="1565" spans="1:2">
       <c r="A1565" s="1" t="s">
+        <v>4405</v>
+      </c>
+      <c r="B1565" t="s">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:2">
+      <c r="A1566" s="1" t="s">
         <v>4407</v>
       </c>
-      <c r="B1565" t="s">
+      <c r="B1566" t="s">
         <v>4408</v>
       </c>
     </row>
@@ -26652,7 +26667,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -27898,7 +27913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -36555,7 +36570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -37282,7 +37297,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" display="https://www.google.rw/search?hl=en&amp;biw=1366&amp;bih=667&amp;q=bujumbura+burundi&amp;stick=H4sIAAAAAAAAAGOovnz8BQMDAw8HsxKHfq6-QVqemblixzKD52fj3Z_cuP7PdUL6nIqaeR4ApIgDhCkAAAA&amp;sa=X&amp;ei=wSMzUYVrk7OEB_i7gJgH&amp;sqi=2&amp;ved=0CJUBEJsTKAI"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://www.google.rw/search?hl=en&amp;biw=1366&amp;bih=667&amp;q=bujumbura+burundi&amp;stick=H4sIAAAAAAAAAGOovnz8BQMDAw8HsxKHfq6-QVqemblixzKD52fj3Z_cuP7PdUL6nIqaeR4ApIgDhCkAAAA&amp;sa=X&amp;ei=wSMzUYVrk7OEB_i7gJgH&amp;sqi=2&amp;ved=0CJUBEJsTKAI" xr:uid="{0A4B2DA9-5864-46FD-9BE7-7E76C4E5CAA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -37290,7 +37305,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -37772,7 +37787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>

</xml_diff>

<commit_message>
feat: update the COA file
</commit_message>
<xml_diff>
--- a/public/6. COA.xlsx
+++ b/public/6. COA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patience.uwase\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patience.uwase\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58089D24-4DDC-47DA-BB87-A4A6F1F6EC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E519333-0A8B-48D2-AD26-6830228BB2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier Details" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Route!$A$4:$B$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4492" uniqueCount="4455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4498" uniqueCount="4461">
   <si>
     <t>ACCESS BANK -USD</t>
   </si>
@@ -13410,6 +13411,24 @@
   </si>
   <si>
     <t>SOCOMAT S.A.R.L</t>
+  </si>
+  <si>
+    <t>Q0025</t>
+  </si>
+  <si>
+    <t>QATAR AIRWAYS GROUP Q.C.S.C/B737-8H6</t>
+  </si>
+  <si>
+    <t>S0183</t>
+  </si>
+  <si>
+    <t>SES INSURANCE</t>
+  </si>
+  <si>
+    <t>S085</t>
+  </si>
+  <si>
+    <t>SMART AVIATION</t>
   </si>
 </sst>
 </file>
@@ -14117,10 +14136,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B1566"/>
+  <dimension ref="A1:B1569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1108" workbookViewId="0">
-      <selection activeCell="B1366" sqref="B1366"/>
+    <sheetView tabSelected="1" topLeftCell="A1423" workbookViewId="0">
+      <selection activeCell="B1440" sqref="B1440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -24411,2249 +24430,2273 @@
     </row>
     <row r="1286" spans="1:2">
       <c r="A1286" s="1" t="s">
-        <v>3864</v>
+        <v>4455</v>
       </c>
       <c r="B1286" t="s">
-        <v>3865</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="1287" spans="1:2">
       <c r="A1287" s="1" t="s">
-        <v>3866</v>
+        <v>3864</v>
       </c>
       <c r="B1287" t="s">
-        <v>3867</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1288" spans="1:2">
       <c r="A1288" s="1" t="s">
-        <v>3868</v>
+        <v>3866</v>
       </c>
       <c r="B1288" t="s">
-        <v>3869</v>
+        <v>3867</v>
       </c>
     </row>
     <row r="1289" spans="1:2">
       <c r="A1289" s="1" t="s">
-        <v>3870</v>
+        <v>3868</v>
       </c>
       <c r="B1289" t="s">
-        <v>3871</v>
+        <v>3869</v>
       </c>
     </row>
     <row r="1290" spans="1:2">
       <c r="A1290" s="1" t="s">
-        <v>3872</v>
+        <v>3870</v>
       </c>
       <c r="B1290" t="s">
-        <v>3873</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1291" spans="1:2">
       <c r="A1291" s="1" t="s">
-        <v>3874</v>
+        <v>3872</v>
       </c>
       <c r="B1291" t="s">
-        <v>3875</v>
+        <v>3873</v>
       </c>
     </row>
     <row r="1292" spans="1:2">
       <c r="A1292" s="1" t="s">
-        <v>3876</v>
+        <v>3874</v>
       </c>
       <c r="B1292" t="s">
-        <v>3877</v>
+        <v>3875</v>
       </c>
     </row>
     <row r="1293" spans="1:2">
       <c r="A1293" s="1" t="s">
-        <v>3878</v>
+        <v>3876</v>
       </c>
       <c r="B1293" t="s">
-        <v>3879</v>
+        <v>3877</v>
       </c>
     </row>
     <row r="1294" spans="1:2">
       <c r="A1294" s="1" t="s">
-        <v>3880</v>
+        <v>3878</v>
       </c>
       <c r="B1294" t="s">
-        <v>3881</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1295" spans="1:2">
       <c r="A1295" s="1" t="s">
-        <v>3882</v>
+        <v>3880</v>
       </c>
       <c r="B1295" t="s">
-        <v>3883</v>
+        <v>3881</v>
       </c>
     </row>
     <row r="1296" spans="1:2">
       <c r="A1296" s="1" t="s">
-        <v>3884</v>
+        <v>3882</v>
       </c>
       <c r="B1296" t="s">
-        <v>3885</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="1297" spans="1:2">
       <c r="A1297" s="1" t="s">
-        <v>3886</v>
+        <v>3884</v>
       </c>
       <c r="B1297" t="s">
-        <v>3887</v>
+        <v>3885</v>
       </c>
     </row>
     <row r="1298" spans="1:2">
       <c r="A1298" s="1" t="s">
-        <v>3888</v>
+        <v>3886</v>
       </c>
       <c r="B1298" t="s">
-        <v>3889</v>
+        <v>3887</v>
       </c>
     </row>
     <row r="1299" spans="1:2">
       <c r="A1299" s="1" t="s">
-        <v>3890</v>
+        <v>3888</v>
       </c>
       <c r="B1299" t="s">
-        <v>3891</v>
+        <v>3889</v>
       </c>
     </row>
     <row r="1300" spans="1:2">
       <c r="A1300" s="1" t="s">
-        <v>3892</v>
+        <v>3890</v>
       </c>
       <c r="B1300" t="s">
-        <v>3893</v>
+        <v>3891</v>
       </c>
     </row>
     <row r="1301" spans="1:2">
       <c r="A1301" s="1" t="s">
-        <v>3894</v>
+        <v>3892</v>
       </c>
       <c r="B1301" t="s">
-        <v>3895</v>
+        <v>3893</v>
       </c>
     </row>
     <row r="1302" spans="1:2">
       <c r="A1302" s="1" t="s">
-        <v>3896</v>
+        <v>3894</v>
       </c>
       <c r="B1302" t="s">
-        <v>3897</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="1303" spans="1:2">
       <c r="A1303" s="1" t="s">
-        <v>3898</v>
+        <v>3896</v>
       </c>
       <c r="B1303" t="s">
-        <v>3899</v>
+        <v>3897</v>
       </c>
     </row>
     <row r="1304" spans="1:2">
       <c r="A1304" s="1" t="s">
-        <v>3900</v>
+        <v>3898</v>
       </c>
       <c r="B1304" t="s">
-        <v>3901</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="1305" spans="1:2">
       <c r="A1305" s="1" t="s">
-        <v>3902</v>
+        <v>3900</v>
       </c>
       <c r="B1305" t="s">
-        <v>3903</v>
+        <v>3901</v>
       </c>
     </row>
     <row r="1306" spans="1:2">
       <c r="A1306" s="1" t="s">
-        <v>3904</v>
+        <v>3902</v>
       </c>
       <c r="B1306" t="s">
-        <v>3905</v>
+        <v>3903</v>
       </c>
     </row>
     <row r="1307" spans="1:2">
       <c r="A1307" s="1" t="s">
-        <v>3906</v>
+        <v>3904</v>
       </c>
       <c r="B1307" t="s">
-        <v>3907</v>
+        <v>3905</v>
       </c>
     </row>
     <row r="1308" spans="1:2">
       <c r="A1308" s="1" t="s">
-        <v>3908</v>
+        <v>3906</v>
       </c>
       <c r="B1308" t="s">
-        <v>3909</v>
+        <v>3907</v>
       </c>
     </row>
     <row r="1309" spans="1:2">
       <c r="A1309" s="1" t="s">
-        <v>3910</v>
+        <v>3908</v>
       </c>
       <c r="B1309" t="s">
-        <v>3911</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="1310" spans="1:2">
       <c r="A1310" s="1" t="s">
-        <v>3912</v>
+        <v>3910</v>
       </c>
       <c r="B1310" t="s">
-        <v>3909</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="1311" spans="1:2">
       <c r="A1311" s="1" t="s">
-        <v>3913</v>
+        <v>3912</v>
       </c>
       <c r="B1311" t="s">
-        <v>3914</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="1312" spans="1:2">
       <c r="A1312" s="1" t="s">
-        <v>3915</v>
+        <v>3913</v>
       </c>
       <c r="B1312" t="s">
-        <v>3916</v>
+        <v>3914</v>
       </c>
     </row>
     <row r="1313" spans="1:2">
       <c r="A1313" s="1" t="s">
-        <v>3917</v>
+        <v>3915</v>
       </c>
       <c r="B1313" t="s">
-        <v>3918</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="1314" spans="1:2">
       <c r="A1314" s="1" t="s">
-        <v>3919</v>
+        <v>3917</v>
       </c>
       <c r="B1314" t="s">
-        <v>3920</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="1315" spans="1:2">
       <c r="A1315" s="1" t="s">
-        <v>3921</v>
+        <v>3919</v>
       </c>
       <c r="B1315" t="s">
-        <v>3922</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="1316" spans="1:2">
       <c r="A1316" s="1" t="s">
-        <v>3923</v>
+        <v>3921</v>
       </c>
       <c r="B1316" t="s">
-        <v>3924</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="1317" spans="1:2">
       <c r="A1317" s="1" t="s">
-        <v>3925</v>
+        <v>3923</v>
       </c>
       <c r="B1317" t="s">
-        <v>3926</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="1318" spans="1:2">
       <c r="A1318" s="1" t="s">
-        <v>3927</v>
+        <v>3925</v>
       </c>
       <c r="B1318" t="s">
-        <v>3928</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="1319" spans="1:2">
       <c r="A1319" s="1" t="s">
-        <v>3929</v>
+        <v>3927</v>
       </c>
       <c r="B1319" t="s">
-        <v>3930</v>
+        <v>3928</v>
       </c>
     </row>
     <row r="1320" spans="1:2">
       <c r="A1320" s="1" t="s">
-        <v>3931</v>
+        <v>3929</v>
       </c>
       <c r="B1320" t="s">
-        <v>3932</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="1321" spans="1:2">
       <c r="A1321" s="1" t="s">
-        <v>3933</v>
+        <v>3931</v>
       </c>
       <c r="B1321" t="s">
-        <v>3934</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1322" spans="1:2">
       <c r="A1322" s="1" t="s">
-        <v>3935</v>
+        <v>3933</v>
       </c>
       <c r="B1322" t="s">
-        <v>3936</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="1323" spans="1:2">
       <c r="A1323" s="1" t="s">
-        <v>3937</v>
+        <v>3935</v>
       </c>
       <c r="B1323" t="s">
-        <v>3938</v>
+        <v>3936</v>
       </c>
     </row>
     <row r="1324" spans="1:2">
       <c r="A1324" s="1" t="s">
-        <v>3939</v>
+        <v>3937</v>
       </c>
       <c r="B1324" t="s">
-        <v>3940</v>
+        <v>3938</v>
       </c>
     </row>
     <row r="1325" spans="1:2">
       <c r="A1325" s="1" t="s">
-        <v>3941</v>
+        <v>3939</v>
       </c>
       <c r="B1325" t="s">
-        <v>3942</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="1326" spans="1:2">
       <c r="A1326" s="1" t="s">
-        <v>3943</v>
+        <v>3941</v>
       </c>
       <c r="B1326" t="s">
-        <v>3944</v>
+        <v>3942</v>
       </c>
     </row>
     <row r="1327" spans="1:2">
       <c r="A1327" s="1" t="s">
-        <v>3945</v>
+        <v>3943</v>
       </c>
       <c r="B1327" t="s">
-        <v>3946</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="1328" spans="1:2">
       <c r="A1328" s="1" t="s">
-        <v>3947</v>
+        <v>3945</v>
       </c>
       <c r="B1328" t="s">
-        <v>3948</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="1329" spans="1:2">
       <c r="A1329" s="1" t="s">
-        <v>3949</v>
+        <v>3947</v>
       </c>
       <c r="B1329" t="s">
-        <v>3950</v>
+        <v>3948</v>
       </c>
     </row>
     <row r="1330" spans="1:2">
       <c r="A1330" s="1" t="s">
-        <v>3951</v>
+        <v>3949</v>
       </c>
       <c r="B1330" t="s">
-        <v>3952</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="1331" spans="1:2">
       <c r="A1331" s="1" t="s">
-        <v>3953</v>
+        <v>3951</v>
       </c>
       <c r="B1331" t="s">
-        <v>3954</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="1332" spans="1:2">
       <c r="A1332" s="1" t="s">
-        <v>3955</v>
+        <v>3953</v>
       </c>
       <c r="B1332" t="s">
-        <v>3942</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1333" spans="1:2">
       <c r="A1333" s="1" t="s">
-        <v>3956</v>
+        <v>3955</v>
       </c>
       <c r="B1333" t="s">
-        <v>3957</v>
+        <v>3942</v>
       </c>
     </row>
     <row r="1334" spans="1:2">
       <c r="A1334" s="1" t="s">
-        <v>3958</v>
+        <v>3956</v>
       </c>
       <c r="B1334" t="s">
-        <v>3959</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="1335" spans="1:2">
       <c r="A1335" s="1" t="s">
-        <v>3960</v>
+        <v>3958</v>
       </c>
       <c r="B1335" t="s">
-        <v>3961</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1336" spans="1:2">
       <c r="A1336" s="1" t="s">
-        <v>3962</v>
+        <v>3960</v>
       </c>
       <c r="B1336" t="s">
-        <v>3963</v>
+        <v>3961</v>
       </c>
     </row>
     <row r="1337" spans="1:2">
       <c r="A1337" s="1" t="s">
-        <v>3964</v>
+        <v>3962</v>
       </c>
       <c r="B1337" t="s">
-        <v>3848</v>
+        <v>3963</v>
       </c>
     </row>
     <row r="1338" spans="1:2">
       <c r="A1338" s="1" t="s">
-        <v>3965</v>
+        <v>3964</v>
       </c>
       <c r="B1338" t="s">
-        <v>3966</v>
+        <v>3848</v>
       </c>
     </row>
     <row r="1339" spans="1:2">
       <c r="A1339" s="1" t="s">
-        <v>3967</v>
+        <v>3965</v>
       </c>
       <c r="B1339" t="s">
-        <v>3968</v>
+        <v>3966</v>
       </c>
     </row>
     <row r="1340" spans="1:2">
       <c r="A1340" s="1" t="s">
-        <v>3969</v>
+        <v>3967</v>
       </c>
       <c r="B1340" t="s">
-        <v>3970</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="1341" spans="1:2">
       <c r="A1341" s="1" t="s">
-        <v>3971</v>
+        <v>3969</v>
       </c>
       <c r="B1341" t="s">
-        <v>3972</v>
+        <v>3970</v>
       </c>
     </row>
     <row r="1342" spans="1:2">
       <c r="A1342" s="1" t="s">
-        <v>3973</v>
+        <v>3971</v>
       </c>
       <c r="B1342" t="s">
-        <v>3974</v>
+        <v>3972</v>
       </c>
     </row>
     <row r="1343" spans="1:2">
       <c r="A1343" s="1" t="s">
-        <v>3975</v>
+        <v>3973</v>
       </c>
       <c r="B1343" t="s">
-        <v>3976</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="1344" spans="1:2">
       <c r="A1344" s="1" t="s">
-        <v>3977</v>
+        <v>3975</v>
       </c>
       <c r="B1344" t="s">
-        <v>3978</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1345" spans="1:2">
       <c r="A1345" s="1" t="s">
-        <v>3979</v>
+        <v>3977</v>
       </c>
       <c r="B1345" t="s">
-        <v>3980</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="1346" spans="1:2">
       <c r="A1346" s="1" t="s">
-        <v>3981</v>
+        <v>3979</v>
       </c>
       <c r="B1346" t="s">
-        <v>3982</v>
+        <v>3980</v>
       </c>
     </row>
     <row r="1347" spans="1:2">
       <c r="A1347" s="1" t="s">
-        <v>3983</v>
+        <v>3981</v>
       </c>
       <c r="B1347" t="s">
-        <v>3984</v>
+        <v>3982</v>
       </c>
     </row>
     <row r="1348" spans="1:2">
       <c r="A1348" s="1" t="s">
-        <v>3985</v>
+        <v>3983</v>
       </c>
       <c r="B1348" t="s">
-        <v>3986</v>
+        <v>3984</v>
       </c>
     </row>
     <row r="1349" spans="1:2">
       <c r="A1349" s="1" t="s">
-        <v>3987</v>
+        <v>3985</v>
       </c>
       <c r="B1349" t="s">
-        <v>3988</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1350" spans="1:2">
       <c r="A1350" s="1" t="s">
-        <v>3989</v>
+        <v>3987</v>
       </c>
       <c r="B1350" t="s">
-        <v>3990</v>
+        <v>3988</v>
       </c>
     </row>
     <row r="1351" spans="1:2">
       <c r="A1351" s="1" t="s">
-        <v>3991</v>
+        <v>3989</v>
       </c>
       <c r="B1351" t="s">
-        <v>3992</v>
+        <v>3990</v>
       </c>
     </row>
     <row r="1352" spans="1:2">
       <c r="A1352" s="1" t="s">
-        <v>3993</v>
+        <v>3991</v>
       </c>
       <c r="B1352" t="s">
-        <v>3994</v>
+        <v>3992</v>
       </c>
     </row>
     <row r="1353" spans="1:2">
       <c r="A1353" s="1" t="s">
-        <v>3995</v>
+        <v>3993</v>
       </c>
       <c r="B1353" t="s">
-        <v>3996</v>
+        <v>3994</v>
       </c>
     </row>
     <row r="1354" spans="1:2">
       <c r="A1354" s="1" t="s">
-        <v>3997</v>
+        <v>3995</v>
       </c>
       <c r="B1354" t="s">
-        <v>3998</v>
+        <v>3996</v>
       </c>
     </row>
     <row r="1355" spans="1:2">
       <c r="A1355" s="1" t="s">
-        <v>3999</v>
+        <v>3997</v>
       </c>
       <c r="B1355" t="s">
-        <v>4000</v>
+        <v>3998</v>
       </c>
     </row>
     <row r="1356" spans="1:2">
       <c r="A1356" s="1" t="s">
-        <v>4001</v>
+        <v>3999</v>
       </c>
       <c r="B1356" t="s">
-        <v>4002</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1357" spans="1:2">
       <c r="A1357" s="1" t="s">
-        <v>4003</v>
+        <v>4001</v>
       </c>
       <c r="B1357" t="s">
-        <v>4004</v>
+        <v>4002</v>
       </c>
     </row>
     <row r="1358" spans="1:2">
       <c r="A1358" s="1" t="s">
-        <v>4005</v>
+        <v>4003</v>
       </c>
       <c r="B1358" t="s">
-        <v>4006</v>
+        <v>4004</v>
       </c>
     </row>
     <row r="1359" spans="1:2">
       <c r="A1359" s="1" t="s">
-        <v>4007</v>
+        <v>4005</v>
       </c>
       <c r="B1359" t="s">
-        <v>4008</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="1360" spans="1:2">
       <c r="A1360" s="1" t="s">
-        <v>4009</v>
+        <v>4007</v>
       </c>
       <c r="B1360" t="s">
-        <v>4010</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="1361" spans="1:2">
       <c r="A1361" s="1" t="s">
-        <v>4011</v>
+        <v>4009</v>
       </c>
       <c r="B1361" t="s">
-        <v>4012</v>
+        <v>4010</v>
       </c>
     </row>
     <row r="1362" spans="1:2">
       <c r="A1362" s="1" t="s">
-        <v>4013</v>
+        <v>4011</v>
       </c>
       <c r="B1362" t="s">
-        <v>4014</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="1363" spans="1:2">
       <c r="A1363" s="1" t="s">
-        <v>4015</v>
+        <v>4013</v>
       </c>
       <c r="B1363" t="s">
-        <v>4016</v>
+        <v>4014</v>
       </c>
     </row>
     <row r="1364" spans="1:2">
       <c r="A1364" s="1" t="s">
-        <v>4453</v>
+        <v>4015</v>
       </c>
       <c r="B1364" t="s">
-        <v>4454</v>
+        <v>4016</v>
       </c>
     </row>
     <row r="1365" spans="1:2">
       <c r="A1365" s="1" t="s">
-        <v>4017</v>
+        <v>4453</v>
       </c>
       <c r="B1365" t="s">
-        <v>4018</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="1366" spans="1:2">
       <c r="A1366" s="1" t="s">
-        <v>4019</v>
+        <v>4017</v>
       </c>
       <c r="B1366" t="s">
-        <v>4020</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="1367" spans="1:2">
       <c r="A1367" s="1" t="s">
-        <v>4021</v>
+        <v>4019</v>
       </c>
       <c r="B1367" t="s">
-        <v>4022</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1368" spans="1:2">
       <c r="A1368" s="1" t="s">
-        <v>4023</v>
+        <v>4021</v>
       </c>
       <c r="B1368" t="s">
-        <v>4024</v>
+        <v>4022</v>
       </c>
     </row>
     <row r="1369" spans="1:2">
       <c r="A1369" s="1" t="s">
-        <v>4025</v>
+        <v>4023</v>
       </c>
       <c r="B1369" t="s">
-        <v>4026</v>
+        <v>4024</v>
       </c>
     </row>
     <row r="1370" spans="1:2">
       <c r="A1370" s="1" t="s">
-        <v>4027</v>
+        <v>4025</v>
       </c>
       <c r="B1370" t="s">
-        <v>4028</v>
+        <v>4026</v>
       </c>
     </row>
     <row r="1371" spans="1:2">
       <c r="A1371" s="1" t="s">
-        <v>4029</v>
+        <v>4027</v>
       </c>
       <c r="B1371" t="s">
-        <v>4030</v>
+        <v>4028</v>
       </c>
     </row>
     <row r="1372" spans="1:2">
       <c r="A1372" s="1" t="s">
-        <v>4031</v>
+        <v>4029</v>
       </c>
       <c r="B1372" t="s">
-        <v>4032</v>
+        <v>4030</v>
       </c>
     </row>
     <row r="1373" spans="1:2">
       <c r="A1373" s="1" t="s">
-        <v>4033</v>
+        <v>4031</v>
       </c>
       <c r="B1373" t="s">
-        <v>4034</v>
+        <v>4032</v>
       </c>
     </row>
     <row r="1374" spans="1:2">
       <c r="A1374" s="1" t="s">
-        <v>4035</v>
+        <v>4033</v>
       </c>
       <c r="B1374" t="s">
-        <v>4036</v>
+        <v>4034</v>
       </c>
     </row>
     <row r="1375" spans="1:2">
       <c r="A1375" s="1" t="s">
-        <v>4037</v>
+        <v>4035</v>
       </c>
       <c r="B1375" t="s">
-        <v>4038</v>
+        <v>4036</v>
       </c>
     </row>
     <row r="1376" spans="1:2">
       <c r="A1376" s="1" t="s">
-        <v>4039</v>
+        <v>4037</v>
       </c>
       <c r="B1376" t="s">
-        <v>4040</v>
+        <v>4038</v>
       </c>
     </row>
     <row r="1377" spans="1:2">
       <c r="A1377" s="1" t="s">
-        <v>4041</v>
+        <v>4039</v>
       </c>
       <c r="B1377" t="s">
-        <v>4042</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1378" spans="1:2">
       <c r="A1378" s="1" t="s">
-        <v>4043</v>
+        <v>4041</v>
       </c>
       <c r="B1378" t="s">
-        <v>4044</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="1379" spans="1:2">
       <c r="A1379" s="1" t="s">
-        <v>4045</v>
+        <v>4043</v>
       </c>
       <c r="B1379" t="s">
-        <v>4046</v>
+        <v>4044</v>
       </c>
     </row>
     <row r="1380" spans="1:2">
       <c r="A1380" s="1" t="s">
-        <v>4047</v>
+        <v>4045</v>
       </c>
       <c r="B1380" t="s">
-        <v>4048</v>
+        <v>4046</v>
       </c>
     </row>
     <row r="1381" spans="1:2">
       <c r="A1381" s="1" t="s">
-        <v>4049</v>
+        <v>4047</v>
       </c>
       <c r="B1381" t="s">
-        <v>4050</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1382" spans="1:2">
       <c r="A1382" s="1" t="s">
-        <v>4051</v>
+        <v>4049</v>
       </c>
       <c r="B1382" t="s">
-        <v>4052</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="1383" spans="1:2">
       <c r="A1383" s="1" t="s">
-        <v>4053</v>
+        <v>4051</v>
       </c>
       <c r="B1383" t="s">
-        <v>4054</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="1384" spans="1:2">
       <c r="A1384" s="1" t="s">
-        <v>4055</v>
+        <v>4053</v>
       </c>
       <c r="B1384" t="s">
-        <v>4056</v>
+        <v>4054</v>
       </c>
     </row>
     <row r="1385" spans="1:2">
       <c r="A1385" s="1" t="s">
-        <v>4057</v>
+        <v>4055</v>
       </c>
       <c r="B1385" t="s">
-        <v>4058</v>
+        <v>4056</v>
       </c>
     </row>
     <row r="1386" spans="1:2">
       <c r="A1386" s="1" t="s">
-        <v>4059</v>
+        <v>4057</v>
       </c>
       <c r="B1386" t="s">
-        <v>4060</v>
+        <v>4058</v>
       </c>
     </row>
     <row r="1387" spans="1:2">
       <c r="A1387" s="1" t="s">
-        <v>4061</v>
+        <v>4059</v>
       </c>
       <c r="B1387" t="s">
-        <v>4062</v>
+        <v>4060</v>
       </c>
     </row>
     <row r="1388" spans="1:2">
       <c r="A1388" s="1" t="s">
-        <v>4063</v>
+        <v>4061</v>
       </c>
       <c r="B1388" t="s">
-        <v>4064</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="1389" spans="1:2">
       <c r="A1389" s="1" t="s">
-        <v>4065</v>
+        <v>4063</v>
       </c>
       <c r="B1389" t="s">
-        <v>4066</v>
+        <v>4064</v>
       </c>
     </row>
     <row r="1390" spans="1:2">
       <c r="A1390" s="1" t="s">
-        <v>4067</v>
+        <v>4065</v>
       </c>
       <c r="B1390" t="s">
-        <v>4068</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="1391" spans="1:2">
       <c r="A1391" s="1" t="s">
-        <v>4069</v>
+        <v>4067</v>
       </c>
       <c r="B1391" t="s">
-        <v>4070</v>
+        <v>4068</v>
       </c>
     </row>
     <row r="1392" spans="1:2">
       <c r="A1392" s="1" t="s">
-        <v>4071</v>
+        <v>4069</v>
       </c>
       <c r="B1392" t="s">
-        <v>4072</v>
+        <v>4070</v>
       </c>
     </row>
     <row r="1393" spans="1:2">
       <c r="A1393" s="1" t="s">
-        <v>4073</v>
+        <v>4071</v>
       </c>
       <c r="B1393" t="s">
-        <v>4074</v>
+        <v>4072</v>
       </c>
     </row>
     <row r="1394" spans="1:2">
       <c r="A1394" s="1" t="s">
-        <v>4075</v>
+        <v>4073</v>
       </c>
       <c r="B1394" t="s">
-        <v>4076</v>
+        <v>4074</v>
       </c>
     </row>
     <row r="1395" spans="1:2">
       <c r="A1395" s="1" t="s">
-        <v>4077</v>
+        <v>4075</v>
       </c>
       <c r="B1395" t="s">
-        <v>4078</v>
+        <v>4076</v>
       </c>
     </row>
     <row r="1396" spans="1:2">
       <c r="A1396" s="1" t="s">
-        <v>4079</v>
+        <v>4077</v>
       </c>
       <c r="B1396" t="s">
-        <v>4080</v>
+        <v>4078</v>
       </c>
     </row>
     <row r="1397" spans="1:2">
       <c r="A1397" s="1" t="s">
-        <v>4081</v>
+        <v>4079</v>
       </c>
       <c r="B1397" t="s">
-        <v>4082</v>
+        <v>4080</v>
       </c>
     </row>
     <row r="1398" spans="1:2">
       <c r="A1398" s="1" t="s">
-        <v>4083</v>
+        <v>4081</v>
       </c>
       <c r="B1398" t="s">
-        <v>4084</v>
+        <v>4082</v>
       </c>
     </row>
     <row r="1399" spans="1:2">
       <c r="A1399" s="1" t="s">
-        <v>4085</v>
+        <v>4083</v>
       </c>
       <c r="B1399" t="s">
-        <v>4086</v>
+        <v>4084</v>
       </c>
     </row>
     <row r="1400" spans="1:2">
       <c r="A1400" s="1" t="s">
-        <v>4087</v>
+        <v>4085</v>
       </c>
       <c r="B1400" t="s">
-        <v>4088</v>
+        <v>4086</v>
       </c>
     </row>
     <row r="1401" spans="1:2">
       <c r="A1401" s="1" t="s">
-        <v>4089</v>
+        <v>4087</v>
       </c>
       <c r="B1401" t="s">
-        <v>4090</v>
+        <v>4088</v>
       </c>
     </row>
     <row r="1402" spans="1:2">
       <c r="A1402" s="1" t="s">
-        <v>4091</v>
+        <v>4089</v>
       </c>
       <c r="B1402" t="s">
-        <v>4092</v>
+        <v>4090</v>
       </c>
     </row>
     <row r="1403" spans="1:2">
       <c r="A1403" s="1" t="s">
-        <v>4093</v>
+        <v>4091</v>
       </c>
       <c r="B1403" t="s">
-        <v>4094</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="1404" spans="1:2">
       <c r="A1404" s="1" t="s">
-        <v>4095</v>
+        <v>4093</v>
       </c>
       <c r="B1404" t="s">
-        <v>4096</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="1405" spans="1:2">
       <c r="A1405" s="1" t="s">
-        <v>4097</v>
+        <v>4095</v>
       </c>
       <c r="B1405" t="s">
-        <v>4098</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="1406" spans="1:2">
       <c r="A1406" s="1" t="s">
-        <v>4099</v>
+        <v>4097</v>
       </c>
       <c r="B1406" t="s">
-        <v>4100</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="1407" spans="1:2">
       <c r="A1407" s="1" t="s">
-        <v>4101</v>
+        <v>4099</v>
       </c>
       <c r="B1407" t="s">
-        <v>4102</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="1408" spans="1:2">
       <c r="A1408" s="1" t="s">
-        <v>4103</v>
+        <v>4101</v>
       </c>
       <c r="B1408" t="s">
-        <v>4104</v>
+        <v>4102</v>
       </c>
     </row>
     <row r="1409" spans="1:2">
       <c r="A1409" s="1" t="s">
-        <v>4105</v>
+        <v>4103</v>
       </c>
       <c r="B1409" t="s">
-        <v>4106</v>
+        <v>4104</v>
       </c>
     </row>
     <row r="1410" spans="1:2">
       <c r="A1410" s="1" t="s">
-        <v>4107</v>
+        <v>4105</v>
       </c>
       <c r="B1410" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="1411" spans="1:2">
       <c r="A1411" s="1" t="s">
-        <v>4109</v>
+        <v>4107</v>
       </c>
       <c r="B1411" t="s">
-        <v>4110</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="1412" spans="1:2">
       <c r="A1412" s="1" t="s">
-        <v>4111</v>
+        <v>4109</v>
       </c>
       <c r="B1412" t="s">
-        <v>4112</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="1413" spans="1:2">
       <c r="A1413" s="1" t="s">
-        <v>4113</v>
+        <v>4111</v>
       </c>
       <c r="B1413" t="s">
-        <v>4114</v>
+        <v>4112</v>
       </c>
     </row>
     <row r="1414" spans="1:2">
       <c r="A1414" s="1" t="s">
-        <v>4115</v>
+        <v>4113</v>
       </c>
       <c r="B1414" t="s">
-        <v>4116</v>
+        <v>4114</v>
       </c>
     </row>
     <row r="1415" spans="1:2">
       <c r="A1415" s="1" t="s">
-        <v>4117</v>
+        <v>4115</v>
       </c>
       <c r="B1415" t="s">
-        <v>4118</v>
+        <v>4116</v>
       </c>
     </row>
     <row r="1416" spans="1:2">
       <c r="A1416" s="1" t="s">
-        <v>4119</v>
+        <v>4117</v>
       </c>
       <c r="B1416" t="s">
-        <v>4120</v>
+        <v>4118</v>
       </c>
     </row>
     <row r="1417" spans="1:2">
       <c r="A1417" s="1" t="s">
-        <v>4121</v>
+        <v>4119</v>
       </c>
       <c r="B1417" t="s">
-        <v>4122</v>
+        <v>4120</v>
       </c>
     </row>
     <row r="1418" spans="1:2">
       <c r="A1418" s="1" t="s">
-        <v>4123</v>
+        <v>4121</v>
       </c>
       <c r="B1418" t="s">
-        <v>4124</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="1419" spans="1:2">
       <c r="A1419" s="1" t="s">
-        <v>4125</v>
+        <v>4123</v>
       </c>
       <c r="B1419" t="s">
-        <v>4126</v>
+        <v>4124</v>
       </c>
     </row>
     <row r="1420" spans="1:2">
       <c r="A1420" s="1" t="s">
-        <v>4127</v>
+        <v>4125</v>
       </c>
       <c r="B1420" t="s">
-        <v>4128</v>
+        <v>4126</v>
       </c>
     </row>
     <row r="1421" spans="1:2">
       <c r="A1421" s="1" t="s">
-        <v>4129</v>
+        <v>4127</v>
       </c>
       <c r="B1421" t="s">
-        <v>4130</v>
+        <v>4128</v>
       </c>
     </row>
     <row r="1422" spans="1:2">
       <c r="A1422" s="1" t="s">
-        <v>4131</v>
+        <v>4129</v>
       </c>
       <c r="B1422" t="s">
-        <v>4132</v>
+        <v>4130</v>
       </c>
     </row>
     <row r="1423" spans="1:2">
       <c r="A1423" s="1" t="s">
-        <v>4133</v>
+        <v>4131</v>
       </c>
       <c r="B1423" t="s">
-        <v>4134</v>
+        <v>4132</v>
       </c>
     </row>
     <row r="1424" spans="1:2">
       <c r="A1424" s="1" t="s">
-        <v>4135</v>
+        <v>4133</v>
       </c>
       <c r="B1424" t="s">
-        <v>4136</v>
+        <v>4134</v>
       </c>
     </row>
     <row r="1425" spans="1:2">
       <c r="A1425" s="1" t="s">
-        <v>4137</v>
+        <v>4135</v>
       </c>
       <c r="B1425" t="s">
-        <v>4138</v>
+        <v>4136</v>
       </c>
     </row>
     <row r="1426" spans="1:2">
       <c r="A1426" s="1" t="s">
-        <v>4139</v>
+        <v>4137</v>
       </c>
       <c r="B1426" t="s">
-        <v>4140</v>
+        <v>4138</v>
       </c>
     </row>
     <row r="1427" spans="1:2">
       <c r="A1427" s="1" t="s">
-        <v>4141</v>
+        <v>4139</v>
       </c>
       <c r="B1427" t="s">
-        <v>4142</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="1428" spans="1:2">
       <c r="A1428" s="1" t="s">
-        <v>4143</v>
+        <v>4141</v>
       </c>
       <c r="B1428" t="s">
-        <v>4144</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="1429" spans="1:2">
       <c r="A1429" s="1" t="s">
-        <v>4423</v>
+        <v>4143</v>
       </c>
       <c r="B1429" t="s">
-        <v>4424</v>
+        <v>4144</v>
       </c>
     </row>
     <row r="1430" spans="1:2">
       <c r="A1430" s="1" t="s">
-        <v>4145</v>
+        <v>4423</v>
       </c>
       <c r="B1430" t="s">
-        <v>4146</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="1431" spans="1:2">
       <c r="A1431" s="1" t="s">
-        <v>4147</v>
+        <v>4145</v>
       </c>
       <c r="B1431" t="s">
-        <v>4148</v>
+        <v>4146</v>
       </c>
     </row>
     <row r="1432" spans="1:2">
       <c r="A1432" s="1" t="s">
-        <v>4149</v>
+        <v>4147</v>
       </c>
       <c r="B1432" t="s">
-        <v>4150</v>
+        <v>4148</v>
       </c>
     </row>
     <row r="1433" spans="1:2">
       <c r="A1433" s="1" t="s">
-        <v>4151</v>
+        <v>4149</v>
       </c>
       <c r="B1433" t="s">
-        <v>4152</v>
+        <v>4150</v>
       </c>
     </row>
     <row r="1434" spans="1:2">
       <c r="A1434" s="1" t="s">
-        <v>4153</v>
+        <v>4151</v>
       </c>
       <c r="B1434" t="s">
-        <v>4154</v>
+        <v>4152</v>
       </c>
     </row>
     <row r="1435" spans="1:2">
       <c r="A1435" s="1" t="s">
-        <v>4155</v>
+        <v>4153</v>
       </c>
       <c r="B1435" t="s">
-        <v>4156</v>
+        <v>4154</v>
       </c>
     </row>
     <row r="1436" spans="1:2">
       <c r="A1436" s="1" t="s">
-        <v>4157</v>
+        <v>4155</v>
       </c>
       <c r="B1436" t="s">
-        <v>4158</v>
+        <v>4156</v>
       </c>
     </row>
     <row r="1437" spans="1:2">
       <c r="A1437" s="1" t="s">
-        <v>4159</v>
+        <v>4157</v>
       </c>
       <c r="B1437" t="s">
-        <v>4160</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="1438" spans="1:2">
       <c r="A1438" s="1" t="s">
-        <v>4161</v>
+        <v>4159</v>
       </c>
       <c r="B1438" t="s">
-        <v>4162</v>
+        <v>4160</v>
       </c>
     </row>
     <row r="1439" spans="1:2">
       <c r="A1439" s="1" t="s">
-        <v>4163</v>
+        <v>4457</v>
       </c>
       <c r="B1439" t="s">
-        <v>4164</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="1440" spans="1:2">
       <c r="A1440" s="1" t="s">
-        <v>4165</v>
+        <v>4459</v>
       </c>
       <c r="B1440" t="s">
-        <v>4166</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="1441" spans="1:2">
       <c r="A1441" s="1" t="s">
-        <v>4167</v>
+        <v>4161</v>
       </c>
       <c r="B1441" t="s">
-        <v>4168</v>
+        <v>4162</v>
       </c>
     </row>
     <row r="1442" spans="1:2">
       <c r="A1442" s="1" t="s">
-        <v>4169</v>
+        <v>4163</v>
       </c>
       <c r="B1442" t="s">
-        <v>4170</v>
+        <v>4164</v>
       </c>
     </row>
     <row r="1443" spans="1:2">
       <c r="A1443" s="1" t="s">
-        <v>4171</v>
+        <v>4165</v>
       </c>
       <c r="B1443" t="s">
-        <v>4172</v>
+        <v>4166</v>
       </c>
     </row>
     <row r="1444" spans="1:2">
       <c r="A1444" s="1" t="s">
-        <v>4173</v>
+        <v>4167</v>
       </c>
       <c r="B1444" t="s">
-        <v>4174</v>
+        <v>4168</v>
       </c>
     </row>
     <row r="1445" spans="1:2">
       <c r="A1445" s="1" t="s">
-        <v>4175</v>
+        <v>4169</v>
       </c>
       <c r="B1445" t="s">
-        <v>4176</v>
+        <v>4170</v>
       </c>
     </row>
     <row r="1446" spans="1:2">
       <c r="A1446" s="1" t="s">
-        <v>4452</v>
+        <v>4171</v>
       </c>
       <c r="B1446" t="s">
-        <v>4451</v>
+        <v>4172</v>
       </c>
     </row>
     <row r="1447" spans="1:2">
       <c r="A1447" s="1" t="s">
-        <v>4177</v>
+        <v>4173</v>
       </c>
       <c r="B1447" t="s">
-        <v>4178</v>
+        <v>4174</v>
       </c>
     </row>
     <row r="1448" spans="1:2">
       <c r="A1448" s="1" t="s">
-        <v>4179</v>
+        <v>4175</v>
       </c>
       <c r="B1448" t="s">
-        <v>4180</v>
+        <v>4176</v>
       </c>
     </row>
     <row r="1449" spans="1:2">
       <c r="A1449" s="1" t="s">
-        <v>4181</v>
+        <v>4452</v>
       </c>
       <c r="B1449" t="s">
-        <v>4182</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="1450" spans="1:2">
       <c r="A1450" s="1" t="s">
-        <v>4183</v>
+        <v>4177</v>
       </c>
       <c r="B1450" t="s">
-        <v>4184</v>
+        <v>4178</v>
       </c>
     </row>
     <row r="1451" spans="1:2">
       <c r="A1451" s="1" t="s">
-        <v>4185</v>
+        <v>4179</v>
       </c>
       <c r="B1451" t="s">
-        <v>4186</v>
+        <v>4180</v>
       </c>
     </row>
     <row r="1452" spans="1:2">
       <c r="A1452" s="1" t="s">
-        <v>4187</v>
+        <v>4181</v>
       </c>
       <c r="B1452" t="s">
-        <v>4188</v>
+        <v>4182</v>
       </c>
     </row>
     <row r="1453" spans="1:2">
       <c r="A1453" s="1" t="s">
-        <v>4189</v>
+        <v>4183</v>
       </c>
       <c r="B1453" t="s">
-        <v>4190</v>
+        <v>4184</v>
       </c>
     </row>
     <row r="1454" spans="1:2">
       <c r="A1454" s="1" t="s">
-        <v>4191</v>
+        <v>4185</v>
       </c>
       <c r="B1454" t="s">
-        <v>4192</v>
+        <v>4186</v>
       </c>
     </row>
     <row r="1455" spans="1:2">
       <c r="A1455" s="1" t="s">
-        <v>4193</v>
+        <v>4187</v>
       </c>
       <c r="B1455" t="s">
-        <v>4194</v>
+        <v>4188</v>
       </c>
     </row>
     <row r="1456" spans="1:2">
       <c r="A1456" s="1" t="s">
-        <v>4195</v>
+        <v>4189</v>
       </c>
       <c r="B1456" t="s">
-        <v>4196</v>
+        <v>4190</v>
       </c>
     </row>
     <row r="1457" spans="1:2">
       <c r="A1457" s="1" t="s">
-        <v>4197</v>
+        <v>4191</v>
       </c>
       <c r="B1457" t="s">
-        <v>4198</v>
+        <v>4192</v>
       </c>
     </row>
     <row r="1458" spans="1:2">
       <c r="A1458" s="1" t="s">
-        <v>4199</v>
+        <v>4193</v>
       </c>
       <c r="B1458" t="s">
-        <v>4200</v>
+        <v>4194</v>
       </c>
     </row>
     <row r="1459" spans="1:2">
       <c r="A1459" s="1" t="s">
-        <v>4201</v>
+        <v>4195</v>
       </c>
       <c r="B1459" t="s">
-        <v>4202</v>
+        <v>4196</v>
       </c>
     </row>
     <row r="1460" spans="1:2">
       <c r="A1460" s="1" t="s">
-        <v>4203</v>
+        <v>4197</v>
       </c>
       <c r="B1460" t="s">
-        <v>4204</v>
+        <v>4198</v>
       </c>
     </row>
     <row r="1461" spans="1:2">
       <c r="A1461" s="1" t="s">
-        <v>4205</v>
+        <v>4199</v>
       </c>
       <c r="B1461" t="s">
-        <v>4206</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="1462" spans="1:2">
       <c r="A1462" s="1" t="s">
-        <v>4207</v>
+        <v>4201</v>
       </c>
       <c r="B1462" t="s">
-        <v>4208</v>
+        <v>4202</v>
       </c>
     </row>
     <row r="1463" spans="1:2">
       <c r="A1463" s="1" t="s">
-        <v>4209</v>
+        <v>4203</v>
       </c>
       <c r="B1463" t="s">
-        <v>4210</v>
+        <v>4204</v>
       </c>
     </row>
     <row r="1464" spans="1:2">
       <c r="A1464" s="1" t="s">
-        <v>4211</v>
+        <v>4205</v>
       </c>
       <c r="B1464" t="s">
-        <v>4212</v>
+        <v>4206</v>
       </c>
     </row>
     <row r="1465" spans="1:2">
       <c r="A1465" s="1" t="s">
-        <v>4213</v>
+        <v>4207</v>
       </c>
       <c r="B1465" t="s">
-        <v>4214</v>
+        <v>4208</v>
       </c>
     </row>
     <row r="1466" spans="1:2">
       <c r="A1466" s="1" t="s">
-        <v>4215</v>
+        <v>4209</v>
       </c>
       <c r="B1466" t="s">
-        <v>4216</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="1467" spans="1:2">
       <c r="A1467" s="1" t="s">
-        <v>4217</v>
+        <v>4211</v>
       </c>
       <c r="B1467" t="s">
-        <v>4218</v>
+        <v>4212</v>
       </c>
     </row>
     <row r="1468" spans="1:2">
       <c r="A1468" s="1" t="s">
-        <v>4219</v>
+        <v>4213</v>
       </c>
       <c r="B1468" t="s">
-        <v>4220</v>
+        <v>4214</v>
       </c>
     </row>
     <row r="1469" spans="1:2">
       <c r="A1469" s="1" t="s">
-        <v>4221</v>
+        <v>4215</v>
       </c>
       <c r="B1469" t="s">
-        <v>4222</v>
+        <v>4216</v>
       </c>
     </row>
     <row r="1470" spans="1:2">
       <c r="A1470" s="1" t="s">
-        <v>4223</v>
+        <v>4217</v>
       </c>
       <c r="B1470" t="s">
-        <v>4224</v>
+        <v>4218</v>
       </c>
     </row>
     <row r="1471" spans="1:2">
       <c r="A1471" s="1" t="s">
-        <v>4225</v>
+        <v>4219</v>
       </c>
       <c r="B1471" t="s">
-        <v>4226</v>
+        <v>4220</v>
       </c>
     </row>
     <row r="1472" spans="1:2">
       <c r="A1472" s="1" t="s">
-        <v>4227</v>
+        <v>4221</v>
       </c>
       <c r="B1472" t="s">
-        <v>4228</v>
+        <v>4222</v>
       </c>
     </row>
     <row r="1473" spans="1:2">
       <c r="A1473" s="1" t="s">
-        <v>4229</v>
+        <v>4223</v>
       </c>
       <c r="B1473" t="s">
-        <v>4230</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="1474" spans="1:2">
       <c r="A1474" s="1" t="s">
-        <v>4231</v>
+        <v>4225</v>
       </c>
       <c r="B1474" t="s">
-        <v>4232</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="1475" spans="1:2">
       <c r="A1475" s="1" t="s">
-        <v>4233</v>
+        <v>4227</v>
       </c>
       <c r="B1475" t="s">
-        <v>4234</v>
+        <v>4228</v>
       </c>
     </row>
     <row r="1476" spans="1:2">
       <c r="A1476" s="1" t="s">
-        <v>4235</v>
+        <v>4229</v>
       </c>
       <c r="B1476" t="s">
-        <v>4236</v>
+        <v>4230</v>
       </c>
     </row>
     <row r="1477" spans="1:2">
       <c r="A1477" s="1" t="s">
-        <v>4237</v>
+        <v>4231</v>
       </c>
       <c r="B1477" t="s">
-        <v>4238</v>
+        <v>4232</v>
       </c>
     </row>
     <row r="1478" spans="1:2">
       <c r="A1478" s="1" t="s">
-        <v>4239</v>
+        <v>4233</v>
       </c>
       <c r="B1478" t="s">
-        <v>4240</v>
+        <v>4234</v>
       </c>
     </row>
     <row r="1479" spans="1:2">
       <c r="A1479" s="1" t="s">
-        <v>4241</v>
+        <v>4235</v>
       </c>
       <c r="B1479" t="s">
-        <v>4242</v>
+        <v>4236</v>
       </c>
     </row>
     <row r="1480" spans="1:2">
       <c r="A1480" s="1" t="s">
-        <v>4243</v>
+        <v>4237</v>
       </c>
       <c r="B1480" t="s">
-        <v>4244</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="1481" spans="1:2">
       <c r="A1481" s="1" t="s">
-        <v>4245</v>
+        <v>4239</v>
       </c>
       <c r="B1481" t="s">
-        <v>4246</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="1482" spans="1:2">
       <c r="A1482" s="1" t="s">
-        <v>4247</v>
+        <v>4241</v>
       </c>
       <c r="B1482" t="s">
-        <v>4248</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="1483" spans="1:2">
       <c r="A1483" s="1" t="s">
-        <v>4249</v>
+        <v>4243</v>
       </c>
       <c r="B1483" t="s">
-        <v>4250</v>
+        <v>4244</v>
       </c>
     </row>
     <row r="1484" spans="1:2">
       <c r="A1484" s="1" t="s">
-        <v>4251</v>
+        <v>4245</v>
       </c>
       <c r="B1484" t="s">
-        <v>4252</v>
+        <v>4246</v>
       </c>
     </row>
     <row r="1485" spans="1:2">
       <c r="A1485" s="1" t="s">
-        <v>4253</v>
+        <v>4247</v>
       </c>
       <c r="B1485" t="s">
-        <v>4254</v>
+        <v>4248</v>
       </c>
     </row>
     <row r="1486" spans="1:2">
       <c r="A1486" s="1" t="s">
-        <v>4255</v>
+        <v>4249</v>
       </c>
       <c r="B1486" t="s">
-        <v>4256</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="1487" spans="1:2">
       <c r="A1487" s="1" t="s">
-        <v>4257</v>
+        <v>4251</v>
       </c>
       <c r="B1487" t="s">
-        <v>4258</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="1488" spans="1:2">
       <c r="A1488" s="1" t="s">
-        <v>4259</v>
+        <v>4253</v>
       </c>
       <c r="B1488" t="s">
-        <v>4260</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="1489" spans="1:2">
       <c r="A1489" s="1" t="s">
-        <v>4261</v>
+        <v>4255</v>
       </c>
       <c r="B1489" t="s">
-        <v>4262</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="1490" spans="1:2">
       <c r="A1490" s="1" t="s">
-        <v>4263</v>
+        <v>4257</v>
       </c>
       <c r="B1490" t="s">
-        <v>4264</v>
+        <v>4258</v>
       </c>
     </row>
     <row r="1491" spans="1:2">
       <c r="A1491" s="1" t="s">
-        <v>4265</v>
+        <v>4259</v>
       </c>
       <c r="B1491" t="s">
-        <v>4266</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="1492" spans="1:2">
       <c r="A1492" s="1" t="s">
-        <v>4267</v>
+        <v>4261</v>
       </c>
       <c r="B1492" t="s">
-        <v>4268</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="1493" spans="1:2">
       <c r="A1493" s="1" t="s">
-        <v>4269</v>
+        <v>4263</v>
       </c>
       <c r="B1493" t="s">
-        <v>4270</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="1494" spans="1:2">
       <c r="A1494" s="1" t="s">
-        <v>4271</v>
+        <v>4265</v>
       </c>
       <c r="B1494" t="s">
-        <v>4272</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="1495" spans="1:2">
       <c r="A1495" s="1" t="s">
-        <v>4273</v>
+        <v>4267</v>
       </c>
       <c r="B1495" t="s">
-        <v>4274</v>
+        <v>4268</v>
       </c>
     </row>
     <row r="1496" spans="1:2">
       <c r="A1496" s="1" t="s">
-        <v>4275</v>
+        <v>4269</v>
       </c>
       <c r="B1496" t="s">
-        <v>4276</v>
+        <v>4270</v>
       </c>
     </row>
     <row r="1497" spans="1:2">
       <c r="A1497" s="1" t="s">
-        <v>4277</v>
+        <v>4271</v>
       </c>
       <c r="B1497" t="s">
-        <v>4278</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="1498" spans="1:2">
       <c r="A1498" s="1" t="s">
-        <v>4279</v>
+        <v>4273</v>
       </c>
       <c r="B1498" t="s">
-        <v>4280</v>
+        <v>4274</v>
       </c>
     </row>
     <row r="1499" spans="1:2">
       <c r="A1499" s="1" t="s">
-        <v>4281</v>
+        <v>4275</v>
       </c>
       <c r="B1499" t="s">
-        <v>4282</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="1500" spans="1:2">
       <c r="A1500" s="1" t="s">
-        <v>4283</v>
+        <v>4277</v>
       </c>
       <c r="B1500" t="s">
-        <v>4284</v>
+        <v>4278</v>
       </c>
     </row>
     <row r="1501" spans="1:2">
       <c r="A1501" s="1" t="s">
-        <v>4285</v>
+        <v>4279</v>
       </c>
       <c r="B1501" t="s">
-        <v>4286</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="1502" spans="1:2">
       <c r="A1502" s="1" t="s">
-        <v>4287</v>
+        <v>4281</v>
       </c>
       <c r="B1502" t="s">
-        <v>4288</v>
+        <v>4282</v>
       </c>
     </row>
     <row r="1503" spans="1:2">
       <c r="A1503" s="1" t="s">
-        <v>4289</v>
+        <v>4283</v>
       </c>
       <c r="B1503" t="s">
-        <v>4290</v>
+        <v>4284</v>
       </c>
     </row>
     <row r="1504" spans="1:2">
       <c r="A1504" s="1" t="s">
-        <v>4291</v>
+        <v>4285</v>
       </c>
       <c r="B1504" t="s">
-        <v>4292</v>
+        <v>4286</v>
       </c>
     </row>
     <row r="1505" spans="1:2">
       <c r="A1505" s="1" t="s">
-        <v>4293</v>
+        <v>4287</v>
       </c>
       <c r="B1505" t="s">
-        <v>4294</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="1506" spans="1:2">
       <c r="A1506" s="1" t="s">
-        <v>4295</v>
+        <v>4289</v>
       </c>
       <c r="B1506" t="s">
-        <v>4296</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="1507" spans="1:2">
       <c r="A1507" s="1" t="s">
-        <v>4297</v>
+        <v>4291</v>
       </c>
       <c r="B1507" t="s">
-        <v>4298</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="1508" spans="1:2">
       <c r="A1508" s="1" t="s">
-        <v>4299</v>
+        <v>4293</v>
       </c>
       <c r="B1508" t="s">
-        <v>4300</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="1509" spans="1:2">
       <c r="A1509" s="1" t="s">
-        <v>4446</v>
+        <v>4295</v>
       </c>
       <c r="B1509" t="s">
-        <v>4447</v>
+        <v>4296</v>
       </c>
     </row>
     <row r="1510" spans="1:2">
       <c r="A1510" s="1" t="s">
-        <v>4431</v>
+        <v>4297</v>
       </c>
       <c r="B1510" t="s">
-        <v>4432</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="1511" spans="1:2">
       <c r="A1511" s="1" t="s">
-        <v>4301</v>
+        <v>4299</v>
       </c>
       <c r="B1511" t="s">
-        <v>4302</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="1512" spans="1:2">
       <c r="A1512" s="1" t="s">
-        <v>4303</v>
+        <v>4446</v>
       </c>
       <c r="B1512" t="s">
-        <v>4304</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="1513" spans="1:2">
       <c r="A1513" s="1" t="s">
-        <v>4305</v>
+        <v>4431</v>
       </c>
       <c r="B1513" t="s">
-        <v>4306</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="1514" spans="1:2">
       <c r="A1514" s="1" t="s">
-        <v>4307</v>
+        <v>4301</v>
       </c>
       <c r="B1514" t="s">
-        <v>4308</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="1515" spans="1:2">
       <c r="A1515" s="1" t="s">
-        <v>4309</v>
+        <v>4303</v>
       </c>
       <c r="B1515" t="s">
-        <v>4310</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="1516" spans="1:2">
       <c r="A1516" s="1" t="s">
-        <v>4311</v>
+        <v>4305</v>
       </c>
       <c r="B1516" t="s">
-        <v>4312</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="1517" spans="1:2">
       <c r="A1517" s="1" t="s">
-        <v>4313</v>
+        <v>4307</v>
       </c>
       <c r="B1517" t="s">
-        <v>4314</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="1518" spans="1:2">
       <c r="A1518" s="1" t="s">
-        <v>4315</v>
+        <v>4309</v>
       </c>
       <c r="B1518" t="s">
-        <v>4316</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="1519" spans="1:2">
       <c r="A1519" s="1" t="s">
-        <v>4317</v>
+        <v>4311</v>
       </c>
       <c r="B1519" t="s">
-        <v>4318</v>
+        <v>4312</v>
       </c>
     </row>
     <row r="1520" spans="1:2">
       <c r="A1520" s="1" t="s">
-        <v>4319</v>
+        <v>4313</v>
       </c>
       <c r="B1520" t="s">
-        <v>4320</v>
+        <v>4314</v>
       </c>
     </row>
     <row r="1521" spans="1:2">
       <c r="A1521" s="1" t="s">
-        <v>4321</v>
+        <v>4315</v>
       </c>
       <c r="B1521" t="s">
-        <v>4322</v>
+        <v>4316</v>
       </c>
     </row>
     <row r="1522" spans="1:2">
       <c r="A1522" s="1" t="s">
-        <v>4323</v>
+        <v>4317</v>
       </c>
       <c r="B1522" t="s">
-        <v>4324</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="1523" spans="1:2">
       <c r="A1523" s="1" t="s">
-        <v>4325</v>
+        <v>4319</v>
       </c>
       <c r="B1523" t="s">
-        <v>4326</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="1524" spans="1:2">
       <c r="A1524" s="1" t="s">
-        <v>4327</v>
+        <v>4321</v>
       </c>
       <c r="B1524" t="s">
-        <v>4328</v>
+        <v>4322</v>
       </c>
     </row>
     <row r="1525" spans="1:2">
       <c r="A1525" s="1" t="s">
-        <v>4329</v>
+        <v>4323</v>
       </c>
       <c r="B1525" t="s">
-        <v>4330</v>
+        <v>4324</v>
       </c>
     </row>
     <row r="1526" spans="1:2">
       <c r="A1526" s="1" t="s">
-        <v>4331</v>
+        <v>4325</v>
       </c>
       <c r="B1526" t="s">
-        <v>4332</v>
+        <v>4326</v>
       </c>
     </row>
     <row r="1527" spans="1:2">
       <c r="A1527" s="1" t="s">
-        <v>4333</v>
+        <v>4327</v>
       </c>
       <c r="B1527" t="s">
-        <v>4334</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="1528" spans="1:2">
       <c r="A1528" s="1" t="s">
-        <v>4335</v>
+        <v>4329</v>
       </c>
       <c r="B1528" t="s">
-        <v>4336</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="1529" spans="1:2">
       <c r="A1529" s="1" t="s">
-        <v>4337</v>
+        <v>4331</v>
       </c>
       <c r="B1529" t="s">
-        <v>4338</v>
+        <v>4332</v>
       </c>
     </row>
     <row r="1530" spans="1:2">
       <c r="A1530" s="1" t="s">
-        <v>4339</v>
+        <v>4333</v>
       </c>
       <c r="B1530" t="s">
-        <v>4340</v>
+        <v>4334</v>
       </c>
     </row>
     <row r="1531" spans="1:2">
       <c r="A1531" s="1" t="s">
-        <v>4341</v>
+        <v>4335</v>
       </c>
       <c r="B1531" t="s">
-        <v>4342</v>
+        <v>4336</v>
       </c>
     </row>
     <row r="1532" spans="1:2">
       <c r="A1532" s="1" t="s">
-        <v>4343</v>
+        <v>4337</v>
       </c>
       <c r="B1532" t="s">
-        <v>4344</v>
+        <v>4338</v>
       </c>
     </row>
     <row r="1533" spans="1:2">
       <c r="A1533" s="1" t="s">
-        <v>4345</v>
+        <v>4339</v>
       </c>
       <c r="B1533" t="s">
-        <v>4346</v>
+        <v>4340</v>
       </c>
     </row>
     <row r="1534" spans="1:2">
       <c r="A1534" s="1" t="s">
-        <v>4347</v>
+        <v>4341</v>
       </c>
       <c r="B1534" t="s">
-        <v>4348</v>
+        <v>4342</v>
       </c>
     </row>
     <row r="1535" spans="1:2">
       <c r="A1535" s="1" t="s">
-        <v>4349</v>
+        <v>4343</v>
       </c>
       <c r="B1535" t="s">
-        <v>4350</v>
+        <v>4344</v>
       </c>
     </row>
     <row r="1536" spans="1:2">
       <c r="A1536" s="1" t="s">
-        <v>4351</v>
+        <v>4345</v>
       </c>
       <c r="B1536" t="s">
-        <v>4352</v>
+        <v>4346</v>
       </c>
     </row>
     <row r="1537" spans="1:2">
       <c r="A1537" s="1" t="s">
-        <v>4353</v>
+        <v>4347</v>
       </c>
       <c r="B1537" t="s">
-        <v>4354</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="1538" spans="1:2">
       <c r="A1538" s="1" t="s">
-        <v>4355</v>
+        <v>4349</v>
       </c>
       <c r="B1538" t="s">
-        <v>4356</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="1539" spans="1:2">
       <c r="A1539" s="1" t="s">
-        <v>4357</v>
+        <v>4351</v>
       </c>
       <c r="B1539" t="s">
-        <v>4358</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="1540" spans="1:2">
       <c r="A1540" s="1" t="s">
-        <v>4359</v>
+        <v>4353</v>
       </c>
       <c r="B1540" t="s">
-        <v>4360</v>
+        <v>4354</v>
       </c>
     </row>
     <row r="1541" spans="1:2">
       <c r="A1541" s="1" t="s">
-        <v>4361</v>
+        <v>4355</v>
       </c>
       <c r="B1541" t="s">
-        <v>4362</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="1542" spans="1:2">
       <c r="A1542" s="1" t="s">
-        <v>4363</v>
+        <v>4357</v>
       </c>
       <c r="B1542" t="s">
-        <v>4364</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="1543" spans="1:2">
       <c r="A1543" s="1" t="s">
-        <v>4365</v>
+        <v>4359</v>
       </c>
       <c r="B1543" t="s">
-        <v>4366</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="1544" spans="1:2">
       <c r="A1544" s="1" t="s">
-        <v>4427</v>
+        <v>4361</v>
       </c>
       <c r="B1544" t="s">
-        <v>4428</v>
+        <v>4362</v>
       </c>
     </row>
     <row r="1545" spans="1:2">
       <c r="A1545" s="1" t="s">
-        <v>4367</v>
+        <v>4363</v>
       </c>
       <c r="B1545" t="s">
-        <v>4368</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="1546" spans="1:2">
       <c r="A1546" s="1" t="s">
-        <v>4369</v>
+        <v>4365</v>
       </c>
       <c r="B1546" t="s">
-        <v>4370</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="1547" spans="1:2">
       <c r="A1547" s="1" t="s">
-        <v>4371</v>
+        <v>4427</v>
       </c>
       <c r="B1547" t="s">
-        <v>4372</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="1548" spans="1:2">
       <c r="A1548" s="1" t="s">
-        <v>4373</v>
+        <v>4367</v>
       </c>
       <c r="B1548" t="s">
-        <v>4374</v>
+        <v>4368</v>
       </c>
     </row>
     <row r="1549" spans="1:2">
       <c r="A1549" s="1" t="s">
-        <v>4375</v>
+        <v>4369</v>
       </c>
       <c r="B1549" t="s">
-        <v>4376</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="1550" spans="1:2">
       <c r="A1550" s="1" t="s">
-        <v>4377</v>
+        <v>4371</v>
       </c>
       <c r="B1550" t="s">
-        <v>4378</v>
+        <v>4372</v>
       </c>
     </row>
     <row r="1551" spans="1:2">
       <c r="A1551" s="1" t="s">
-        <v>4379</v>
+        <v>4373</v>
       </c>
       <c r="B1551" t="s">
-        <v>4380</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="1552" spans="1:2">
       <c r="A1552" s="1" t="s">
-        <v>4438</v>
+        <v>4375</v>
       </c>
       <c r="B1552" t="s">
-        <v>4439</v>
+        <v>4376</v>
       </c>
     </row>
     <row r="1553" spans="1:2">
       <c r="A1553" s="1" t="s">
-        <v>4381</v>
+        <v>4377</v>
       </c>
       <c r="B1553" t="s">
-        <v>4382</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="1554" spans="1:2">
       <c r="A1554" s="1" t="s">
-        <v>4383</v>
+        <v>4379</v>
       </c>
       <c r="B1554" t="s">
-        <v>4384</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="1555" spans="1:2">
       <c r="A1555" s="1" t="s">
-        <v>4385</v>
+        <v>4438</v>
       </c>
       <c r="B1555" t="s">
-        <v>4386</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="1556" spans="1:2">
       <c r="A1556" s="1" t="s">
-        <v>4387</v>
+        <v>4381</v>
       </c>
       <c r="B1556" t="s">
-        <v>4388</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="1557" spans="1:2">
       <c r="A1557" s="1" t="s">
-        <v>4389</v>
+        <v>4383</v>
       </c>
       <c r="B1557" t="s">
-        <v>4390</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="1558" spans="1:2">
       <c r="A1558" s="1" t="s">
-        <v>4391</v>
+        <v>4385</v>
       </c>
       <c r="B1558" t="s">
-        <v>4392</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="1559" spans="1:2">
       <c r="A1559" s="1" t="s">
-        <v>4393</v>
+        <v>4387</v>
       </c>
       <c r="B1559" t="s">
-        <v>4394</v>
+        <v>4388</v>
       </c>
     </row>
     <row r="1560" spans="1:2">
       <c r="A1560" s="1" t="s">
-        <v>4395</v>
+        <v>4389</v>
       </c>
       <c r="B1560" t="s">
-        <v>4396</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="1561" spans="1:2">
       <c r="A1561" s="1" t="s">
-        <v>4397</v>
+        <v>4391</v>
       </c>
       <c r="B1561" t="s">
-        <v>4398</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="1562" spans="1:2">
       <c r="A1562" s="1" t="s">
-        <v>4399</v>
+        <v>4393</v>
       </c>
       <c r="B1562" t="s">
-        <v>4400</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="1563" spans="1:2">
       <c r="A1563" s="1" t="s">
-        <v>4401</v>
+        <v>4395</v>
       </c>
       <c r="B1563" t="s">
-        <v>4402</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="1564" spans="1:2">
       <c r="A1564" s="1" t="s">
-        <v>4403</v>
+        <v>4397</v>
       </c>
       <c r="B1564" t="s">
-        <v>4404</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="1565" spans="1:2">
       <c r="A1565" s="1" t="s">
-        <v>4405</v>
+        <v>4399</v>
       </c>
       <c r="B1565" t="s">
-        <v>4406</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="1566" spans="1:2">
       <c r="A1566" s="1" t="s">
+        <v>4401</v>
+      </c>
+      <c r="B1566" t="s">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:2">
+      <c r="A1567" s="1" t="s">
+        <v>4403</v>
+      </c>
+      <c r="B1567" t="s">
+        <v>4404</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:2">
+      <c r="A1568" s="1" t="s">
+        <v>4405</v>
+      </c>
+      <c r="B1568" t="s">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:2">
+      <c r="A1569" s="1" t="s">
         <v>4407</v>
       </c>
-      <c r="B1566" t="s">
+      <c r="B1569" t="s">
         <v>4408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: COA and Petty cash
</commit_message>
<xml_diff>
--- a/public/6. COA.xlsx
+++ b/public/6. COA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier Details" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4518" uniqueCount="4481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4521" uniqueCount="4484">
   <si>
     <t>ACCESS BANK -USD</t>
   </si>
@@ -13487,6 +13487,15 @@
   </si>
   <si>
     <t>KING GEORGE IV COURT TRUST</t>
+  </si>
+  <si>
+    <t>W0021</t>
+  </si>
+  <si>
+    <t>WORLDPAY</t>
+  </si>
+  <si>
+    <t>UK</t>
   </si>
 </sst>
 </file>
@@ -13641,7 +13650,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -13740,13 +13749,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -13864,6 +13884,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14194,10 +14219,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B1579"/>
+  <dimension ref="A1:B1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1575" workbookViewId="0">
-      <selection activeCell="B1581" sqref="B1581"/>
+    <sheetView tabSelected="1" topLeftCell="A1566" workbookViewId="0">
+      <selection activeCell="B1582" sqref="B1582"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26836,6 +26861,14 @@
       </c>
       <c r="B1579" t="s">
         <v>4480</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:2">
+      <c r="A1580" s="73" t="s">
+        <v>4481</v>
+      </c>
+      <c r="B1580" s="74" t="s">
+        <v>4482</v>
       </c>
     </row>
   </sheetData>
@@ -26854,7 +26887,7 @@
   </sheetPr>
   <dimension ref="A2:B160"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+    <sheetView topLeftCell="A118" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -27918,7 +27951,7 @@
         <v>3231</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="409.6">
+    <row r="132" spans="1:2">
       <c r="A132" s="24">
         <v>1361</v>
       </c>
@@ -27926,11 +27959,11 @@
         <v>3231</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="409.6">
+    <row r="133" spans="1:2">
       <c r="A133" s="24"/>
       <c r="B133" s="24"/>
     </row>
-    <row r="134" spans="1:2" ht="409.6">
+    <row r="134" spans="1:2" ht="15">
       <c r="A134" s="23">
         <v>1400</v>
       </c>
@@ -27938,7 +27971,7 @@
         <v>3114</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="409.6">
+    <row r="135" spans="1:2">
       <c r="A135" s="24">
         <f>+A134+1</f>
         <v>1401</v>
@@ -27947,7 +27980,7 @@
         <v>3115</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="409.6">
+    <row r="136" spans="1:2" ht="15">
       <c r="A136" s="39">
         <v>1410</v>
       </c>
@@ -27955,7 +27988,7 @@
         <v>3116</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="409.6">
+    <row r="137" spans="1:2">
       <c r="A137" s="24">
         <f>+A136+1</f>
         <v>1411</v>
@@ -27964,7 +27997,7 @@
         <v>3117</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="409.6">
+    <row r="138" spans="1:2">
       <c r="A138" s="24">
         <f>+A137+1</f>
         <v>1412</v>
@@ -27973,7 +28006,7 @@
         <v>3118</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="409.6">
+    <row r="139" spans="1:2">
       <c r="A139" s="24">
         <f>+A138+1</f>
         <v>1413</v>
@@ -27982,7 +28015,7 @@
         <v>3119</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="409.6">
+    <row r="140" spans="1:2" ht="15">
       <c r="A140" s="39">
         <v>1420</v>
       </c>
@@ -27990,7 +28023,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="409.6">
+    <row r="141" spans="1:2">
       <c r="A141" s="24">
         <f>+A140+1</f>
         <v>1421</v>
@@ -27999,7 +28032,7 @@
         <v>3121</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="409.6">
+    <row r="142" spans="1:2">
       <c r="A142" s="24">
         <v>1422</v>
       </c>
@@ -28007,7 +28040,7 @@
         <v>3314</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="409.6">
+    <row r="143" spans="1:2">
       <c r="A143" s="24">
         <v>1423</v>
       </c>
@@ -28015,7 +28048,7 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="409.6">
+    <row r="144" spans="1:2">
       <c r="A144" s="24">
         <v>1424</v>
       </c>
@@ -28023,67 +28056,67 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="409.6">
+    <row r="145" spans="1:2">
       <c r="A145" s="44"/>
       <c r="B145" s="45"/>
     </row>
-    <row r="146" spans="1:2" ht="409.6">
+    <row r="146" spans="1:2">
       <c r="A146" s="46"/>
       <c r="B146" s="47"/>
     </row>
-    <row r="147" spans="1:2" ht="409.6">
+    <row r="147" spans="1:2">
       <c r="A147" s="46"/>
       <c r="B147" s="47"/>
     </row>
-    <row r="148" spans="1:2" ht="409.6">
+    <row r="148" spans="1:2">
       <c r="A148" s="46"/>
       <c r="B148" s="47"/>
     </row>
-    <row r="149" spans="1:2" ht="409.6">
+    <row r="149" spans="1:2">
       <c r="A149" s="43"/>
       <c r="B149" s="43"/>
     </row>
-    <row r="150" spans="1:2" ht="409.6">
+    <row r="150" spans="1:2">
       <c r="A150" s="43"/>
       <c r="B150" s="43"/>
     </row>
-    <row r="151" spans="1:2" ht="409.6">
+    <row r="151" spans="1:2">
       <c r="A151" s="43"/>
       <c r="B151" s="43"/>
     </row>
-    <row r="152" spans="1:2" ht="409.6">
+    <row r="152" spans="1:2">
       <c r="A152" s="43"/>
       <c r="B152" s="43"/>
     </row>
-    <row r="153" spans="1:2" ht="409.6">
+    <row r="153" spans="1:2">
       <c r="A153" s="43"/>
       <c r="B153" s="43"/>
     </row>
-    <row r="154" spans="1:2" ht="409.6">
+    <row r="154" spans="1:2">
       <c r="A154" s="43"/>
       <c r="B154" s="43"/>
     </row>
-    <row r="155" spans="1:2" ht="409.6">
+    <row r="155" spans="1:2">
       <c r="A155" s="43"/>
       <c r="B155" s="43"/>
     </row>
-    <row r="156" spans="1:2" ht="409.6">
+    <row r="156" spans="1:2">
       <c r="A156" s="43"/>
       <c r="B156" s="43"/>
     </row>
-    <row r="157" spans="1:2" ht="409.6">
+    <row r="157" spans="1:2">
       <c r="A157" s="43"/>
       <c r="B157" s="43"/>
     </row>
-    <row r="158" spans="1:2" ht="409.6">
+    <row r="158" spans="1:2">
       <c r="A158" s="43"/>
       <c r="B158" s="43"/>
     </row>
-    <row r="159" spans="1:2" ht="409.6">
+    <row r="159" spans="1:2">
       <c r="A159" s="43"/>
       <c r="B159" s="43"/>
     </row>
-    <row r="160" spans="1:2" ht="409.6">
+    <row r="160" spans="1:2">
       <c r="A160" s="43"/>
       <c r="B160" s="43"/>
     </row>
@@ -28100,7 +28133,7 @@
   </sheetPr>
   <dimension ref="A1:B1387"/>
   <sheetViews>
-    <sheetView topLeftCell="A890" workbookViewId="0">
+    <sheetView topLeftCell="A1023" workbookViewId="0">
       <selection activeCell="B902" sqref="B902"/>
     </sheetView>
   </sheetViews>
@@ -36755,10 +36788,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A2:B90"/>
+  <dimension ref="A2:B91"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A70" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -37332,7 +37365,7 @@
         <v>3235</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="409.6">
+    <row r="73" spans="1:2">
       <c r="A73" s="58">
         <v>3012</v>
       </c>
@@ -37340,7 +37373,7 @@
         <v>3234</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="409.6">
+    <row r="74" spans="1:2">
       <c r="A74" s="64">
         <v>3020</v>
       </c>
@@ -37348,7 +37381,7 @@
         <v>3236</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="409.6">
+    <row r="75" spans="1:2">
       <c r="A75" s="58">
         <v>3011</v>
       </c>
@@ -37356,7 +37389,7 @@
         <v>3237</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="409.6">
+    <row r="76" spans="1:2">
       <c r="A76" s="64">
         <v>3030</v>
       </c>
@@ -37364,7 +37397,7 @@
         <v>3238</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="409.6">
+    <row r="77" spans="1:2">
       <c r="A77" s="58">
         <v>3031</v>
       </c>
@@ -37372,7 +37405,7 @@
         <v>3239</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="409.6">
+    <row r="78" spans="1:2">
       <c r="A78" s="58">
         <v>1111</v>
       </c>
@@ -37380,7 +37413,7 @@
         <v>4409</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="409.6">
+    <row r="79" spans="1:2">
       <c r="A79" s="58">
         <v>1112</v>
       </c>
@@ -37388,7 +37421,7 @@
         <v>4410</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="409.6">
+    <row r="80" spans="1:2">
       <c r="A80" s="58">
         <v>2026</v>
       </c>
@@ -37396,7 +37429,7 @@
         <v>4411</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="409.6">
+    <row r="81" spans="1:2">
       <c r="A81" s="58">
         <v>2525</v>
       </c>
@@ -37404,7 +37437,7 @@
         <v>4412</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="409.6">
+    <row r="82" spans="1:2">
       <c r="A82" s="58">
         <v>1121</v>
       </c>
@@ -37412,7 +37445,7 @@
         <v>3154</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="409.6">
+    <row r="83" spans="1:2">
       <c r="A83" s="58">
         <v>1142</v>
       </c>
@@ -37420,7 +37453,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="409.6">
+    <row r="84" spans="1:2">
       <c r="A84" s="60">
         <v>1141</v>
       </c>
@@ -37428,7 +37461,7 @@
         <v>4414</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="409.6">
+    <row r="85" spans="1:2">
       <c r="A85" s="60">
         <v>1062</v>
       </c>
@@ -37436,7 +37469,7 @@
         <v>4415</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="409.6">
+    <row r="86" spans="1:2">
       <c r="A86" s="60">
         <v>1061</v>
       </c>
@@ -37444,7 +37477,7 @@
         <v>4416</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="409.6">
+    <row r="87" spans="1:2">
       <c r="A87" s="60">
         <v>2024</v>
       </c>
@@ -37452,7 +37485,7 @@
         <v>4417</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="409.6">
+    <row r="88" spans="1:2">
       <c r="A88" s="60">
         <v>2023</v>
       </c>
@@ -37460,7 +37493,7 @@
         <v>4418</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="409.6">
+    <row r="89" spans="1:2">
       <c r="A89" s="60">
         <v>1324</v>
       </c>
@@ -37468,12 +37501,17 @@
         <v>4419</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="409.6">
+    <row r="90" spans="1:2">
       <c r="A90" s="60">
         <v>1323</v>
       </c>
       <c r="B90" s="61" t="s">
         <v>4420</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="B91" s="75" t="s">
+        <v>4483</v>
       </c>
     </row>
   </sheetData>
@@ -37492,7 +37530,7 @@
   </sheetPr>
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -38236,7 +38274,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="409.6">
+    <row r="36" spans="2:3">
       <c r="B36" s="29">
         <v>2650</v>
       </c>
@@ -38244,7 +38282,7 @@
         <v>3251</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="409.6">
+    <row r="37" spans="2:3">
       <c r="B37" s="29">
         <v>3550</v>
       </c>
@@ -38252,7 +38290,7 @@
         <v>3252</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="409.6">
+    <row r="38" spans="2:3">
       <c r="B38" s="29">
         <v>3550</v>
       </c>
@@ -38260,7 +38298,7 @@
         <v>3253</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="409.6">
+    <row r="39" spans="2:3">
       <c r="B39" s="29">
         <v>2650</v>
       </c>
@@ -38268,13 +38306,13 @@
         <v>3254</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="409.6">
+    <row r="40" spans="2:3">
       <c r="B40" s="34"/>
       <c r="C40" s="17" t="s">
         <v>3255</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="409.6">
+    <row r="41" spans="2:3">
       <c r="B41" s="29">
         <v>2000</v>
       </c>
@@ -38282,7 +38320,7 @@
         <v>3178</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="409.6">
+    <row r="42" spans="2:3">
       <c r="B42" s="29">
         <v>2000</v>
       </c>
@@ -38290,13 +38328,13 @@
         <v>3256</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="409.6">
+    <row r="43" spans="2:3">
       <c r="B43" s="34"/>
       <c r="C43" s="17" t="s">
         <v>3257</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="409.6">
+    <row r="44" spans="2:3">
       <c r="B44" s="29">
         <v>1850</v>
       </c>
@@ -38304,7 +38342,7 @@
         <v>3180</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="409.6">
+    <row r="45" spans="2:3">
       <c r="B45" s="29">
         <v>2400</v>
       </c>
@@ -38312,7 +38350,7 @@
         <v>3258</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="409.6">
+    <row r="46" spans="2:3">
       <c r="B46" s="29">
         <v>2400</v>
       </c>
@@ -38320,7 +38358,7 @@
         <v>3259</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="409.6">
+    <row r="47" spans="2:3">
       <c r="B47" s="29">
         <v>1850</v>
       </c>
@@ -38328,13 +38366,13 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="48" spans="2:3" ht="409.6">
+    <row r="48" spans="2:3">
       <c r="B48" s="34"/>
       <c r="C48" s="17" t="s">
         <v>3261</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="409.6">
+    <row r="49" spans="2:3">
       <c r="B49" s="29">
         <v>4600</v>
       </c>
@@ -38342,7 +38380,7 @@
         <v>3262</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="409.6">
+    <row r="50" spans="2:3">
       <c r="B50" s="29">
         <v>4650</v>
       </c>
@@ -38350,7 +38388,7 @@
         <v>3263</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="409.6">
+    <row r="51" spans="2:3">
       <c r="B51" s="29">
         <v>4650</v>
       </c>
@@ -38358,7 +38396,7 @@
         <v>3264</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="409.6">
+    <row r="52" spans="2:3">
       <c r="B52" s="29">
         <v>4600</v>
       </c>
@@ -38366,13 +38404,13 @@
         <v>3265</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="409.6">
+    <row r="53" spans="2:3">
       <c r="B53" s="34"/>
       <c r="C53" s="17" t="s">
         <v>3266</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="409.6">
+    <row r="54" spans="2:3">
       <c r="B54" s="29">
         <v>2350</v>
       </c>
@@ -38380,7 +38418,7 @@
         <v>3179</v>
       </c>
     </row>
-    <row r="55" spans="2:3" ht="409.6">
+    <row r="55" spans="2:3">
       <c r="B55" s="29">
         <v>2350</v>
       </c>
@@ -38388,13 +38426,13 @@
         <v>3267</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="409.6">
+    <row r="56" spans="2:3">
       <c r="B56" s="34"/>
       <c r="C56" s="17" t="s">
         <v>3268</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="409.6">
+    <row r="57" spans="2:3">
       <c r="B57" s="29">
         <v>1000</v>
       </c>
@@ -38402,7 +38440,7 @@
         <v>3186</v>
       </c>
     </row>
-    <row r="58" spans="2:3" ht="409.6">
+    <row r="58" spans="2:3">
       <c r="B58" s="29">
         <v>1000</v>
       </c>
@@ -38410,7 +38448,7 @@
         <v>3269</v>
       </c>
     </row>
-    <row r="59" spans="2:3" ht="409.6">
+    <row r="59" spans="2:3">
       <c r="B59" s="29">
         <v>1000</v>
       </c>
@@ -38418,7 +38456,7 @@
         <v>3270</v>
       </c>
     </row>
-    <row r="60" spans="2:3" ht="409.6">
+    <row r="60" spans="2:3">
       <c r="B60" s="29">
         <v>1000</v>
       </c>
@@ -38426,13 +38464,13 @@
         <v>3271</v>
       </c>
     </row>
-    <row r="61" spans="2:3" ht="409.6">
+    <row r="61" spans="2:3">
       <c r="B61" s="34"/>
       <c r="C61" s="17" t="s">
         <v>3277</v>
       </c>
     </row>
-    <row r="62" spans="2:3" ht="409.6">
+    <row r="62" spans="2:3">
       <c r="B62" s="29">
         <v>5000</v>
       </c>
@@ -38440,7 +38478,7 @@
         <v>3272</v>
       </c>
     </row>
-    <row r="63" spans="2:3" ht="409.6">
+    <row r="63" spans="2:3">
       <c r="B63" s="29">
         <v>5000</v>
       </c>
@@ -38448,13 +38486,13 @@
         <v>3273</v>
       </c>
     </row>
-    <row r="64" spans="2:3" ht="409.6">
+    <row r="64" spans="2:3">
       <c r="B64" s="34"/>
       <c r="C64" s="17" t="s">
         <v>3278</v>
       </c>
     </row>
-    <row r="65" spans="2:3" ht="409.6">
+    <row r="65" spans="2:3">
       <c r="B65" s="29">
         <v>3700</v>
       </c>
@@ -38462,7 +38500,7 @@
         <v>3206</v>
       </c>
     </row>
-    <row r="66" spans="2:3" ht="409.6">
+    <row r="66" spans="2:3">
       <c r="B66" s="29">
         <v>6000</v>
       </c>
@@ -38470,7 +38508,7 @@
         <v>3246</v>
       </c>
     </row>
-    <row r="67" spans="2:3" ht="409.6">
+    <row r="67" spans="2:3">
       <c r="B67" s="29">
         <v>6000</v>
       </c>
@@ -38478,7 +38516,7 @@
         <v>3247</v>
       </c>
     </row>
-    <row r="68" spans="2:3" ht="409.6">
+    <row r="68" spans="2:3">
       <c r="B68" s="29">
         <v>3700</v>
       </c>
@@ -38486,13 +38524,13 @@
         <v>3248</v>
       </c>
     </row>
-    <row r="69" spans="2:3" ht="409.6">
+    <row r="69" spans="2:3">
       <c r="B69" s="34"/>
       <c r="C69" s="17" t="s">
         <v>3279</v>
       </c>
     </row>
-    <row r="70" spans="2:3" ht="409.6">
+    <row r="70" spans="2:3">
       <c r="B70" s="29">
         <v>3650</v>
       </c>
@@ -38500,7 +38538,7 @@
         <v>3229</v>
       </c>
     </row>
-    <row r="71" spans="2:3" ht="409.6">
+    <row r="71" spans="2:3">
       <c r="B71" s="29">
         <v>3650</v>
       </c>
@@ -38508,10 +38546,10 @@
         <v>3249</v>
       </c>
     </row>
-    <row r="72" spans="2:3" ht="409.6">
+    <row r="72" spans="2:3">
       <c r="B72" s="31"/>
     </row>
-    <row r="73" spans="2:3" ht="409.6">
+    <row r="73" spans="2:3">
       <c r="B73" s="31"/>
     </row>
   </sheetData>

</xml_diff>